<commit_message>
AB Bug Fixes and new FORMAT_VALIDATOR transformer
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -18,14 +18,15 @@
     <sheet name="Country" sheetId="9" r:id="rId4"/>
     <sheet name="Default_AB" sheetId="4" r:id="rId5"/>
     <sheet name="Default_BC" sheetId="1" r:id="rId6"/>
-    <sheet name="Format" sheetId="7" r:id="rId7"/>
-    <sheet name="FrenchTranslation" sheetId="8" r:id="rId8"/>
-    <sheet name="Keyword" sheetId="5" r:id="rId9"/>
-    <sheet name="Progress" sheetId="10" r:id="rId10"/>
-    <sheet name="Role" sheetId="11" r:id="rId11"/>
-    <sheet name="SpatialRef" sheetId="13" r:id="rId12"/>
-    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId13"/>
-    <sheet name="Update" sheetId="6" r:id="rId14"/>
+    <sheet name="ESRI_AB" sheetId="15" r:id="rId7"/>
+    <sheet name="Format" sheetId="7" r:id="rId8"/>
+    <sheet name="FrenchTranslation" sheetId="8" r:id="rId9"/>
+    <sheet name="Keyword" sheetId="5" r:id="rId10"/>
+    <sheet name="Progress" sheetId="10" r:id="rId11"/>
+    <sheet name="Role" sheetId="11" r:id="rId12"/>
+    <sheet name="SpatialRef" sheetId="13" r:id="rId13"/>
+    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId14"/>
+    <sheet name="Update" sheetId="6" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2374" uniqueCount="750">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="793">
   <si>
     <t>default_key</t>
   </si>
@@ -2287,6 +2288,135 @@
   </si>
   <si>
     <t>contact_postal_code</t>
+  </si>
+  <si>
+    <t>lookup_title</t>
+  </si>
+  <si>
+    <t>Access and Facility Polygons</t>
+  </si>
+  <si>
+    <t>Access and Facility Roads</t>
+  </si>
+  <si>
+    <t>Alberta Provincial Boundary - 2007</t>
+  </si>
+  <si>
+    <t>ATS v4.1 Alberta Provincial Boundary</t>
+  </si>
+  <si>
+    <t>ATS v4.1 Polygons - Legal Subdivision (LSD) with Road Allowance</t>
+  </si>
+  <si>
+    <t>ATS v4.1 Polygons - Quarter Section with Road Allowance</t>
+  </si>
+  <si>
+    <t>ATS v4.1 Polygons - Section with Road Allowance</t>
+  </si>
+  <si>
+    <t>ATS v4.1 Polygons - Township Index</t>
+  </si>
+  <si>
+    <t>Base Hydrography Point Event</t>
+  </si>
+  <si>
+    <t>Base Hydrography Point Update</t>
+  </si>
+  <si>
+    <t>Base Stream and Flow Representation</t>
+  </si>
+  <si>
+    <t>Base Stream and Flow Representation Update</t>
+  </si>
+  <si>
+    <t>Base Waterbody Polygon Arc</t>
+  </si>
+  <si>
+    <t>Base Waterbody Polygon Update</t>
+  </si>
+  <si>
+    <t>Cutlines and Trails</t>
+  </si>
+  <si>
+    <t>DND Air Weapons Range</t>
+  </si>
+  <si>
+    <t>DND Military Base</t>
+  </si>
+  <si>
+    <t>Education - Authorities District</t>
+  </si>
+  <si>
+    <t>Education - Authorities Francophone</t>
+  </si>
+  <si>
+    <t>Education - Authorities Public</t>
+  </si>
+  <si>
+    <t>Education - Authorities Separate</t>
+  </si>
+  <si>
+    <t>Facility Points</t>
+  </si>
+  <si>
+    <t>Fish and Wildlife District</t>
+  </si>
+  <si>
+    <t>Green/White Area</t>
+  </si>
+  <si>
+    <t>Green/White Area Historical</t>
+  </si>
+  <si>
+    <t>Hamlet, Locality and Townsite Point</t>
+  </si>
+  <si>
+    <t>Indian Reserve</t>
+  </si>
+  <si>
+    <t>Integrated Resource Plan - Local</t>
+  </si>
+  <si>
+    <t>Integrated Resource Plan - Subregional</t>
+  </si>
+  <si>
+    <t>Land-use Framework Planning Regions</t>
+  </si>
+  <si>
+    <t>Metis Settlement</t>
+  </si>
+  <si>
+    <t>Non-Permit Area</t>
+  </si>
+  <si>
+    <t>NTS Grid 1:20 000</t>
+  </si>
+  <si>
+    <t>NTS Grid 1:250 000</t>
+  </si>
+  <si>
+    <t>NTS Grid 1:50 000</t>
+  </si>
+  <si>
+    <t>Powerlines</t>
+  </si>
+  <si>
+    <t>Provincial Electoral Division - Current 2010</t>
+  </si>
+  <si>
+    <t>Provincial Electoral Division - Historical 2003</t>
+  </si>
+  <si>
+    <t>Railway Point Events</t>
+  </si>
+  <si>
+    <t>Railways</t>
+  </si>
+  <si>
+    <t>Road Point Events</t>
+  </si>
+  <si>
+    <t>layer_name</t>
   </si>
 </sst>
 </file>
@@ -2685,6 +2815,224 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>201</v>
+      </c>
+      <c r="B22" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2858,7 +3206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -3117,7 +3465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -3250,7 +3598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -3369,7 +3717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -3674,8 +4022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78:B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4652,7 +5000,7 @@
   <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="B71" sqref="B71:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5586,7 +5934,7 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:A44"/>
+      <selection activeCell="A42" sqref="A42:A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5924,7 +6272,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B42" t="s">
         <v>744</v>
@@ -5932,7 +6280,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -5940,7 +6288,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B44" t="s">
         <v>745</v>
@@ -5960,7 +6308,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A26" sqref="A26:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6170,7 +6518,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B26" t="s">
         <v>747</v>
@@ -6178,7 +6526,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B27" t="s">
         <v>19</v>
@@ -6186,7 +6534,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B28" t="s">
         <v>748</v>
@@ -6198,6 +6546,361 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>751</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>752</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>753</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>754</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>755</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>756</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>757</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>758</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>759</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>760</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>761</v>
+      </c>
+      <c r="B12">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>762</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>763</v>
+      </c>
+      <c r="B14">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>764</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>765</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>766</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>767</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>768</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>769</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>770</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>771</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>772</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>773</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>774</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>775</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>776</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>777</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>778</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>779</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>780</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>781</v>
+      </c>
+      <c r="B32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>782</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>783</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>784</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>785</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>786</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>787</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>788</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>789</v>
+      </c>
+      <c r="B40">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>790</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>791</v>
+      </c>
+      <c r="B42">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D354"/>
   <sheetViews>
@@ -11175,7 +11878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -11215,222 +11918,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>208</v>
-      </c>
-      <c r="B8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>209</v>
-      </c>
-      <c r="B10" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>169</v>
-      </c>
-      <c r="B11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>210</v>
-      </c>
-      <c r="B12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>212</v>
-      </c>
-      <c r="B14" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>213</v>
-      </c>
-      <c r="B15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>214</v>
-      </c>
-      <c r="B16" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>216</v>
-      </c>
-      <c r="B18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>217</v>
-      </c>
-      <c r="B19" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>218</v>
-      </c>
-      <c r="B20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>219</v>
-      </c>
-      <c r="B21" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>220</v>
-      </c>
-      <c r="B23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>221</v>
-      </c>
-      <c r="B24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>222</v>
-      </c>
-      <c r="B25" t="s">
-        <v>213</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update BC workspace to set spatial type representation
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" firstSheet="7" activeTab="21"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -33,7 +33,8 @@
     <sheet name="SpatialRef" sheetId="13" r:id="rId19"/>
     <sheet name="SpatialRepresentation" sheetId="14" r:id="rId20"/>
     <sheet name="Update" sheetId="6" r:id="rId21"/>
-    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId22"/>
+    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId22"/>
+    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId23"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3546" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3578" uniqueCount="1044">
   <si>
     <t>default_key</t>
   </si>
@@ -3132,6 +3133,51 @@
   </si>
   <si>
     <t>cad5639a-437e-4cc2-adaf-62e4fccbbc30</t>
+  </si>
+  <si>
+    <t>fda19189-6cb4-4712-992f-500acadae749</t>
+  </si>
+  <si>
+    <t>1137004b-39bc-4b52-aefc-cc9328f1384b</t>
+  </si>
+  <si>
+    <t>7e986391-c740-4d1b-9294-7576af2d2998</t>
+  </si>
+  <si>
+    <t>5712e5f8-dd01-4cdb-947c-7227b15cf1af</t>
+  </si>
+  <si>
+    <t>bad79704-3fc9-43e7-b5d4-660657199af8</t>
+  </si>
+  <si>
+    <t>c819aef2-2cb3-43ee-a41b-77debdecd81e</t>
+  </si>
+  <si>
+    <t>a5965764-a3d0-48aa-97e7-10f873cb5e78</t>
+  </si>
+  <si>
+    <t>509cbf74-7ee7-44d3-a88d-4e088ea67325</t>
+  </si>
+  <si>
+    <t>ade4f36a-1fd4-4583-8253-2b2a1bbe34ff</t>
+  </si>
+  <si>
+    <t>f7efa3ea-bf1c-4c4f-bb33-ba841aa076c0</t>
+  </si>
+  <si>
+    <t>90653877-c55a-435f-bd71-dca4fd55bb0e</t>
+  </si>
+  <si>
+    <t>8ec88f64-24b4-4301-861b-4d0d3f3e2c17</t>
+  </si>
+  <si>
+    <t>230bdb21-2cb8-478f-873a-80f30377d7b5</t>
+  </si>
+  <si>
+    <t>2db77f8b-765b-488f-9752-f1349cf6ebfc</t>
+  </si>
+  <si>
+    <t>f6d17c00-d4b9-401b-a20e-ef7e37b6d5e3</t>
   </si>
 </sst>
 </file>
@@ -3224,7 +3270,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3238,6 +3284,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3946,7 +3993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D430"/>
   <sheetViews>
-    <sheetView topLeftCell="A404" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A404" workbookViewId="0">
       <selection activeCell="B430" sqref="B430:D430"/>
     </sheetView>
   </sheetViews>
@@ -14113,10 +14160,157 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>998</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16878,7 +17072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FORMAT TABLE: JPG2 revised to JP2
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="1201">
   <si>
     <t>default_key</t>
   </si>
@@ -3635,9 +3635,6 @@
   </si>
   <si>
     <t>date_added</t>
-  </si>
-  <si>
-    <t>JPG2</t>
   </si>
   <si>
     <t>gpk</t>
@@ -3658,7 +3655,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3766,8 +3763,8 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -4053,7 +4050,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -4121,7 +4118,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -4472,11 +4469,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B305" sqref="B305"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B332" sqref="B332"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="151.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -4502,7 +4499,7 @@
         <v>1195</v>
       </c>
       <c r="F1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -8738,7 +8735,7 @@
         <v>287</v>
       </c>
       <c r="B304" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>275</v>
@@ -8752,7 +8749,7 @@
         <v>288</v>
       </c>
       <c r="B305" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>275</v>
@@ -8833,7 +8830,7 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="9" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B311" s="9" t="s">
         <v>824</v>
@@ -9136,7 +9133,7 @@
         <v>1194</v>
       </c>
       <c r="B332" t="s">
-        <v>1196</v>
+        <v>1053</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>275</v>
@@ -9405,7 +9402,7 @@
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="9" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B351" s="9" t="s">
         <v>1050</v>
@@ -9611,7 +9608,7 @@
     </row>
     <row r="365" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="9" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B365" t="s">
         <v>784</v>
@@ -10670,7 +10667,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -10714,7 +10711,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -10889,7 +10886,7 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -11595,7 +11592,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -11813,7 +11810,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -11896,7 +11893,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -12071,7 +12068,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -12330,7 +12327,7 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -13418,7 +13415,7 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -14395,7 +14392,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -14560,7 +14557,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -14679,7 +14676,7 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -15092,7 +15089,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -16223,7 +16220,7 @@
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -16413,7 +16410,7 @@
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -17308,11 +17305,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -17983,7 +17980,7 @@
         <v>146</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
         <v>132</v>
@@ -18211,7 +18208,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -18474,7 +18471,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -18509,7 +18506,7 @@
       <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>
@@ -18843,7 +18840,7 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>
@@ -19085,7 +19082,7 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updates to have less parameters
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3949" uniqueCount="1201">
   <si>
     <t>default_key</t>
   </si>
@@ -3635,9 +3635,6 @@
   </si>
   <si>
     <t>date_added</t>
-  </si>
-  <si>
-    <t>JPG2</t>
   </si>
   <si>
     <t>gpk</t>
@@ -4472,8 +4469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B305" sqref="B305"/>
+    <sheetView tabSelected="1" topLeftCell="A312" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B332" sqref="B332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4502,7 +4499,7 @@
         <v>1195</v>
       </c>
       <c r="F1" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -8738,7 +8735,7 @@
         <v>287</v>
       </c>
       <c r="B304" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C304" s="3" t="s">
         <v>275</v>
@@ -8752,7 +8749,7 @@
         <v>288</v>
       </c>
       <c r="B305" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C305" s="3" t="s">
         <v>275</v>
@@ -8833,7 +8830,7 @@
     </row>
     <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="9" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B311" s="9" t="s">
         <v>824</v>
@@ -9136,7 +9133,7 @@
         <v>1194</v>
       </c>
       <c r="B332" t="s">
-        <v>1196</v>
+        <v>1053</v>
       </c>
       <c r="C332" s="3" t="s">
         <v>275</v>
@@ -9405,7 +9402,7 @@
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="9" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B351" s="9" t="s">
         <v>1050</v>
@@ -9611,7 +9608,7 @@
     </row>
     <row r="365" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A365" s="9" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B365" t="s">
         <v>784</v>

</xml_diff>

<commit_message>
Backup Ontario Work In Progress
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="10260" tabRatio="868" firstSheet="11" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -31,11 +31,13 @@
     <sheet name="Progress" sheetId="10" r:id="rId17"/>
     <sheet name="Role" sheetId="11" r:id="rId18"/>
     <sheet name="Sector_QC" sheetId="22" r:id="rId19"/>
-    <sheet name="SpatialRef" sheetId="13" r:id="rId20"/>
-    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId21"/>
-    <sheet name="Update" sheetId="6" r:id="rId22"/>
-    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId23"/>
-    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId24"/>
+    <sheet name="Sector_ON" sheetId="28" r:id="rId20"/>
+    <sheet name="Spatial_ON" sheetId="29" r:id="rId21"/>
+    <sheet name="SpatialRef" sheetId="13" r:id="rId22"/>
+    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId23"/>
+    <sheet name="Update" sheetId="6" r:id="rId24"/>
+    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId25"/>
+    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId26"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4089" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="1286">
   <si>
     <t>default_key</t>
   </si>
@@ -3763,12 +3765,156 @@
   <si>
     <t xml:space="preserve">
 **This third party metadata element was translated using an automated translation tool (Amazon Translate). To report any discrepancies, please contact us at nrcan.fgp-pgf.rncan@canada.ca.**</t>
+  </si>
+  <si>
+    <t>tags_value</t>
+  </si>
+  <si>
+    <t>Ministry of Agriculture Food and Rural Affairs</t>
+  </si>
+  <si>
+    <t>Ministry of Children Community and Social Services</t>
+  </si>
+  <si>
+    <t>Ministry of Education</t>
+  </si>
+  <si>
+    <t>Ministry of Energy Northern Development and Mines</t>
+  </si>
+  <si>
+    <t>Ministry of Environment</t>
+  </si>
+  <si>
+    <t>Ministry of Government and Consumer Services</t>
+  </si>
+  <si>
+    <t>Ministry of Health and Long Term Care</t>
+  </si>
+  <si>
+    <t>Ministry of Municipal Affairs and Housing</t>
+  </si>
+  <si>
+    <t>Ministry of Natural Resources</t>
+  </si>
+  <si>
+    <t>Ministry of Natural Resources and Forestry</t>
+  </si>
+  <si>
+    <t>Ministry of Transportation</t>
+  </si>
+  <si>
+    <t>Ministry of the Environment Conservation and Parks</t>
+  </si>
+  <si>
+    <t>Indigenous Affairs</t>
+  </si>
+  <si>
+    <t>Ministry of Indigenous Affairs</t>
+  </si>
+  <si>
+    <t>Ontario Parks</t>
+  </si>
+  <si>
+    <t>aerial photo</t>
+  </si>
+  <si>
+    <t>aerial photography</t>
+  </si>
+  <si>
+    <t>aerial photos</t>
+  </si>
+  <si>
+    <t>airborne topographic lidar</t>
+  </si>
+  <si>
+    <t>cloca lidar</t>
+  </si>
+  <si>
+    <t>dem</t>
+  </si>
+  <si>
+    <t>digital elevation model</t>
+  </si>
+  <si>
+    <t>digital raster acquisition project eastern ontario</t>
+  </si>
+  <si>
+    <t>digital raster project eastern ontario</t>
+  </si>
+  <si>
+    <t>digital surface model</t>
+  </si>
+  <si>
+    <t>digital terrain model</t>
+  </si>
+  <si>
+    <t>digital topographic data base</t>
+  </si>
+  <si>
+    <t>digitial raster project eastern ontario</t>
+  </si>
+  <si>
+    <t>gta lidar</t>
+  </si>
+  <si>
+    <t>imagery</t>
+  </si>
+  <si>
+    <t>imagery and base maps</t>
+  </si>
+  <si>
+    <t>landsat</t>
+  </si>
+  <si>
+    <t>landsat-7</t>
+  </si>
+  <si>
+    <t>lidar</t>
+  </si>
+  <si>
+    <t>lidar eastern acquisition project</t>
+  </si>
+  <si>
+    <t>omafra lidar</t>
+  </si>
+  <si>
+    <t>ontario radar digital surface model</t>
+  </si>
+  <si>
+    <t>orthoimagery</t>
+  </si>
+  <si>
+    <t>orthophoto</t>
+  </si>
+  <si>
+    <t>orthophotography</t>
+  </si>
+  <si>
+    <t>provincial digital elevation model</t>
+  </si>
+  <si>
+    <t>raster</t>
+  </si>
+  <si>
+    <t>remote sensing</t>
+  </si>
+  <si>
+    <t>satellite imagery</t>
+  </si>
+  <si>
+    <t>shuttle radar topography mission</t>
+  </si>
+  <si>
+    <t>softcopy photogrammetry</t>
+  </si>
+  <si>
+    <t>south nation lidar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3882,8 +4028,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -4169,7 +4315,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -4237,7 +4383,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -4592,7 +4738,7 @@
       <selection activeCell="B469" sqref="B469:D469"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -11276,7 +11422,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -11320,7 +11466,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -11495,7 +11641,7 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -12201,7 +12347,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -12419,7 +12565,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -12502,7 +12648,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -12677,7 +12823,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -12932,11 +13078,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -14024,7 +14170,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -14995,13 +15141,435 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B5" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B7" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B8" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B9" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B10" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B11" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B12" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B13" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B14" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B15" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B16" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B17" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B18" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B19" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B20" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B21" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B22" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B23" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B24" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B25" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B26" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B27" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B28" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B29" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B30" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B31" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B32" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B33" t="s">
+        <v>567</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -15158,7 +15726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -15166,7 +15734,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -15277,7 +15845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -15285,7 +15853,7 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -15690,7 +16258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B139"/>
   <sheetViews>
@@ -15698,7 +16266,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -16821,7 +17389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -16829,7 +17397,7 @@
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -17019,7 +17587,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -17918,7 +18486,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -18818,7 +19386,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -19081,7 +19649,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -19112,11 +19680,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>
@@ -19447,10 +20015,10 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>
@@ -19688,11 +20256,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Backup ON Work In Progress
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="21" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4864" uniqueCount="1440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4944" uniqueCount="1440">
   <si>
     <t>default_key</t>
   </si>
@@ -4383,7 +4383,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4884,7 +4884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>30</v>
       </c>
@@ -4964,7 +4964,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>6</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>1368</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>43</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>728</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>732</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
         <v>725</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>1372</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>2</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>4</v>
       </c>
@@ -5068,7 +5068,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>12</v>
       </c>
@@ -5076,7 +5076,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>14</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
         <v>24</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>1377</v>
       </c>
@@ -18504,8 +18504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19403,7 +19403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -21278,10 +21278,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21290,644 +21290,884 @@
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>1221</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>69</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>71</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>77</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
         <v>79</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>81</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>82</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
         <v>84</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>86</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>88</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>90</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>20</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>105</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>30</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>109</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>112</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>114</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>26</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>122</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>124</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>126</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>129</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>132</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>134</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>136</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>138</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
         <v>140</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
         <v>141</v>
       </c>
       <c r="B63" s="20" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>143</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>145</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>147</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>149</v>
       </c>
       <c r="B67" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>150</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>725</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>726</v>
       </c>
       <c r="B70" s="20" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>727</v>
       </c>
       <c r="B71" s="20" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>729</v>
       </c>
       <c r="B72" s="20" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>731</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>91</v>
       </c>
       <c r="B74" s="20" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>97</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="20" t="s">
         <v>101</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
         <v>739</v>
       </c>
       <c r="B79" s="20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="20" t="s">
         <v>103</v>
       </c>
       <c r="B80" s="20" t="s">
         <v>104</v>
+      </c>
+      <c r="C80" s="27" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Draft of Ontario ETL tool - lookup tables, workspace, transformers
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="16" activeTab="26"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="20" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="1485">
   <si>
     <t>default_key</t>
   </si>
@@ -4508,6 +4508,12 @@
   </si>
   <si>
     <t>b7d9e240-6576-4ddc-b4cb-1c19e2116cf1</t>
+  </si>
+  <si>
+    <t>application/msaccess</t>
+  </si>
+  <si>
+    <t>current</t>
   </si>
 </sst>
 </file>
@@ -5977,10 +5983,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F470"/>
+  <dimension ref="A1:F471"/>
   <sheetViews>
-    <sheetView topLeftCell="A286" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A338" sqref="A338"/>
+    <sheetView topLeftCell="A432" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E461" sqref="E461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12663,6 +12669,20 @@
         <v>274</v>
       </c>
       <c r="D470" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B471" s="27" t="s">
+        <v>783</v>
+      </c>
+      <c r="C471" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D471" s="27" t="s">
         <v>275</v>
       </c>
     </row>
@@ -18181,7 +18201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
@@ -19882,10 +19902,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20356,6 +20376,20 @@
       </c>
       <c r="D33" s="27" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "First Draft of Ontario ETL tool - lookup tables, workspace, transformers"
This reverts commit 539bd5f8c7e2aeb8d9ea70195255e85db2568319.
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="20" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="16" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="1485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1483">
   <si>
     <t>default_key</t>
   </si>
@@ -4508,12 +4508,6 @@
   </si>
   <si>
     <t>b7d9e240-6576-4ddc-b4cb-1c19e2116cf1</t>
-  </si>
-  <si>
-    <t>application/msaccess</t>
-  </si>
-  <si>
-    <t>current</t>
   </si>
 </sst>
 </file>
@@ -5983,10 +5977,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F471"/>
+  <dimension ref="A1:F470"/>
   <sheetViews>
-    <sheetView topLeftCell="A432" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E461" sqref="E461"/>
+    <sheetView topLeftCell="A286" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12669,20 +12663,6 @@
         <v>274</v>
       </c>
       <c r="D470" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B471" s="27" t="s">
-        <v>783</v>
-      </c>
-      <c r="C471" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D471" s="27" t="s">
         <v>275</v>
       </c>
     </row>
@@ -18201,7 +18181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
@@ -19902,10 +19882,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20376,20 +20356,6 @@
       </c>
       <c r="D33" s="27" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1484</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ontario ETL tool first draft - lookup tables, workspace, transformers
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="20" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="1485">
   <si>
     <t>default_key</t>
   </si>
@@ -3739,6 +3739,9 @@
     <t>Gouvernement et municipalités du Québec</t>
   </si>
   <si>
+    <t>Government  and municipalities of Quebec</t>
+  </si>
+  <si>
     <t>jurisdiction</t>
   </si>
   <si>
@@ -4507,13 +4510,16 @@
     <t>b7d9e240-6576-4ddc-b4cb-1c19e2116cf1</t>
   </si>
   <si>
-    <t>Quebec Government and Municipalities</t>
+    <t>application/msaccess</t>
+  </si>
+  <si>
+    <t>current</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4646,8 +4652,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -4933,7 +4939,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -5001,7 +5007,7 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -5028,15 +5034,15 @@
         <v>28</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5049,10 +5055,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5073,7 +5079,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>518</v>
@@ -5108,12 +5114,12 @@
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>168</v>
@@ -5140,7 +5146,7 @@
         <v>728</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5148,7 +5154,7 @@
         <v>732</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5164,7 +5170,7 @@
         <v>725</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5177,7 +5183,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>25</v>
@@ -5188,7 +5194,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5196,7 +5202,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5212,7 +5218,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5220,7 +5226,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5281,11 +5287,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -5447,8 +5453,8 @@
       <c r="A20" s="7" t="s">
         <v>790</v>
       </c>
-      <c r="B20" t="s">
-        <v>1482</v>
+      <c r="B20" s="7" t="s">
+        <v>1226</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5517,63 +5523,63 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B31" t="s">
         <v>1233</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1232</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B33" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="B34" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="B35" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="B36" t="s">
         <v>518</v>
@@ -5581,34 +5587,34 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B37" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="B38" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B39" t="s">
         <v>1248</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="B40" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
     </row>
   </sheetData>
@@ -5628,7 +5634,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -5977,13 +5983,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F470"/>
+  <dimension ref="A1:F471"/>
   <sheetViews>
-    <sheetView topLeftCell="A286" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A338" sqref="A338"/>
+    <sheetView topLeftCell="A432" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E461" sqref="E461"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -12654,7 +12660,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
       <c r="B470" t="s">
         <v>324</v>
@@ -12663,6 +12669,20 @@
         <v>274</v>
       </c>
       <c r="D470" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B471" s="27" t="s">
+        <v>783</v>
+      </c>
+      <c r="C471" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D471" s="27" t="s">
         <v>275</v>
       </c>
     </row>
@@ -12683,17 +12703,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B1" t="s">
         <v>1291</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -12818,7 +12838,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
       <c r="B17" t="s">
         <v>783</v>
@@ -13059,7 +13079,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -13103,7 +13123,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -13278,7 +13298,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -13990,7 +14010,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -14208,7 +14228,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -14291,7 +14311,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -15268,7 +15288,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -15443,7 +15463,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
@@ -15452,101 +15472,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="B3" t="s">
         <v>791</v>
       </c>
       <c r="C3" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="B4" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="C4" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="B5" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
       <c r="C5" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="B6" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="C6" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="B9" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
       <c r="C9" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -15557,7 +15577,7 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -15568,7 +15588,7 @@
         <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -15579,7 +15599,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -15590,7 +15610,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -15601,29 +15621,29 @@
         <v>794</v>
       </c>
       <c r="C14" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B16" t="s">
         <v>1341</v>
       </c>
-      <c r="B16" t="s">
-        <v>1340</v>
-      </c>
       <c r="C16" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -15634,95 +15654,95 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="C19" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="C20" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="B21" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="C21" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B22" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="C22" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="C24" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="B25" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="C25" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -15733,7 +15753,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -15744,194 +15764,194 @@
         <v>790</v>
       </c>
       <c r="C27" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="B28" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="C28" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="B29" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="C29" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="B30" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="C30" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="C31" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B32" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="C32" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="B33" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="C33" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="B34" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="C34" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="B35" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="C35" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="B36" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="C36" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="B37" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="C37" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="B38" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="C38" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="B40" t="s">
         <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="B41" t="s">
         <v>856</v>
       </c>
       <c r="C41" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B42" t="s">
         <v>1330</v>
       </c>
-      <c r="B42" t="s">
-        <v>1329</v>
-      </c>
       <c r="C42" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B43" t="s">
         <v>1328</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>1327</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="B44" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="C44" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
   </sheetData>
@@ -15947,46 +15967,46 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B1" t="s">
         <v>1291</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B2" t="s">
         <v>1359</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1358</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B3" t="s">
         <v>1357</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1356</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="B4" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B5" t="s">
         <v>1354</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1353</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -15994,7 +16014,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
   </sheetData>
@@ -16010,7 +16030,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -16269,7 +16289,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -16279,282 +16299,282 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>1395</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>1394</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C17" s="25" t="s">
         <v>1396</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>1379</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>1395</v>
-      </c>
       <c r="D17" s="24" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
     </row>
   </sheetData>
@@ -16577,11 +16597,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -16604,7 +16624,7 @@
         <v>976</v>
       </c>
       <c r="E1" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -16612,16 +16632,16 @@
         <v>883</v>
       </c>
       <c r="B2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C2" t="s">
         <v>1279</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1278</v>
       </c>
       <c r="D2" t="s">
         <v>889</v>
       </c>
       <c r="E2" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16638,7 +16658,7 @@
         <v>889</v>
       </c>
       <c r="E3" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -16655,7 +16675,7 @@
         <v>889</v>
       </c>
       <c r="E4" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -16672,7 +16692,7 @@
         <v>889</v>
       </c>
       <c r="E5" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -16689,7 +16709,7 @@
         <v>889</v>
       </c>
       <c r="E6" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -16706,7 +16726,7 @@
         <v>889</v>
       </c>
       <c r="E7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -16723,7 +16743,7 @@
         <v>889</v>
       </c>
       <c r="E8" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -16740,7 +16760,7 @@
         <v>889</v>
       </c>
       <c r="E9" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -16757,7 +16777,7 @@
         <v>889</v>
       </c>
       <c r="E10" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -16774,7 +16794,7 @@
         <v>889</v>
       </c>
       <c r="E11" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -16791,7 +16811,7 @@
         <v>889</v>
       </c>
       <c r="E12" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -16808,7 +16828,7 @@
         <v>889</v>
       </c>
       <c r="E13" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -16825,7 +16845,7 @@
         <v>889</v>
       </c>
       <c r="E14" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -16842,7 +16862,7 @@
         <v>889</v>
       </c>
       <c r="E15" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -16859,7 +16879,7 @@
         <v>889</v>
       </c>
       <c r="E16" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -16876,7 +16896,7 @@
         <v>889</v>
       </c>
       <c r="E17" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -16893,7 +16913,7 @@
         <v>889</v>
       </c>
       <c r="E18" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -16910,7 +16930,7 @@
         <v>889</v>
       </c>
       <c r="E19" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -16927,7 +16947,7 @@
         <v>889</v>
       </c>
       <c r="E20" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -16944,7 +16964,7 @@
         <v>889</v>
       </c>
       <c r="E21" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -16961,7 +16981,7 @@
         <v>889</v>
       </c>
       <c r="E22" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -16978,7 +16998,7 @@
         <v>889</v>
       </c>
       <c r="E23" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -16995,7 +17015,7 @@
         <v>889</v>
       </c>
       <c r="E24" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -17012,7 +17032,7 @@
         <v>889</v>
       </c>
       <c r="E25" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -17029,7 +17049,7 @@
         <v>889</v>
       </c>
       <c r="E26" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -17046,7 +17066,7 @@
         <v>889</v>
       </c>
       <c r="E27" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -17063,7 +17083,7 @@
         <v>889</v>
       </c>
       <c r="E28" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -17080,7 +17100,7 @@
         <v>889</v>
       </c>
       <c r="E29" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -17097,7 +17117,7 @@
         <v>889</v>
       </c>
       <c r="E30" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -17114,7 +17134,7 @@
         <v>889</v>
       </c>
       <c r="E31" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -17122,16 +17142,16 @@
         <v>936</v>
       </c>
       <c r="B32" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C32" t="s">
         <v>1260</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1259</v>
       </c>
       <c r="D32" t="s">
         <v>889</v>
       </c>
       <c r="E32" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -17148,7 +17168,7 @@
         <v>889</v>
       </c>
       <c r="E33" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -17156,7 +17176,7 @@
         <v>974</v>
       </c>
       <c r="B34" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="C34" t="s">
         <v>937</v>
@@ -17165,7 +17185,7 @@
         <v>889</v>
       </c>
       <c r="E34" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -17182,7 +17202,7 @@
         <v>889</v>
       </c>
       <c r="E35" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -17199,7 +17219,7 @@
         <v>889</v>
       </c>
       <c r="E36" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -17216,7 +17236,7 @@
         <v>889</v>
       </c>
       <c r="E37" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -17233,7 +17253,7 @@
         <v>889</v>
       </c>
       <c r="E38" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -17250,7 +17270,7 @@
         <v>889</v>
       </c>
       <c r="E39" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -17267,7 +17287,7 @@
         <v>889</v>
       </c>
       <c r="E40" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -17278,13 +17298,13 @@
         <v>887</v>
       </c>
       <c r="C41" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="D41" t="s">
         <v>889</v>
       </c>
       <c r="E41" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -17292,16 +17312,16 @@
         <v>890</v>
       </c>
       <c r="B42" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="D42" t="s">
         <v>889</v>
       </c>
       <c r="E42" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -17309,16 +17329,16 @@
         <v>891</v>
       </c>
       <c r="B43" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="C43" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D43" t="s">
         <v>889</v>
       </c>
       <c r="E43" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -17335,7 +17355,7 @@
         <v>886</v>
       </c>
       <c r="E44" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -17352,7 +17372,7 @@
         <v>886</v>
       </c>
       <c r="E45" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -17360,16 +17380,16 @@
         <v>894</v>
       </c>
       <c r="B46" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="C46" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="D46" t="s">
         <v>889</v>
       </c>
       <c r="E46" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -17380,13 +17400,13 @@
         <v>898</v>
       </c>
       <c r="C47" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="D47" t="s">
         <v>889</v>
       </c>
       <c r="E47" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -17394,16 +17414,16 @@
         <v>900</v>
       </c>
       <c r="B48" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="C48" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="D48" t="s">
         <v>889</v>
       </c>
       <c r="E48" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -17420,7 +17440,7 @@
         <v>886</v>
       </c>
       <c r="E49" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -17431,13 +17451,13 @@
         <v>902</v>
       </c>
       <c r="C50" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="D50" t="s">
         <v>889</v>
       </c>
       <c r="E50" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -17454,7 +17474,7 @@
         <v>886</v>
       </c>
       <c r="E51" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -17465,13 +17485,13 @@
         <v>908</v>
       </c>
       <c r="C52" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="D52" t="s">
         <v>889</v>
       </c>
       <c r="E52" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -17479,16 +17499,16 @@
         <v>909</v>
       </c>
       <c r="B53" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="C53" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="D53" t="s">
         <v>889</v>
       </c>
       <c r="E53" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -17499,13 +17519,13 @@
         <v>928</v>
       </c>
       <c r="C54" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="D54" t="s">
         <v>889</v>
       </c>
       <c r="E54" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -17522,7 +17542,7 @@
         <v>886</v>
       </c>
       <c r="E55" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -17533,13 +17553,13 @@
         <v>930</v>
       </c>
       <c r="C56" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="D56" t="s">
         <v>889</v>
       </c>
       <c r="E56" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -17550,13 +17570,13 @@
         <v>931</v>
       </c>
       <c r="C57" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="D57" t="s">
         <v>889</v>
       </c>
       <c r="E57" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -17564,16 +17584,16 @@
         <v>941</v>
       </c>
       <c r="B58" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C58" t="s">
         <v>1263</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1262</v>
       </c>
       <c r="D58" t="s">
         <v>889</v>
       </c>
       <c r="E58" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -17581,16 +17601,16 @@
         <v>942</v>
       </c>
       <c r="B59" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="C59" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="D59" t="s">
         <v>889</v>
       </c>
       <c r="E59" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -17598,16 +17618,16 @@
         <v>943</v>
       </c>
       <c r="B60" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="C60" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="D60" t="s">
         <v>889</v>
       </c>
       <c r="E60" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -17615,16 +17635,16 @@
         <v>944</v>
       </c>
       <c r="B61" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="C61" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="D61" t="s">
         <v>889</v>
       </c>
       <c r="E61" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -17635,13 +17655,13 @@
         <v>945</v>
       </c>
       <c r="C62" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="D62" t="s">
         <v>889</v>
       </c>
       <c r="E62" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -17658,7 +17678,7 @@
         <v>886</v>
       </c>
       <c r="E63" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -17669,13 +17689,13 @@
         <v>947</v>
       </c>
       <c r="C64" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
       <c r="D64" t="s">
         <v>889</v>
       </c>
       <c r="E64" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -17683,16 +17703,16 @@
         <v>949</v>
       </c>
       <c r="B65" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="C65" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="D65" t="s">
         <v>889</v>
       </c>
       <c r="E65" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -17700,16 +17720,16 @@
         <v>950</v>
       </c>
       <c r="B66" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="C66" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="D66" t="s">
         <v>889</v>
       </c>
       <c r="E66" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -17717,16 +17737,16 @@
         <v>975</v>
       </c>
       <c r="B67" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="D67" t="s">
         <v>889</v>
       </c>
       <c r="E67" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -17743,7 +17763,7 @@
         <v>889</v>
       </c>
       <c r="E68" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -17760,7 +17780,7 @@
         <v>889</v>
       </c>
       <c r="E69" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -17777,7 +17797,7 @@
         <v>889</v>
       </c>
       <c r="E70" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -17794,7 +17814,7 @@
         <v>889</v>
       </c>
       <c r="E71" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -17811,7 +17831,7 @@
         <v>889</v>
       </c>
       <c r="E72" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -17828,7 +17848,7 @@
         <v>889</v>
       </c>
       <c r="E73" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -17845,7 +17865,7 @@
         <v>889</v>
       </c>
       <c r="E74" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -17862,7 +17882,7 @@
         <v>889</v>
       </c>
       <c r="E75" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -17879,7 +17899,7 @@
         <v>889</v>
       </c>
       <c r="E76" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -17902,7 +17922,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
@@ -17910,7 +17930,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>8</v>
@@ -17918,7 +17938,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>567</v>
@@ -17926,7 +17946,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>567</v>
@@ -17934,7 +17954,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>567</v>
@@ -17942,7 +17962,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>567</v>
@@ -17950,7 +17970,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>567</v>
@@ -17958,7 +17978,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>567</v>
@@ -17966,7 +17986,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>567</v>
@@ -17974,7 +17994,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>567</v>
@@ -17982,7 +18002,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>567</v>
@@ -17990,7 +18010,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>567</v>
@@ -17998,7 +18018,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>567</v>
@@ -18006,7 +18026,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>567</v>
@@ -18014,7 +18034,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>567</v>
@@ -18022,7 +18042,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>567</v>
@@ -18030,7 +18050,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>567</v>
@@ -18038,7 +18058,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>567</v>
@@ -18046,7 +18066,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>567</v>
@@ -18054,7 +18074,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>567</v>
@@ -18062,7 +18082,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>567</v>
@@ -18070,7 +18090,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>567</v>
@@ -18078,7 +18098,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>567</v>
@@ -18086,7 +18106,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>567</v>
@@ -18094,7 +18114,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>567</v>
@@ -18102,7 +18122,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>567</v>
@@ -18110,7 +18130,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>567</v>
@@ -18118,7 +18138,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>567</v>
@@ -18126,7 +18146,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>567</v>
@@ -18134,7 +18154,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>567</v>
@@ -18142,7 +18162,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>567</v>
@@ -18150,7 +18170,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -18158,7 +18178,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -18166,7 +18186,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>567</v>
@@ -18185,7 +18205,7 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
@@ -18201,7 +18221,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
       <c r="B2" t="s">
         <v>564</v>
@@ -18209,7 +18229,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>564</v>
@@ -18217,7 +18237,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>564</v>
@@ -18225,7 +18245,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>564</v>
@@ -18233,7 +18253,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>564</v>
@@ -18241,7 +18261,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>564</v>
@@ -18249,7 +18269,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -18257,7 +18277,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1449</v>
+        <v>1450</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>9</v>
@@ -18265,7 +18285,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1450</v>
+        <v>1451</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>9</v>
@@ -18273,7 +18293,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1451</v>
+        <v>1452</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>9</v>
@@ -18281,7 +18301,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1452</v>
+        <v>1453</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>9</v>
@@ -18289,7 +18309,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1453</v>
+        <v>1454</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>9</v>
@@ -18297,7 +18317,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1454</v>
+        <v>1455</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>564</v>
@@ -18305,7 +18325,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1455</v>
+        <v>1456</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>9</v>
@@ -18313,7 +18333,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1456</v>
+        <v>1457</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>564</v>
@@ -18321,7 +18341,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1457</v>
+        <v>1458</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>9</v>
@@ -18329,7 +18349,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1458</v>
+        <v>1459</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>9</v>
@@ -18337,7 +18357,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1459</v>
+        <v>1460</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>9</v>
@@ -18345,7 +18365,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1460</v>
+        <v>1461</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>9</v>
@@ -18353,7 +18373,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1461</v>
+        <v>1462</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>9</v>
@@ -18361,7 +18381,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1462</v>
+        <v>1463</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>9</v>
@@ -18369,7 +18389,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1463</v>
+        <v>1464</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>564</v>
@@ -18377,7 +18397,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1464</v>
+        <v>1465</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>564</v>
@@ -18385,7 +18405,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1465</v>
+        <v>1466</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>9</v>
@@ -18393,7 +18413,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1466</v>
+        <v>1467</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>9</v>
@@ -18401,7 +18421,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1467</v>
+        <v>1468</v>
       </c>
       <c r="B27" t="s">
         <v>567</v>
@@ -18409,7 +18429,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1468</v>
+        <v>1469</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>564</v>
@@ -18417,7 +18437,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1469</v>
+        <v>1470</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>564</v>
@@ -18425,7 +18445,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1470</v>
+        <v>1471</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>9</v>
@@ -18433,7 +18453,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1471</v>
+        <v>1472</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -18441,7 +18461,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1472</v>
+        <v>1473</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -18449,7 +18469,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1473</v>
+        <v>1474</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>9</v>
@@ -18457,7 +18477,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1474</v>
+        <v>1475</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>9</v>
@@ -18465,7 +18485,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1475</v>
+        <v>1476</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>9</v>
@@ -18473,7 +18493,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>9</v>
@@ -18481,7 +18501,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1477</v>
+        <v>1478</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>9</v>
@@ -18489,7 +18509,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1478</v>
+        <v>1479</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>9</v>
@@ -18497,7 +18517,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1479</v>
+        <v>1480</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>9</v>
@@ -18505,7 +18525,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1480</v>
+        <v>1481</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>9</v>
@@ -18513,7 +18533,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1481</v>
+        <v>1482</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>564</v>
@@ -18532,7 +18552,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -18697,7 +18717,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -18816,7 +18836,7 @@
       <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -19715,7 +19735,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
@@ -19723,13 +19743,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
       <c r="B1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C1" t="s">
         <v>1324</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1323</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -19740,139 +19760,139 @@
         <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
       <c r="B3" t="s">
         <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
       <c r="B4" t="s">
         <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="B5" t="s">
         <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
       <c r="B6" t="s">
         <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
       <c r="B7" t="s">
         <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
       <c r="B8" t="s">
         <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="B9" t="s">
         <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="B10" t="s">
         <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
       <c r="B11" t="s">
         <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="B12" t="s">
         <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="B13" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
       <c r="C13" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
       <c r="B14" t="s">
         <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
     </row>
   </sheetData>
@@ -19882,13 +19902,13 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -20290,7 +20310,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>226</v>
@@ -20318,7 +20338,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>221</v>
@@ -20332,7 +20352,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>226</v>
@@ -20346,7 +20366,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>25</v>
@@ -20356,6 +20376,20 @@
       </c>
       <c r="D33" s="27" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -20372,14 +20406,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B1" t="s">
         <v>1291</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -20395,7 +20429,7 @@
         <v>860</v>
       </c>
       <c r="B3" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20403,7 +20437,7 @@
         <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -20411,7 +20445,7 @@
         <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20427,7 +20461,7 @@
         <v>861</v>
       </c>
       <c r="B7" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -20435,7 +20469,7 @@
         <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -20451,7 +20485,7 @@
         <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -20459,7 +20493,7 @@
         <v>863</v>
       </c>
       <c r="B11" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -20467,7 +20501,7 @@
         <v>864</v>
       </c>
       <c r="B12" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -20475,7 +20509,7 @@
         <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -20483,7 +20517,7 @@
         <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -20491,7 +20525,7 @@
         <v>865</v>
       </c>
       <c r="B15" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -20515,7 +20549,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -21646,7 +21680,7 @@
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -21836,7 +21870,7 @@
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -22735,7 +22769,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -23635,7 +23669,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -23898,7 +23932,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -23933,7 +23967,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>
@@ -24267,7 +24301,7 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Revert "Ontario ETL tool first draft - lookup tables, workspace, transformers"
This reverts commit 26cff72f2c7ac8e719dabca3fa265d459e746ad3.
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="20" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="1485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1483">
   <si>
     <t>default_key</t>
   </si>
@@ -3739,9 +3739,6 @@
     <t>Gouvernement et municipalités du Québec</t>
   </si>
   <si>
-    <t>Government  and municipalities of Quebec</t>
-  </si>
-  <si>
     <t>jurisdiction</t>
   </si>
   <si>
@@ -4510,16 +4507,13 @@
     <t>b7d9e240-6576-4ddc-b4cb-1c19e2116cf1</t>
   </si>
   <si>
-    <t>application/msaccess</t>
-  </si>
-  <si>
-    <t>current</t>
+    <t>Quebec Government and Municipalities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4652,8 +4646,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -4939,7 +4933,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -5007,7 +5001,7 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -5034,15 +5028,15 @@
         <v>28</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5055,10 +5049,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>1364</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>1365</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5079,7 +5073,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>518</v>
@@ -5114,12 +5108,12 @@
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>168</v>
@@ -5146,7 +5140,7 @@
         <v>728</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5154,7 +5148,7 @@
         <v>732</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5170,7 +5164,7 @@
         <v>725</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5183,7 +5177,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>25</v>
@@ -5194,7 +5188,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5202,7 +5196,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5218,7 +5212,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5226,7 +5220,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5287,11 +5281,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -5453,8 +5447,8 @@
       <c r="A20" s="7" t="s">
         <v>790</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>1226</v>
+      <c r="B20" t="s">
+        <v>1482</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -5523,63 +5517,63 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>1230</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>1231</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>1232</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B31" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>1235</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>1236</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B33" t="s">
         <v>1237</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1238</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B34" t="s">
         <v>1239</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B35" t="s">
         <v>1241</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1242</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B36" t="s">
         <v>518</v>
@@ -5587,34 +5581,34 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B37" t="s">
         <v>1244</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1245</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B38" t="s">
         <v>1246</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B39" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B40" t="s">
         <v>1250</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1251</v>
       </c>
     </row>
   </sheetData>
@@ -5634,7 +5628,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -5983,13 +5977,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F471"/>
+  <dimension ref="A1:F470"/>
   <sheetViews>
-    <sheetView topLeftCell="A432" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E461" sqref="E461"/>
+    <sheetView topLeftCell="A286" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -12660,7 +12654,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B470" t="s">
         <v>324</v>
@@ -12669,20 +12663,6 @@
         <v>274</v>
       </c>
       <c r="D470" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A471" t="s">
-        <v>1483</v>
-      </c>
-      <c r="B471" s="27" t="s">
-        <v>783</v>
-      </c>
-      <c r="C471" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D471" s="27" t="s">
         <v>275</v>
       </c>
     </row>
@@ -12703,17 +12683,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -12838,7 +12818,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="B17" t="s">
         <v>783</v>
@@ -13079,7 +13059,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -13123,7 +13103,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -13298,7 +13278,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -14010,7 +13990,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -14228,7 +14208,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -14311,7 +14291,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -15288,7 +15268,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -15463,7 +15443,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
@@ -15472,101 +15452,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="B3" t="s">
         <v>791</v>
       </c>
       <c r="C3" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="B4" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="C4" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="B5" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="C5" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B6" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="C6" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="B9" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="C9" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -15577,7 +15557,7 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -15588,7 +15568,7 @@
         <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -15599,7 +15579,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -15610,7 +15590,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -15621,29 +15601,29 @@
         <v>794</v>
       </c>
       <c r="C14" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="B16" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="C16" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -15654,95 +15634,95 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="C19" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C20" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B21" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C21" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B22" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="C22" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="C24" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B25" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C25" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -15753,7 +15733,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -15764,194 +15744,194 @@
         <v>790</v>
       </c>
       <c r="C27" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="B28" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="C28" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="B29" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="C29" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B30" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="C30" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="C31" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="B32" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C32" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B33" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C33" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="B34" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C34" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="B35" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C35" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="B36" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="C36" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="B37" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="C37" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C38" t="s">
         <v>1325</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1325</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="B40" t="s">
         <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="B41" t="s">
         <v>856</v>
       </c>
       <c r="C41" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="B42" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="C42" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="B43" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="C43" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="B44" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="C44" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
   </sheetData>
@@ -15967,46 +15947,46 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B2" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B3" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B4" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="B5" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -16014,7 +15994,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
     </row>
   </sheetData>
@@ -16030,7 +16010,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -16289,7 +16269,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -16299,282 +16279,282 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>1387</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>1388</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>1391</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>1392</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>1394</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="C16" s="25" t="s">
         <v>1395</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>1396</v>
-      </c>
       <c r="D16" s="24" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>1398</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>1399</v>
-      </c>
       <c r="C18" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>1403</v>
       </c>
-      <c r="B22" s="24" t="s">
-        <v>1404</v>
-      </c>
       <c r="C22" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
     </row>
   </sheetData>
@@ -16597,11 +16577,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -16624,7 +16604,7 @@
         <v>976</v>
       </c>
       <c r="E1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -16632,16 +16612,16 @@
         <v>883</v>
       </c>
       <c r="B2" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C2" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="D2" t="s">
         <v>889</v>
       </c>
       <c r="E2" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -16658,7 +16638,7 @@
         <v>889</v>
       </c>
       <c r="E3" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -16675,7 +16655,7 @@
         <v>889</v>
       </c>
       <c r="E4" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -16692,7 +16672,7 @@
         <v>889</v>
       </c>
       <c r="E5" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -16709,7 +16689,7 @@
         <v>889</v>
       </c>
       <c r="E6" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -16726,7 +16706,7 @@
         <v>889</v>
       </c>
       <c r="E7" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -16743,7 +16723,7 @@
         <v>889</v>
       </c>
       <c r="E8" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -16760,7 +16740,7 @@
         <v>889</v>
       </c>
       <c r="E9" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -16777,7 +16757,7 @@
         <v>889</v>
       </c>
       <c r="E10" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -16794,7 +16774,7 @@
         <v>889</v>
       </c>
       <c r="E11" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -16811,7 +16791,7 @@
         <v>889</v>
       </c>
       <c r="E12" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -16828,7 +16808,7 @@
         <v>889</v>
       </c>
       <c r="E13" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -16845,7 +16825,7 @@
         <v>889</v>
       </c>
       <c r="E14" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -16862,7 +16842,7 @@
         <v>889</v>
       </c>
       <c r="E15" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -16879,7 +16859,7 @@
         <v>889</v>
       </c>
       <c r="E16" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -16896,7 +16876,7 @@
         <v>889</v>
       </c>
       <c r="E17" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -16913,7 +16893,7 @@
         <v>889</v>
       </c>
       <c r="E18" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -16930,7 +16910,7 @@
         <v>889</v>
       </c>
       <c r="E19" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -16947,7 +16927,7 @@
         <v>889</v>
       </c>
       <c r="E20" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -16964,7 +16944,7 @@
         <v>889</v>
       </c>
       <c r="E21" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -16981,7 +16961,7 @@
         <v>889</v>
       </c>
       <c r="E22" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -16998,7 +16978,7 @@
         <v>889</v>
       </c>
       <c r="E23" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -17015,7 +16995,7 @@
         <v>889</v>
       </c>
       <c r="E24" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -17032,7 +17012,7 @@
         <v>889</v>
       </c>
       <c r="E25" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -17049,7 +17029,7 @@
         <v>889</v>
       </c>
       <c r="E26" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -17066,7 +17046,7 @@
         <v>889</v>
       </c>
       <c r="E27" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -17083,7 +17063,7 @@
         <v>889</v>
       </c>
       <c r="E28" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -17100,7 +17080,7 @@
         <v>889</v>
       </c>
       <c r="E29" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -17117,7 +17097,7 @@
         <v>889</v>
       </c>
       <c r="E30" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -17134,7 +17114,7 @@
         <v>889</v>
       </c>
       <c r="E31" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -17142,16 +17122,16 @@
         <v>936</v>
       </c>
       <c r="B32" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C32" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="D32" t="s">
         <v>889</v>
       </c>
       <c r="E32" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -17168,7 +17148,7 @@
         <v>889</v>
       </c>
       <c r="E33" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -17176,7 +17156,7 @@
         <v>974</v>
       </c>
       <c r="B34" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C34" t="s">
         <v>937</v>
@@ -17185,7 +17165,7 @@
         <v>889</v>
       </c>
       <c r="E34" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -17202,7 +17182,7 @@
         <v>889</v>
       </c>
       <c r="E35" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -17219,7 +17199,7 @@
         <v>889</v>
       </c>
       <c r="E36" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -17236,7 +17216,7 @@
         <v>889</v>
       </c>
       <c r="E37" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -17253,7 +17233,7 @@
         <v>889</v>
       </c>
       <c r="E38" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -17270,7 +17250,7 @@
         <v>889</v>
       </c>
       <c r="E39" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -17287,7 +17267,7 @@
         <v>889</v>
       </c>
       <c r="E40" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -17298,13 +17278,13 @@
         <v>887</v>
       </c>
       <c r="C41" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="D41" t="s">
         <v>889</v>
       </c>
       <c r="E41" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -17312,16 +17292,16 @@
         <v>890</v>
       </c>
       <c r="B42" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>1252</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>1253</v>
       </c>
       <c r="D42" t="s">
         <v>889</v>
       </c>
       <c r="E42" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -17329,16 +17309,16 @@
         <v>891</v>
       </c>
       <c r="B43" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C43" t="s">
         <v>1254</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1255</v>
       </c>
       <c r="D43" t="s">
         <v>889</v>
       </c>
       <c r="E43" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -17355,7 +17335,7 @@
         <v>886</v>
       </c>
       <c r="E44" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -17372,7 +17352,7 @@
         <v>886</v>
       </c>
       <c r="E45" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -17380,16 +17360,16 @@
         <v>894</v>
       </c>
       <c r="B46" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C46" t="s">
         <v>1256</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1257</v>
       </c>
       <c r="D46" t="s">
         <v>889</v>
       </c>
       <c r="E46" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -17400,13 +17380,13 @@
         <v>898</v>
       </c>
       <c r="C47" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="D47" t="s">
         <v>889</v>
       </c>
       <c r="E47" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -17414,16 +17394,16 @@
         <v>900</v>
       </c>
       <c r="B48" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C48" t="s">
         <v>1258</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1259</v>
       </c>
       <c r="D48" t="s">
         <v>889</v>
       </c>
       <c r="E48" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -17440,7 +17420,7 @@
         <v>886</v>
       </c>
       <c r="E49" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -17451,13 +17431,13 @@
         <v>902</v>
       </c>
       <c r="C50" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="D50" t="s">
         <v>889</v>
       </c>
       <c r="E50" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -17474,7 +17454,7 @@
         <v>886</v>
       </c>
       <c r="E51" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -17485,13 +17465,13 @@
         <v>908</v>
       </c>
       <c r="C52" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="D52" t="s">
         <v>889</v>
       </c>
       <c r="E52" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -17499,16 +17479,16 @@
         <v>909</v>
       </c>
       <c r="B53" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C53" t="s">
         <v>1275</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1276</v>
       </c>
       <c r="D53" t="s">
         <v>889</v>
       </c>
       <c r="E53" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -17519,13 +17499,13 @@
         <v>928</v>
       </c>
       <c r="C54" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="D54" t="s">
         <v>889</v>
       </c>
       <c r="E54" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -17542,7 +17522,7 @@
         <v>886</v>
       </c>
       <c r="E55" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -17553,13 +17533,13 @@
         <v>930</v>
       </c>
       <c r="C56" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D56" t="s">
         <v>889</v>
       </c>
       <c r="E56" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -17570,13 +17550,13 @@
         <v>931</v>
       </c>
       <c r="C57" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="D57" t="s">
         <v>889</v>
       </c>
       <c r="E57" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -17584,16 +17564,16 @@
         <v>941</v>
       </c>
       <c r="B58" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C58" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="D58" t="s">
         <v>889</v>
       </c>
       <c r="E58" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -17601,16 +17581,16 @@
         <v>942</v>
       </c>
       <c r="B59" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C59" t="s">
         <v>1265</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1266</v>
       </c>
       <c r="D59" t="s">
         <v>889</v>
       </c>
       <c r="E59" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -17618,16 +17598,16 @@
         <v>943</v>
       </c>
       <c r="B60" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C60" t="s">
         <v>1267</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1268</v>
       </c>
       <c r="D60" t="s">
         <v>889</v>
       </c>
       <c r="E60" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -17635,16 +17615,16 @@
         <v>944</v>
       </c>
       <c r="B61" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C61" t="s">
         <v>1269</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1270</v>
       </c>
       <c r="D61" t="s">
         <v>889</v>
       </c>
       <c r="E61" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -17655,13 +17635,13 @@
         <v>945</v>
       </c>
       <c r="C62" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="D62" t="s">
         <v>889</v>
       </c>
       <c r="E62" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -17678,7 +17658,7 @@
         <v>886</v>
       </c>
       <c r="E63" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -17689,13 +17669,13 @@
         <v>947</v>
       </c>
       <c r="C64" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="D64" t="s">
         <v>889</v>
       </c>
       <c r="E64" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -17703,16 +17683,16 @@
         <v>949</v>
       </c>
       <c r="B65" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C65" t="s">
         <v>1277</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1278</v>
       </c>
       <c r="D65" t="s">
         <v>889</v>
       </c>
       <c r="E65" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -17720,16 +17700,16 @@
         <v>950</v>
       </c>
       <c r="B66" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C66" t="s">
         <v>1271</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1272</v>
       </c>
       <c r="D66" t="s">
         <v>889</v>
       </c>
       <c r="E66" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -17737,16 +17717,16 @@
         <v>975</v>
       </c>
       <c r="B67" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>1273</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>1274</v>
       </c>
       <c r="D67" t="s">
         <v>889</v>
       </c>
       <c r="E67" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -17763,7 +17743,7 @@
         <v>889</v>
       </c>
       <c r="E68" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -17780,7 +17760,7 @@
         <v>889</v>
       </c>
       <c r="E69" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -17797,7 +17777,7 @@
         <v>889</v>
       </c>
       <c r="E70" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -17814,7 +17794,7 @@
         <v>889</v>
       </c>
       <c r="E71" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -17831,7 +17811,7 @@
         <v>889</v>
       </c>
       <c r="E72" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -17848,7 +17828,7 @@
         <v>889</v>
       </c>
       <c r="E73" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -17865,7 +17845,7 @@
         <v>889</v>
       </c>
       <c r="E74" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -17882,7 +17862,7 @@
         <v>889</v>
       </c>
       <c r="E75" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -17899,7 +17879,7 @@
         <v>889</v>
       </c>
       <c r="E76" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
   </sheetData>
@@ -17922,7 +17902,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
@@ -17930,7 +17910,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>8</v>
@@ -17938,7 +17918,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>567</v>
@@ -17946,7 +17926,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>567</v>
@@ -17954,7 +17934,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>567</v>
@@ -17962,7 +17942,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>567</v>
@@ -17970,7 +17950,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>567</v>
@@ -17978,7 +17958,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>567</v>
@@ -17986,7 +17966,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>567</v>
@@ -17994,7 +17974,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>567</v>
@@ -18002,7 +17982,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>567</v>
@@ -18010,7 +17990,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>567</v>
@@ -18018,7 +17998,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>567</v>
@@ -18026,7 +18006,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>567</v>
@@ -18034,7 +18014,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>567</v>
@@ -18042,7 +18022,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>567</v>
@@ -18050,7 +18030,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>567</v>
@@ -18058,7 +18038,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>567</v>
@@ -18066,7 +18046,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>567</v>
@@ -18074,7 +18054,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>567</v>
@@ -18082,7 +18062,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>567</v>
@@ -18090,7 +18070,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>567</v>
@@ -18098,7 +18078,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>567</v>
@@ -18106,7 +18086,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>567</v>
@@ -18114,7 +18094,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>567</v>
@@ -18122,7 +18102,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>567</v>
@@ -18130,7 +18110,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>567</v>
@@ -18138,7 +18118,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>567</v>
@@ -18146,7 +18126,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>567</v>
@@ -18154,7 +18134,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>567</v>
@@ -18162,7 +18142,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>567</v>
@@ -18170,7 +18150,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -18178,7 +18158,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -18186,7 +18166,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>567</v>
@@ -18205,7 +18185,7 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
@@ -18221,7 +18201,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="B2" t="s">
         <v>564</v>
@@ -18229,7 +18209,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>564</v>
@@ -18237,7 +18217,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>564</v>
@@ -18245,7 +18225,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>564</v>
@@ -18253,7 +18233,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>564</v>
@@ -18261,7 +18241,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>564</v>
@@ -18269,7 +18249,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -18277,7 +18257,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>9</v>
@@ -18285,7 +18265,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>9</v>
@@ -18293,7 +18273,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>9</v>
@@ -18301,7 +18281,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>9</v>
@@ -18309,7 +18289,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>9</v>
@@ -18317,7 +18297,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>564</v>
@@ -18325,7 +18305,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>9</v>
@@ -18333,7 +18313,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>564</v>
@@ -18341,7 +18321,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>9</v>
@@ -18349,7 +18329,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>9</v>
@@ -18357,7 +18337,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>9</v>
@@ -18365,7 +18345,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>9</v>
@@ -18373,7 +18353,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>9</v>
@@ -18381,7 +18361,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>9</v>
@@ -18389,7 +18369,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>564</v>
@@ -18397,7 +18377,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>564</v>
@@ -18405,7 +18385,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>9</v>
@@ -18413,7 +18393,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>9</v>
@@ -18421,7 +18401,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B27" t="s">
         <v>567</v>
@@ -18429,7 +18409,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>564</v>
@@ -18437,7 +18417,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>564</v>
@@ -18445,7 +18425,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>9</v>
@@ -18453,7 +18433,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -18461,7 +18441,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -18469,7 +18449,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>9</v>
@@ -18477,7 +18457,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>9</v>
@@ -18485,7 +18465,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>9</v>
@@ -18493,7 +18473,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>9</v>
@@ -18501,7 +18481,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>9</v>
@@ -18509,7 +18489,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>9</v>
@@ -18517,7 +18497,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>9</v>
@@ -18525,7 +18505,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>9</v>
@@ -18533,7 +18513,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>564</v>
@@ -18552,7 +18532,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -18717,7 +18697,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -18836,7 +18816,7 @@
       <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -19735,7 +19715,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
@@ -19743,13 +19723,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C1" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -19760,139 +19740,139 @@
         <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="B3" t="s">
         <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="B4" t="s">
         <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="B5" t="s">
         <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="B6" t="s">
         <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="B7" t="s">
         <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="B8" t="s">
         <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="B9" t="s">
         <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B10" t="s">
         <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="B11" t="s">
         <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="B12" t="s">
         <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="B13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="C13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B14" t="s">
         <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
   </sheetData>
@@ -19902,13 +19882,13 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -20310,7 +20290,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>226</v>
@@ -20338,7 +20318,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>221</v>
@@ -20352,7 +20332,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>226</v>
@@ -20366,7 +20346,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>25</v>
@@ -20376,20 +20356,6 @@
       </c>
       <c r="D33" s="27" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1484</v>
-      </c>
-      <c r="B34" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>233</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -20406,14 +20372,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -20429,7 +20395,7 @@
         <v>860</v>
       </c>
       <c r="B3" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -20437,7 +20403,7 @@
         <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -20445,7 +20411,7 @@
         <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -20461,7 +20427,7 @@
         <v>861</v>
       </c>
       <c r="B7" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -20469,7 +20435,7 @@
         <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -20485,7 +20451,7 @@
         <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -20493,7 +20459,7 @@
         <v>863</v>
       </c>
       <c r="B11" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -20501,7 +20467,7 @@
         <v>864</v>
       </c>
       <c r="B12" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -20509,7 +20475,7 @@
         <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -20517,7 +20483,7 @@
         <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -20525,7 +20491,7 @@
         <v>865</v>
       </c>
       <c r="B15" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -20549,7 +20515,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -21680,7 +21646,7 @@
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -21870,7 +21836,7 @@
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -22769,7 +22735,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -23669,7 +23635,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -23932,7 +23898,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -23967,7 +23933,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>
@@ -24301,7 +24267,7 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
First draft Ontario ETL tool - lookup table, workspace, transformers
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robennet\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5044" uniqueCount="1483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="1485">
   <si>
     <t>default_key</t>
   </si>
@@ -4508,6 +4508,12 @@
   </si>
   <si>
     <t>Quebec Government and Municipalities</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">application/msaccess </t>
   </si>
 </sst>
 </file>
@@ -4646,8 +4652,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -4933,7 +4939,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -5001,7 +5007,7 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -5281,11 +5287,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -5628,7 +5634,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -5977,13 +5983,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F470"/>
+  <dimension ref="A1:F471"/>
   <sheetViews>
-    <sheetView topLeftCell="A286" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A338" sqref="A338"/>
+    <sheetView tabSelected="1" topLeftCell="A439" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B471" sqref="B471:D471"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -12663,6 +12669,20 @@
         <v>274</v>
       </c>
       <c r="D470" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>1484</v>
+      </c>
+      <c r="B471" s="27" t="s">
+        <v>783</v>
+      </c>
+      <c r="C471" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D471" s="27" t="s">
         <v>275</v>
       </c>
     </row>
@@ -12683,7 +12703,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -13059,7 +13079,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -13103,7 +13123,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -13278,7 +13298,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -13990,7 +14010,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -14208,7 +14228,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -14291,7 +14311,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -15268,7 +15288,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -15443,7 +15463,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
@@ -15947,7 +15967,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -16010,7 +16030,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -16269,7 +16289,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -16581,7 +16601,7 @@
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -17902,7 +17922,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
@@ -18185,7 +18205,7 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
@@ -18532,7 +18552,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -18697,7 +18717,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -18816,7 +18836,7 @@
       <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -19715,7 +19735,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
@@ -19882,13 +19902,13 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:D33"/>
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -20356,6 +20376,20 @@
       </c>
       <c r="D33" s="27" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1483</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -20372,7 +20406,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -20515,7 +20549,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -21646,7 +21680,7 @@
       <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -21836,7 +21870,7 @@
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -22735,7 +22769,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -23635,7 +23669,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -23898,7 +23932,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -23933,7 +23967,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>
@@ -24267,7 +24301,7 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/federal-geospatial-platform/fgp-metadata-proxy"
This reverts commit 4f3977e63a9b696cd94d6cde8c1a2e0de7378316, reversing
changes made to 8a0ba24e2a442ccc79e6789faf4b3dfbbc54fd99.
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -3729,6 +3729,14 @@
     <t>abstract_other_lang_warning_en</t>
   </si>
   <si>
+    <t xml:space="preserve">
+** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate). Pour signaler toute anomalie, veuillez communiquer avec nous à nrcan.fgp-pgf.rncan@canada.ca **</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+**This third party metadata element was translated using an automated translation tool (Amazon Translate). To report any discrepancies, please contact us at nrcan.fgp-pgf.rncan@canada.ca.**</t>
+  </si>
+  <si>
     <t>Gouvernement et municipalités du Québec</t>
   </si>
   <si>
@@ -4135,6 +4143,9 @@
   </si>
   <si>
     <t>RAD Boundaries (ZIP)</t>
+  </si>
+  <si>
+    <t>** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate). Pour signaler toute anomalie, veuillez communiquer avec nous à nrcan.fgp-pgf.rncan@canada.ca **</t>
   </si>
   <si>
     <t>lio@ontario.ca</t>
@@ -5086,23 +5097,12 @@
   </si>
   <si>
     <t>CC0-1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate).**</t>
-  </si>
-  <si>
-    <t>** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate).**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-**This third party metadata element was translated using an automated translation tool (Amazon Translate).**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5238,8 +5238,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -5525,7 +5525,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -5589,11 +5589,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -5615,20 +5615,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>1676</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>1359</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5641,10 +5641,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>1360</v>
+        <v>1363</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>1361</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5665,7 +5665,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>1362</v>
+        <v>1365</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>518</v>
@@ -5700,12 +5700,12 @@
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>1363</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>1364</v>
+        <v>1367</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>168</v>
@@ -5732,7 +5732,7 @@
         <v>728</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>1365</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5740,7 +5740,7 @@
         <v>732</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>1366</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5756,7 +5756,7 @@
         <v>725</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>1367</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5769,7 +5769,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>1368</v>
+        <v>1371</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>25</v>
@@ -5780,7 +5780,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>1369</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5788,7 +5788,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>1370</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5804,7 +5804,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>1371</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5812,7 +5812,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>1372</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5873,11 +5873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -5907,12 +5907,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>1677</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6040,7 +6040,7 @@
         <v>790</v>
       </c>
       <c r="B20" t="s">
-        <v>1479</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6048,7 +6048,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6109,63 +6109,63 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="B31" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B33" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="B34" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="B35" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="B36" t="s">
         <v>518</v>
@@ -6173,34 +6173,34 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="B37" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="B38" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="B39" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="B40" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
   </sheetData>
@@ -6220,7 +6220,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -6575,7 +6575,7 @@
       <selection activeCell="B471" sqref="B471:D471"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -13246,7 +13246,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1358</v>
+        <v>1360</v>
       </c>
       <c r="B470" t="s">
         <v>324</v>
@@ -13260,7 +13260,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>1481</v>
+        <v>1484</v>
       </c>
       <c r="B471" s="27" t="s">
         <v>783</v>
@@ -13289,17 +13289,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -13424,7 +13424,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="B17" t="s">
         <v>783</v>
@@ -13665,7 +13665,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -13709,7 +13709,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -13884,7 +13884,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -14596,7 +14596,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -14810,11 +14810,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -14886,7 +14886,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1674</v>
+        <v>1677</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>886</v>
@@ -14905,7 +14905,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -15882,7 +15882,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -16057,7 +16057,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
@@ -16066,101 +16066,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1350</v>
+        <v>1352</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>1349</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1348</v>
+        <v>1350</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1347</v>
+        <v>1349</v>
       </c>
       <c r="B3" t="s">
         <v>791</v>
       </c>
       <c r="C3" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1346</v>
+        <v>1348</v>
       </c>
       <c r="B4" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="C4" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="B5" t="s">
-        <v>1345</v>
+        <v>1347</v>
       </c>
       <c r="C5" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="B6" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="C6" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1344</v>
+        <v>1346</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1343</v>
+        <v>1345</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1342</v>
+        <v>1344</v>
       </c>
       <c r="B9" t="s">
-        <v>1342</v>
+        <v>1344</v>
       </c>
       <c r="C9" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -16171,7 +16171,7 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -16182,7 +16182,7 @@
         <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -16193,7 +16193,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>1341</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -16204,7 +16204,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -16215,29 +16215,29 @@
         <v>794</v>
       </c>
       <c r="C14" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1340</v>
+        <v>1342</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="B16" t="s">
-        <v>1338</v>
+        <v>1340</v>
       </c>
       <c r="C16" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -16248,95 +16248,95 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1337</v>
+        <v>1339</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="C19" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="C20" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="B21" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="C21" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="B22" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="C22" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1336</v>
+        <v>1338</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="C24" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="B25" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="C25" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -16347,7 +16347,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -16358,194 +16358,194 @@
         <v>790</v>
       </c>
       <c r="C27" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="B28" t="s">
-        <v>1335</v>
+        <v>1337</v>
       </c>
       <c r="C28" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="B29" t="s">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="C29" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="B30" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
       <c r="C30" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="C31" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="B32" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
       <c r="C32" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="B33" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="C33" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="B34" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="C34" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="B35" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="C35" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="B36" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="C36" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="B37" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
       <c r="C37" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="B38" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="C38" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1330</v>
+        <v>1332</v>
       </c>
       <c r="B40" t="s">
         <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="B41" t="s">
         <v>856</v>
       </c>
       <c r="C41" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1328</v>
+        <v>1330</v>
       </c>
       <c r="B42" t="s">
-        <v>1327</v>
+        <v>1329</v>
       </c>
       <c r="C42" t="s">
-        <v>1324</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C43" t="s">
         <v>1326</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1325</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="B44" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="C44" t="s">
-        <v>1323</v>
+        <v>1325</v>
       </c>
     </row>
   </sheetData>
@@ -16561,46 +16561,46 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1357</v>
+        <v>1359</v>
       </c>
       <c r="B2" t="s">
-        <v>1356</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1355</v>
+        <v>1357</v>
       </c>
       <c r="B3" t="s">
-        <v>1354</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1353</v>
+        <v>1355</v>
       </c>
       <c r="B4" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1352</v>
+        <v>1354</v>
       </c>
       <c r="B5" t="s">
-        <v>1351</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -16608,7 +16608,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
     </row>
   </sheetData>
@@ -16624,7 +16624,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -16883,7 +16883,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -16893,282 +16893,282 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>1373</v>
+        <v>1376</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>1339</v>
+        <v>1341</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>1374</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>1375</v>
+        <v>1378</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>1375</v>
+        <v>1378</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>1376</v>
+        <v>1379</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1376</v>
+        <v>1379</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>1377</v>
+        <v>1380</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1377</v>
+        <v>1380</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>1378</v>
+        <v>1381</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1378</v>
+        <v>1381</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>1379</v>
+        <v>1382</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>1379</v>
+        <v>1382</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>1380</v>
+        <v>1383</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>1380</v>
+        <v>1383</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>1381</v>
+        <v>1384</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>1381</v>
+        <v>1384</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>1382</v>
+        <v>1385</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1382</v>
+        <v>1385</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>1383</v>
+        <v>1386</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>1384</v>
+        <v>1387</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>1384</v>
+        <v>1387</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>1384</v>
+        <v>1387</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>1385</v>
+        <v>1388</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1385</v>
+        <v>1388</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>1386</v>
+        <v>1389</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>1386</v>
+        <v>1389</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>1387</v>
+        <v>1390</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>1388</v>
+        <v>1391</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>1389</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>1386</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>1390</v>
+        <v>1393</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>1391</v>
+        <v>1394</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>1391</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>1393</v>
+        <v>1396</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>1376</v>
+        <v>1379</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>1376</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>1394</v>
+        <v>1397</v>
       </c>
       <c r="B18" s="26" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C18" s="25" t="s">
         <v>1395</v>
       </c>
-      <c r="C18" s="25" t="s">
-        <v>1392</v>
-      </c>
       <c r="D18" s="26" t="s">
-        <v>1395</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>1396</v>
+        <v>1399</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>1381</v>
+        <v>1384</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>1381</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>1397</v>
+        <v>1400</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>1382</v>
+        <v>1385</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>1382</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>1398</v>
+        <v>1401</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>1384</v>
+        <v>1387</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>1384</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>1399</v>
+        <v>1402</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>1400</v>
+        <v>1403</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>1400</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>1401</v>
+        <v>1404</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>1385</v>
+        <v>1388</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>1385</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>1402</v>
+        <v>1405</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>1402</v>
+        <v>1405</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>1392</v>
+        <v>1395</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>1402</v>
+        <v>1405</v>
       </c>
     </row>
   </sheetData>
@@ -17195,7 +17195,7 @@
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -17218,7 +17218,7 @@
         <v>976</v>
       </c>
       <c r="E1" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -17226,16 +17226,16 @@
         <v>883</v>
       </c>
       <c r="B2" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="C2" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="D2" t="s">
         <v>889</v>
       </c>
       <c r="E2" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -17252,7 +17252,7 @@
         <v>889</v>
       </c>
       <c r="E3" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -17269,7 +17269,7 @@
         <v>889</v>
       </c>
       <c r="E4" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -17286,7 +17286,7 @@
         <v>889</v>
       </c>
       <c r="E5" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -17303,7 +17303,7 @@
         <v>889</v>
       </c>
       <c r="E6" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -17320,7 +17320,7 @@
         <v>889</v>
       </c>
       <c r="E7" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -17337,7 +17337,7 @@
         <v>889</v>
       </c>
       <c r="E8" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -17354,7 +17354,7 @@
         <v>889</v>
       </c>
       <c r="E9" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -17371,7 +17371,7 @@
         <v>889</v>
       </c>
       <c r="E10" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -17388,7 +17388,7 @@
         <v>889</v>
       </c>
       <c r="E11" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -17405,7 +17405,7 @@
         <v>889</v>
       </c>
       <c r="E12" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -17422,7 +17422,7 @@
         <v>889</v>
       </c>
       <c r="E13" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -17439,7 +17439,7 @@
         <v>889</v>
       </c>
       <c r="E14" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -17456,7 +17456,7 @@
         <v>889</v>
       </c>
       <c r="E15" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -17473,7 +17473,7 @@
         <v>889</v>
       </c>
       <c r="E16" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -17490,7 +17490,7 @@
         <v>889</v>
       </c>
       <c r="E17" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -17507,7 +17507,7 @@
         <v>889</v>
       </c>
       <c r="E18" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -17524,7 +17524,7 @@
         <v>889</v>
       </c>
       <c r="E19" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -17541,7 +17541,7 @@
         <v>889</v>
       </c>
       <c r="E20" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -17558,7 +17558,7 @@
         <v>889</v>
       </c>
       <c r="E21" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -17575,7 +17575,7 @@
         <v>889</v>
       </c>
       <c r="E22" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -17592,7 +17592,7 @@
         <v>889</v>
       </c>
       <c r="E23" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -17609,7 +17609,7 @@
         <v>889</v>
       </c>
       <c r="E24" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -17626,7 +17626,7 @@
         <v>889</v>
       </c>
       <c r="E25" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -17643,7 +17643,7 @@
         <v>889</v>
       </c>
       <c r="E26" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -17660,7 +17660,7 @@
         <v>889</v>
       </c>
       <c r="E27" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -17677,7 +17677,7 @@
         <v>889</v>
       </c>
       <c r="E28" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -17694,7 +17694,7 @@
         <v>889</v>
       </c>
       <c r="E29" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -17711,7 +17711,7 @@
         <v>889</v>
       </c>
       <c r="E30" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -17728,7 +17728,7 @@
         <v>889</v>
       </c>
       <c r="E31" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -17736,16 +17736,16 @@
         <v>936</v>
       </c>
       <c r="B32" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="C32" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="D32" t="s">
         <v>889</v>
       </c>
       <c r="E32" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -17762,7 +17762,7 @@
         <v>889</v>
       </c>
       <c r="E33" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -17770,7 +17770,7 @@
         <v>974</v>
       </c>
       <c r="B34" t="s">
-        <v>1259</v>
+        <v>1261</v>
       </c>
       <c r="C34" t="s">
         <v>937</v>
@@ -17779,7 +17779,7 @@
         <v>889</v>
       </c>
       <c r="E34" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -17796,7 +17796,7 @@
         <v>889</v>
       </c>
       <c r="E35" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -17813,7 +17813,7 @@
         <v>889</v>
       </c>
       <c r="E36" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -17830,7 +17830,7 @@
         <v>889</v>
       </c>
       <c r="E37" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -17847,7 +17847,7 @@
         <v>889</v>
       </c>
       <c r="E38" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -17864,7 +17864,7 @@
         <v>889</v>
       </c>
       <c r="E39" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -17881,7 +17881,7 @@
         <v>889</v>
       </c>
       <c r="E40" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -17892,13 +17892,13 @@
         <v>887</v>
       </c>
       <c r="C41" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="D41" t="s">
         <v>889</v>
       </c>
       <c r="E41" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -17906,16 +17906,16 @@
         <v>890</v>
       </c>
       <c r="B42" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
       <c r="D42" t="s">
         <v>889</v>
       </c>
       <c r="E42" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -17923,16 +17923,16 @@
         <v>891</v>
       </c>
       <c r="B43" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="C43" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="D43" t="s">
         <v>889</v>
       </c>
       <c r="E43" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -17949,7 +17949,7 @@
         <v>886</v>
       </c>
       <c r="E44" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -17966,7 +17966,7 @@
         <v>886</v>
       </c>
       <c r="E45" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -17974,16 +17974,16 @@
         <v>894</v>
       </c>
       <c r="B46" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
       <c r="C46" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="D46" t="s">
         <v>889</v>
       </c>
       <c r="E46" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -17994,13 +17994,13 @@
         <v>898</v>
       </c>
       <c r="C47" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="D47" t="s">
         <v>889</v>
       </c>
       <c r="E47" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -18008,16 +18008,16 @@
         <v>900</v>
       </c>
       <c r="B48" t="s">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="C48" t="s">
-        <v>1256</v>
+        <v>1258</v>
       </c>
       <c r="D48" t="s">
         <v>889</v>
       </c>
       <c r="E48" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -18034,7 +18034,7 @@
         <v>886</v>
       </c>
       <c r="E49" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -18045,13 +18045,13 @@
         <v>902</v>
       </c>
       <c r="C50" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="D50" t="s">
         <v>889</v>
       </c>
       <c r="E50" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -18068,7 +18068,7 @@
         <v>886</v>
       </c>
       <c r="E51" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -18079,13 +18079,13 @@
         <v>908</v>
       </c>
       <c r="C52" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="D52" t="s">
         <v>889</v>
       </c>
       <c r="E52" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -18093,16 +18093,16 @@
         <v>909</v>
       </c>
       <c r="B53" t="s">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="C53" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="D53" t="s">
         <v>889</v>
       </c>
       <c r="E53" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -18113,13 +18113,13 @@
         <v>928</v>
       </c>
       <c r="C54" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="D54" t="s">
         <v>889</v>
       </c>
       <c r="E54" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -18136,7 +18136,7 @@
         <v>886</v>
       </c>
       <c r="E55" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -18147,13 +18147,13 @@
         <v>930</v>
       </c>
       <c r="C56" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="D56" t="s">
         <v>889</v>
       </c>
       <c r="E56" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -18164,13 +18164,13 @@
         <v>931</v>
       </c>
       <c r="C57" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="D57" t="s">
         <v>889</v>
       </c>
       <c r="E57" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -18178,16 +18178,16 @@
         <v>941</v>
       </c>
       <c r="B58" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="C58" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="D58" t="s">
         <v>889</v>
       </c>
       <c r="E58" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -18195,16 +18195,16 @@
         <v>942</v>
       </c>
       <c r="B59" t="s">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="C59" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="D59" t="s">
         <v>889</v>
       </c>
       <c r="E59" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -18212,16 +18212,16 @@
         <v>943</v>
       </c>
       <c r="B60" t="s">
-        <v>1264</v>
+        <v>1266</v>
       </c>
       <c r="C60" t="s">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="D60" t="s">
         <v>889</v>
       </c>
       <c r="E60" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -18229,16 +18229,16 @@
         <v>944</v>
       </c>
       <c r="B61" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="C61" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="D61" t="s">
         <v>889</v>
       </c>
       <c r="E61" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -18249,13 +18249,13 @@
         <v>945</v>
       </c>
       <c r="C62" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="D62" t="s">
         <v>889</v>
       </c>
       <c r="E62" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -18272,7 +18272,7 @@
         <v>886</v>
       </c>
       <c r="E63" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -18283,13 +18283,13 @@
         <v>947</v>
       </c>
       <c r="C64" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="D64" t="s">
         <v>889</v>
       </c>
       <c r="E64" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -18297,16 +18297,16 @@
         <v>949</v>
       </c>
       <c r="B65" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="C65" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="D65" t="s">
         <v>889</v>
       </c>
       <c r="E65" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -18314,16 +18314,16 @@
         <v>950</v>
       </c>
       <c r="B66" t="s">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="C66" t="s">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="D66" t="s">
         <v>889</v>
       </c>
       <c r="E66" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -18331,16 +18331,16 @@
         <v>975</v>
       </c>
       <c r="B67" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="D67" t="s">
         <v>889</v>
       </c>
       <c r="E67" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -18357,7 +18357,7 @@
         <v>889</v>
       </c>
       <c r="E68" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -18374,7 +18374,7 @@
         <v>889</v>
       </c>
       <c r="E69" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -18391,7 +18391,7 @@
         <v>889</v>
       </c>
       <c r="E70" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -18408,7 +18408,7 @@
         <v>889</v>
       </c>
       <c r="E71" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -18425,7 +18425,7 @@
         <v>889</v>
       </c>
       <c r="E72" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -18442,7 +18442,7 @@
         <v>889</v>
       </c>
       <c r="E73" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -18459,7 +18459,7 @@
         <v>889</v>
       </c>
       <c r="E74" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -18476,7 +18476,7 @@
         <v>889</v>
       </c>
       <c r="E75" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -18493,7 +18493,7 @@
         <v>889</v>
       </c>
       <c r="E76" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
     </row>
   </sheetData>
@@ -18516,7 +18516,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
@@ -18524,7 +18524,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>1373</v>
+        <v>1376</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>8</v>
@@ -18532,7 +18532,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>1403</v>
+        <v>1406</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>567</v>
@@ -18540,7 +18540,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>1404</v>
+        <v>1407</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>567</v>
@@ -18548,7 +18548,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>1405</v>
+        <v>1408</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>567</v>
@@ -18556,7 +18556,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>1406</v>
+        <v>1409</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>567</v>
@@ -18564,7 +18564,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>1407</v>
+        <v>1410</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>567</v>
@@ -18572,7 +18572,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1408</v>
+        <v>1411</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>567</v>
@@ -18580,7 +18580,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>1409</v>
+        <v>1412</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>567</v>
@@ -18588,7 +18588,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1410</v>
+        <v>1413</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>567</v>
@@ -18596,7 +18596,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>1411</v>
+        <v>1414</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>567</v>
@@ -18604,7 +18604,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>1412</v>
+        <v>1415</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>567</v>
@@ -18612,7 +18612,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>1413</v>
+        <v>1416</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>567</v>
@@ -18620,7 +18620,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>1414</v>
+        <v>1417</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>567</v>
@@ -18628,7 +18628,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>1415</v>
+        <v>1418</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>567</v>
@@ -18636,7 +18636,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>1416</v>
+        <v>1419</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>567</v>
@@ -18644,7 +18644,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>1417</v>
+        <v>1420</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>567</v>
@@ -18652,7 +18652,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>1418</v>
+        <v>1421</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>567</v>
@@ -18660,7 +18660,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>1419</v>
+        <v>1422</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>567</v>
@@ -18668,7 +18668,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>1420</v>
+        <v>1423</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>567</v>
@@ -18676,7 +18676,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>1421</v>
+        <v>1424</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>567</v>
@@ -18684,7 +18684,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>1422</v>
+        <v>1425</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>567</v>
@@ -18692,7 +18692,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1423</v>
+        <v>1426</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>567</v>
@@ -18700,7 +18700,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>1424</v>
+        <v>1427</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>567</v>
@@ -18708,7 +18708,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>1425</v>
+        <v>1428</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>567</v>
@@ -18716,7 +18716,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>1426</v>
+        <v>1429</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>567</v>
@@ -18724,7 +18724,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>1427</v>
+        <v>1430</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>567</v>
@@ -18732,7 +18732,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>1428</v>
+        <v>1431</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>567</v>
@@ -18740,7 +18740,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>1429</v>
+        <v>1432</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>567</v>
@@ -18748,7 +18748,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>1430</v>
+        <v>1433</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>567</v>
@@ -18756,7 +18756,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>1431</v>
+        <v>1434</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>567</v>
@@ -18764,7 +18764,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>1432</v>
+        <v>1435</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -18772,7 +18772,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>1433</v>
+        <v>1436</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -18780,7 +18780,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>1434</v>
+        <v>1437</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>567</v>
@@ -18799,7 +18799,7 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
@@ -18815,7 +18815,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1439</v>
+        <v>1442</v>
       </c>
       <c r="B2" t="s">
         <v>564</v>
@@ -18823,7 +18823,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1440</v>
+        <v>1443</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>564</v>
@@ -18831,7 +18831,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1441</v>
+        <v>1444</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>564</v>
@@ -18839,7 +18839,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1442</v>
+        <v>1445</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>564</v>
@@ -18847,7 +18847,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1443</v>
+        <v>1446</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>564</v>
@@ -18855,7 +18855,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1444</v>
+        <v>1447</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>564</v>
@@ -18863,7 +18863,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1445</v>
+        <v>1448</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -18871,7 +18871,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1446</v>
+        <v>1449</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>9</v>
@@ -18879,7 +18879,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1447</v>
+        <v>1450</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>9</v>
@@ -18887,7 +18887,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1448</v>
+        <v>1451</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>9</v>
@@ -18895,7 +18895,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1449</v>
+        <v>1452</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>9</v>
@@ -18903,7 +18903,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1450</v>
+        <v>1453</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>9</v>
@@ -18911,7 +18911,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1451</v>
+        <v>1454</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>564</v>
@@ -18919,7 +18919,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1452</v>
+        <v>1455</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>9</v>
@@ -18927,7 +18927,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1453</v>
+        <v>1456</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>564</v>
@@ -18935,7 +18935,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1454</v>
+        <v>1457</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>9</v>
@@ -18943,7 +18943,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1455</v>
+        <v>1458</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>9</v>
@@ -18951,7 +18951,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1456</v>
+        <v>1459</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>9</v>
@@ -18959,7 +18959,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1457</v>
+        <v>1460</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>9</v>
@@ -18967,7 +18967,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1458</v>
+        <v>1461</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>9</v>
@@ -18975,7 +18975,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1459</v>
+        <v>1462</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>9</v>
@@ -18983,7 +18983,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1460</v>
+        <v>1463</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>564</v>
@@ -18991,7 +18991,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1461</v>
+        <v>1464</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>564</v>
@@ -18999,7 +18999,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1462</v>
+        <v>1465</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>9</v>
@@ -19007,7 +19007,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1463</v>
+        <v>1466</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>9</v>
@@ -19015,7 +19015,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1464</v>
+        <v>1467</v>
       </c>
       <c r="B27" t="s">
         <v>567</v>
@@ -19023,7 +19023,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1465</v>
+        <v>1468</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>564</v>
@@ -19031,7 +19031,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1466</v>
+        <v>1469</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>564</v>
@@ -19039,7 +19039,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1467</v>
+        <v>1470</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>9</v>
@@ -19047,7 +19047,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1468</v>
+        <v>1471</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -19055,7 +19055,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1469</v>
+        <v>1472</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -19063,7 +19063,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1470</v>
+        <v>1473</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>9</v>
@@ -19071,7 +19071,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1471</v>
+        <v>1474</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>9</v>
@@ -19079,7 +19079,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1472</v>
+        <v>1475</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>9</v>
@@ -19087,7 +19087,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1473</v>
+        <v>1476</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>9</v>
@@ -19095,7 +19095,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1474</v>
+        <v>1477</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>9</v>
@@ -19103,7 +19103,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1475</v>
+        <v>1478</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>9</v>
@@ -19111,7 +19111,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1476</v>
+        <v>1479</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>9</v>
@@ -19119,7 +19119,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1477</v>
+        <v>1480</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>9</v>
@@ -19127,7 +19127,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1478</v>
+        <v>1481</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>564</v>
@@ -19146,7 +19146,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -19311,7 +19311,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -19430,7 +19430,7 @@
       <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -20329,7 +20329,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
@@ -20337,13 +20337,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1322</v>
+        <v>1324</v>
       </c>
       <c r="C1" t="s">
-        <v>1321</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -20354,139 +20354,139 @@
         <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1320</v>
+        <v>1322</v>
       </c>
       <c r="B3" t="s">
         <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>1319</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1318</v>
+        <v>1320</v>
       </c>
       <c r="B4" t="s">
         <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1317</v>
+        <v>1319</v>
       </c>
       <c r="B5" t="s">
         <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="B6" t="s">
         <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>1315</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1314</v>
+        <v>1316</v>
       </c>
       <c r="B7" t="s">
         <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>1313</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
       <c r="B8" t="s">
         <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="B9" t="s">
         <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>1310</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
       <c r="B10" t="s">
         <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="B11" t="s">
         <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="B12" t="s">
         <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="B13" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="C13" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="B14" t="s">
         <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
     </row>
   </sheetData>
@@ -20502,7 +20502,7 @@
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -20904,7 +20904,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>1435</v>
+        <v>1438</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>226</v>
@@ -20932,7 +20932,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>1436</v>
+        <v>1439</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>221</v>
@@ -20946,7 +20946,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1437</v>
+        <v>1440</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>226</v>
@@ -20960,7 +20960,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1438</v>
+        <v>1441</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>25</v>
@@ -20974,7 +20974,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1480</v>
+        <v>1483</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>232</v>
@@ -21000,14 +21000,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="B1" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -21023,7 +21023,7 @@
         <v>860</v>
       </c>
       <c r="B3" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -21031,7 +21031,7 @@
         <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -21039,7 +21039,7 @@
         <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -21055,7 +21055,7 @@
         <v>861</v>
       </c>
       <c r="B7" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -21063,7 +21063,7 @@
         <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -21079,7 +21079,7 @@
         <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -21087,7 +21087,7 @@
         <v>863</v>
       </c>
       <c r="B11" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -21095,7 +21095,7 @@
         <v>864</v>
       </c>
       <c r="B12" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -21103,7 +21103,7 @@
         <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -21111,7 +21111,7 @@
         <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>1291</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -21119,7 +21119,7 @@
         <v>865</v>
       </c>
       <c r="B15" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -21143,7 +21143,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -22274,7 +22274,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -22450,7 +22450,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1673</v>
+        <v>1676</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -22472,7 +22472,7 @@
       <selection activeCell="B50" sqref="B2:B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="54.140625" style="27" customWidth="1"/>
     <col min="3" max="3" width="180.5703125" style="31" customWidth="1"/>
@@ -22484,10 +22484,10 @@
         <v>37</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>1374</v>
+        <v>1377</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -22495,7 +22495,7 @@
         <v>986</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>1522</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -22503,23 +22503,23 @@
         <v>985</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1482</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>1483</v>
+        <v>1486</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>1484</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>1485</v>
+        <v>1488</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>1486</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -22527,199 +22527,199 @@
         <v>988</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>1487</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1488</v>
+        <v>1491</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>1489</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>1500</v>
+        <v>1503</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>1501</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1506</v>
+        <v>1509</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>1492</v>
+        <v>1495</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>1493</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>1498</v>
+        <v>1501</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>1499</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>1490</v>
+        <v>1493</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>1491</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>1508</v>
+        <v>1511</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>1509</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>1503</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>1521</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>1496</v>
+        <v>1499</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>1497</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>1519</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>1517</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>1511</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>1515</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>1512</v>
+        <v>1515</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1494</v>
+        <v>1497</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>1495</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>1504</v>
+        <v>1507</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>1505</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>1523</v>
+        <v>1526</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>1524</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>1546</v>
+        <v>1549</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>1547</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>1534</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>1531</v>
+        <v>1534</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>1532</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>1550</v>
+        <v>1553</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>1551</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>1558</v>
+        <v>1561</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>1559</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>1542</v>
+        <v>1545</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>1543</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -22727,95 +22727,95 @@
         <v>1011</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>1529</v>
+        <v>1532</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>1530</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>1548</v>
+        <v>1551</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>1549</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>1544</v>
+        <v>1547</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>1545</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>1527</v>
+        <v>1530</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>1535</v>
+        <v>1538</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>1536</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>1557</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>1554</v>
+        <v>1557</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>1552</v>
+        <v>1555</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>1553</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>1539</v>
+        <v>1542</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>1540</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>1537</v>
+        <v>1540</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>1538</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -22823,335 +22823,335 @@
         <v>987</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>1560</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>1561</v>
+        <v>1564</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>1562</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
-        <v>1563</v>
+        <v>1566</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>1564</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
-        <v>1567</v>
+        <v>1570</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>1568</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
-        <v>1569</v>
+        <v>1572</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>1570</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
-        <v>1565</v>
+        <v>1568</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>1566</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>1573</v>
+        <v>1576</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>1574</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>1571</v>
+        <v>1574</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>1572</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="27" t="s">
-        <v>1671</v>
+        <v>1674</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>1672</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
-        <v>1575</v>
+        <v>1578</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>1576</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
-        <v>1577</v>
+        <v>1580</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>1578</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="27" t="s">
-        <v>1670</v>
+        <v>1673</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>1578</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
-        <v>1579</v>
+        <v>1582</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>1580</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
-        <v>1603</v>
+        <v>1606</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>1604</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
-        <v>1593</v>
+        <v>1596</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>1594</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
-        <v>1599</v>
+        <v>1602</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>1600</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
-        <v>1595</v>
+        <v>1598</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>1596</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
-        <v>1587</v>
+        <v>1590</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>1588</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>1591</v>
+        <v>1594</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>1592</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
-        <v>1605</v>
+        <v>1608</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>1606</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
-        <v>1589</v>
+        <v>1592</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>1590</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
-        <v>1581</v>
+        <v>1584</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>1582</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="27" t="s">
-        <v>1601</v>
+        <v>1604</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>1602</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
-        <v>1597</v>
+        <v>1600</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>1598</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
-        <v>1585</v>
+        <v>1588</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>1586</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
-        <v>1583</v>
+        <v>1586</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>1584</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
-        <v>1620</v>
+        <v>1623</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>1621</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
-        <v>1630</v>
+        <v>1633</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>1631</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
-        <v>1614</v>
+        <v>1617</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>1615</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
-        <v>1640</v>
+        <v>1643</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>1641</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
-        <v>1646</v>
+        <v>1649</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>1647</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
-        <v>1642</v>
+        <v>1645</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>1643</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
-        <v>1634</v>
+        <v>1637</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>1635</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
-        <v>1608</v>
+        <v>1611</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>1609</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
-        <v>1650</v>
+        <v>1653</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>1651</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
-        <v>1648</v>
+        <v>1651</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>1649</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
-        <v>1656</v>
+        <v>1659</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>1657</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
-        <v>1658</v>
+        <v>1661</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>1659</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
-        <v>1626</v>
+        <v>1629</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>1627</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
-        <v>1618</v>
+        <v>1621</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>1619</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>1636</v>
+        <v>1639</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>1637</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
-        <v>1622</v>
+        <v>1625</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>1623</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -23159,127 +23159,127 @@
         <v>984</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>1607</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
-        <v>1628</v>
+        <v>1631</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>1629</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>1652</v>
+        <v>1655</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>1653</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
-        <v>1610</v>
+        <v>1613</v>
       </c>
       <c r="C88" s="31" t="s">
-        <v>1611</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
-        <v>1612</v>
+        <v>1615</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>1613</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
-        <v>1624</v>
+        <v>1627</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>1625</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
-        <v>1616</v>
+        <v>1619</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>1617</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="27" t="s">
-        <v>1654</v>
+        <v>1657</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>1655</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="27" t="s">
-        <v>1644</v>
+        <v>1647</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>1645</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
-        <v>1660</v>
+        <v>1663</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>1661</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
-        <v>1638</v>
+        <v>1641</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>1639</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="27" t="s">
-        <v>1632</v>
+        <v>1635</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>1633</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="27" t="s">
-        <v>1662</v>
+        <v>1665</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>1663</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="27" t="s">
-        <v>1668</v>
+        <v>1671</v>
       </c>
       <c r="C98" s="31" t="s">
-        <v>1669</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="27" t="s">
-        <v>1664</v>
+        <v>1667</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>1665</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="27" t="s">
-        <v>1666</v>
+        <v>1669</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>1667</v>
+        <v>1670</v>
       </c>
     </row>
   </sheetData>
@@ -23301,7 +23301,7 @@
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -24200,7 +24200,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -25100,7 +25100,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -25363,7 +25363,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -25394,14 +25394,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -25548,12 +25547,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>1675</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -25729,14 +25728,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -25875,12 +25873,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>1675</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/federal-geospatial-platform/fgp-metadata-proxy""
This reverts commit a90ddfcf11ccaab080bbb3bd3f9a5f999e3bdd4b.
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" firstSheet="17" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -3729,14 +3729,6 @@
     <t>abstract_other_lang_warning_en</t>
   </si>
   <si>
-    <t xml:space="preserve">
-** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate). Pour signaler toute anomalie, veuillez communiquer avec nous à nrcan.fgp-pgf.rncan@canada.ca **</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-**This third party metadata element was translated using an automated translation tool (Amazon Translate). To report any discrepancies, please contact us at nrcan.fgp-pgf.rncan@canada.ca.**</t>
-  </si>
-  <si>
     <t>Gouvernement et municipalités du Québec</t>
   </si>
   <si>
@@ -4143,9 +4135,6 @@
   </si>
   <si>
     <t>RAD Boundaries (ZIP)</t>
-  </si>
-  <si>
-    <t>** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate). Pour signaler toute anomalie, veuillez communiquer avec nous à nrcan.fgp-pgf.rncan@canada.ca **</t>
   </si>
   <si>
     <t>lio@ontario.ca</t>
@@ -5097,12 +5086,23 @@
   </si>
   <si>
     <t>CC0-1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate).**</t>
+  </si>
+  <si>
+    <t>** Cet élément de métadonnées provenant d’une tierce partie a été traduit à l'aide d'un outil de traduction automatisée (Amazon Translate).**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+**This third party metadata element was translated using an automated translation tool (Amazon Translate).**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5238,8 +5238,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -5525,7 +5525,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -5589,11 +5589,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -5615,20 +5615,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>1361</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5641,10 +5641,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -5665,7 +5665,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>518</v>
@@ -5700,12 +5700,12 @@
         <v>6</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>168</v>
@@ -5732,7 +5732,7 @@
         <v>728</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5740,7 +5740,7 @@
         <v>732</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5756,7 +5756,7 @@
         <v>725</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5769,7 +5769,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>25</v>
@@ -5780,7 +5780,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5788,7 +5788,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5804,7 +5804,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5812,7 +5812,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5873,11 +5873,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -5907,12 +5907,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>1224</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6040,7 +6040,7 @@
         <v>790</v>
       </c>
       <c r="B20" t="s">
-        <v>1482</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6048,7 +6048,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -6109,63 +6109,63 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B31" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B33" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B34" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B35" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B36" t="s">
         <v>518</v>
@@ -6173,34 +6173,34 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B37" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B38" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B39" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B40" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
   </sheetData>
@@ -6220,7 +6220,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -6575,7 +6575,7 @@
       <selection activeCell="B471" sqref="B471:D471"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -13246,7 +13246,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B470" t="s">
         <v>324</v>
@@ -13260,7 +13260,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>1484</v>
+        <v>1481</v>
       </c>
       <c r="B471" s="27" t="s">
         <v>783</v>
@@ -13289,17 +13289,17 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B1" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -13424,7 +13424,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="B17" t="s">
         <v>783</v>
@@ -13665,7 +13665,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -13709,7 +13709,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -13884,7 +13884,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -14596,7 +14596,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -14810,11 +14810,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -14886,7 +14886,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>886</v>
@@ -14905,7 +14905,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -15882,7 +15882,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -16057,7 +16057,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
@@ -16066,101 +16066,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="B1" t="s">
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B3" t="s">
         <v>791</v>
       </c>
       <c r="C3" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="B4" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C4" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="B5" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="C5" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="B6" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="C6" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="B8" t="s">
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="B9" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="C9" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -16171,7 +16171,7 @@
         <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -16182,7 +16182,7 @@
         <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -16193,7 +16193,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -16204,7 +16204,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -16215,29 +16215,29 @@
         <v>794</v>
       </c>
       <c r="C14" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B16" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="C16" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -16248,95 +16248,95 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="C19" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="C20" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B21" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="C21" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="B22" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="C22" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
       </c>
       <c r="C23" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="C24" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B25" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="C25" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -16347,7 +16347,7 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -16358,194 +16358,194 @@
         <v>790</v>
       </c>
       <c r="C27" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="B28" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="C28" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="B29" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C29" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B30" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="C30" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="C31" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B32" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="C32" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B33" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="C33" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B34" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="C34" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="B35" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="C35" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="B36" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="C36" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C37" t="s">
         <v>1323</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1323</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1325</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B38" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="C38" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>
       <c r="C39" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B40" t="s">
         <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B41" t="s">
         <v>856</v>
       </c>
       <c r="C41" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B42" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="C42" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B43" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="C43" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B44" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="C44" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
     </row>
   </sheetData>
@@ -16561,46 +16561,46 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B1" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="B2" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="B3" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="B4" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="B5" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -16608,7 +16608,7 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
   </sheetData>
@@ -16624,7 +16624,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -16883,7 +16883,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -16893,282 +16893,282 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>1396</v>
+        <v>1393</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>1398</v>
+        <v>1395</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>1395</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>1398</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>1399</v>
+        <v>1396</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
-        <v>1400</v>
+        <v>1397</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>1401</v>
+        <v>1398</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>1402</v>
+        <v>1399</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
     </row>
   </sheetData>
@@ -17195,7 +17195,7 @@
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -17218,7 +17218,7 @@
         <v>976</v>
       </c>
       <c r="E1" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -17226,16 +17226,16 @@
         <v>883</v>
       </c>
       <c r="B2" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="C2" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="D2" t="s">
         <v>889</v>
       </c>
       <c r="E2" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -17252,7 +17252,7 @@
         <v>889</v>
       </c>
       <c r="E3" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -17269,7 +17269,7 @@
         <v>889</v>
       </c>
       <c r="E4" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -17286,7 +17286,7 @@
         <v>889</v>
       </c>
       <c r="E5" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -17303,7 +17303,7 @@
         <v>889</v>
       </c>
       <c r="E6" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -17320,7 +17320,7 @@
         <v>889</v>
       </c>
       <c r="E7" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -17337,7 +17337,7 @@
         <v>889</v>
       </c>
       <c r="E8" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -17354,7 +17354,7 @@
         <v>889</v>
       </c>
       <c r="E9" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -17371,7 +17371,7 @@
         <v>889</v>
       </c>
       <c r="E10" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -17388,7 +17388,7 @@
         <v>889</v>
       </c>
       <c r="E11" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -17405,7 +17405,7 @@
         <v>889</v>
       </c>
       <c r="E12" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -17422,7 +17422,7 @@
         <v>889</v>
       </c>
       <c r="E13" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -17439,7 +17439,7 @@
         <v>889</v>
       </c>
       <c r="E14" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -17456,7 +17456,7 @@
         <v>889</v>
       </c>
       <c r="E15" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -17473,7 +17473,7 @@
         <v>889</v>
       </c>
       <c r="E16" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -17490,7 +17490,7 @@
         <v>889</v>
       </c>
       <c r="E17" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -17507,7 +17507,7 @@
         <v>889</v>
       </c>
       <c r="E18" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -17524,7 +17524,7 @@
         <v>889</v>
       </c>
       <c r="E19" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -17541,7 +17541,7 @@
         <v>889</v>
       </c>
       <c r="E20" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -17558,7 +17558,7 @@
         <v>889</v>
       </c>
       <c r="E21" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -17575,7 +17575,7 @@
         <v>889</v>
       </c>
       <c r="E22" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -17592,7 +17592,7 @@
         <v>889</v>
       </c>
       <c r="E23" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -17609,7 +17609,7 @@
         <v>889</v>
       </c>
       <c r="E24" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -17626,7 +17626,7 @@
         <v>889</v>
       </c>
       <c r="E25" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -17643,7 +17643,7 @@
         <v>889</v>
       </c>
       <c r="E26" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -17660,7 +17660,7 @@
         <v>889</v>
       </c>
       <c r="E27" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -17677,7 +17677,7 @@
         <v>889</v>
       </c>
       <c r="E28" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -17694,7 +17694,7 @@
         <v>889</v>
       </c>
       <c r="E29" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -17711,7 +17711,7 @@
         <v>889</v>
       </c>
       <c r="E30" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -17728,7 +17728,7 @@
         <v>889</v>
       </c>
       <c r="E31" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -17736,16 +17736,16 @@
         <v>936</v>
       </c>
       <c r="B32" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="C32" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="D32" t="s">
         <v>889</v>
       </c>
       <c r="E32" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -17762,7 +17762,7 @@
         <v>889</v>
       </c>
       <c r="E33" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -17770,7 +17770,7 @@
         <v>974</v>
       </c>
       <c r="B34" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="C34" t="s">
         <v>937</v>
@@ -17779,7 +17779,7 @@
         <v>889</v>
       </c>
       <c r="E34" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -17796,7 +17796,7 @@
         <v>889</v>
       </c>
       <c r="E35" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -17813,7 +17813,7 @@
         <v>889</v>
       </c>
       <c r="E36" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -17830,7 +17830,7 @@
         <v>889</v>
       </c>
       <c r="E37" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -17847,7 +17847,7 @@
         <v>889</v>
       </c>
       <c r="E38" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -17864,7 +17864,7 @@
         <v>889</v>
       </c>
       <c r="E39" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -17881,7 +17881,7 @@
         <v>889</v>
       </c>
       <c r="E40" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -17892,13 +17892,13 @@
         <v>887</v>
       </c>
       <c r="C41" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="D41" t="s">
         <v>889</v>
       </c>
       <c r="E41" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -17906,16 +17906,16 @@
         <v>890</v>
       </c>
       <c r="B42" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="D42" t="s">
         <v>889</v>
       </c>
       <c r="E42" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -17923,16 +17923,16 @@
         <v>891</v>
       </c>
       <c r="B43" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="C43" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="D43" t="s">
         <v>889</v>
       </c>
       <c r="E43" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -17949,7 +17949,7 @@
         <v>886</v>
       </c>
       <c r="E44" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -17966,7 +17966,7 @@
         <v>886</v>
       </c>
       <c r="E45" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -17974,16 +17974,16 @@
         <v>894</v>
       </c>
       <c r="B46" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="C46" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="D46" t="s">
         <v>889</v>
       </c>
       <c r="E46" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -17994,13 +17994,13 @@
         <v>898</v>
       </c>
       <c r="C47" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="D47" t="s">
         <v>889</v>
       </c>
       <c r="E47" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -18008,16 +18008,16 @@
         <v>900</v>
       </c>
       <c r="B48" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="C48" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="D48" t="s">
         <v>889</v>
       </c>
       <c r="E48" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -18034,7 +18034,7 @@
         <v>886</v>
       </c>
       <c r="E49" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -18045,13 +18045,13 @@
         <v>902</v>
       </c>
       <c r="C50" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="D50" t="s">
         <v>889</v>
       </c>
       <c r="E50" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -18068,7 +18068,7 @@
         <v>886</v>
       </c>
       <c r="E51" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -18079,13 +18079,13 @@
         <v>908</v>
       </c>
       <c r="C52" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="D52" t="s">
         <v>889</v>
       </c>
       <c r="E52" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -18093,16 +18093,16 @@
         <v>909</v>
       </c>
       <c r="B53" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="C53" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="D53" t="s">
         <v>889</v>
       </c>
       <c r="E53" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -18113,13 +18113,13 @@
         <v>928</v>
       </c>
       <c r="C54" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="D54" t="s">
         <v>889</v>
       </c>
       <c r="E54" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -18136,7 +18136,7 @@
         <v>886</v>
       </c>
       <c r="E55" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -18147,13 +18147,13 @@
         <v>930</v>
       </c>
       <c r="C56" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="D56" t="s">
         <v>889</v>
       </c>
       <c r="E56" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -18164,13 +18164,13 @@
         <v>931</v>
       </c>
       <c r="C57" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="D57" t="s">
         <v>889</v>
       </c>
       <c r="E57" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -18178,16 +18178,16 @@
         <v>941</v>
       </c>
       <c r="B58" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="C58" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="D58" t="s">
         <v>889</v>
       </c>
       <c r="E58" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -18195,16 +18195,16 @@
         <v>942</v>
       </c>
       <c r="B59" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="C59" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="D59" t="s">
         <v>889</v>
       </c>
       <c r="E59" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -18212,16 +18212,16 @@
         <v>943</v>
       </c>
       <c r="B60" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="C60" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="D60" t="s">
         <v>889</v>
       </c>
       <c r="E60" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -18229,16 +18229,16 @@
         <v>944</v>
       </c>
       <c r="B61" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="C61" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="D61" t="s">
         <v>889</v>
       </c>
       <c r="E61" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -18249,13 +18249,13 @@
         <v>945</v>
       </c>
       <c r="C62" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="D62" t="s">
         <v>889</v>
       </c>
       <c r="E62" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -18272,7 +18272,7 @@
         <v>886</v>
       </c>
       <c r="E63" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -18283,13 +18283,13 @@
         <v>947</v>
       </c>
       <c r="C64" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="D64" t="s">
         <v>889</v>
       </c>
       <c r="E64" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -18297,16 +18297,16 @@
         <v>949</v>
       </c>
       <c r="B65" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="C65" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="D65" t="s">
         <v>889</v>
       </c>
       <c r="E65" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -18314,16 +18314,16 @@
         <v>950</v>
       </c>
       <c r="B66" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="C66" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="D66" t="s">
         <v>889</v>
       </c>
       <c r="E66" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -18331,16 +18331,16 @@
         <v>975</v>
       </c>
       <c r="B67" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="D67" t="s">
         <v>889</v>
       </c>
       <c r="E67" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -18357,7 +18357,7 @@
         <v>889</v>
       </c>
       <c r="E68" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -18374,7 +18374,7 @@
         <v>889</v>
       </c>
       <c r="E69" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -18391,7 +18391,7 @@
         <v>889</v>
       </c>
       <c r="E70" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -18408,7 +18408,7 @@
         <v>889</v>
       </c>
       <c r="E71" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -18425,7 +18425,7 @@
         <v>889</v>
       </c>
       <c r="E72" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -18442,7 +18442,7 @@
         <v>889</v>
       </c>
       <c r="E73" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -18459,7 +18459,7 @@
         <v>889</v>
       </c>
       <c r="E74" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -18476,7 +18476,7 @@
         <v>889</v>
       </c>
       <c r="E75" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -18493,7 +18493,7 @@
         <v>889</v>
       </c>
       <c r="E76" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
   </sheetData>
@@ -18516,7 +18516,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
@@ -18524,7 +18524,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>8</v>
@@ -18532,7 +18532,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>1406</v>
+        <v>1403</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>567</v>
@@ -18540,7 +18540,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>1407</v>
+        <v>1404</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>567</v>
@@ -18548,7 +18548,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>567</v>
@@ -18556,7 +18556,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>567</v>
@@ -18564,7 +18564,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
-        <v>1410</v>
+        <v>1407</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>567</v>
@@ -18572,7 +18572,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1411</v>
+        <v>1408</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>567</v>
@@ -18580,7 +18580,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>1412</v>
+        <v>1409</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>567</v>
@@ -18588,7 +18588,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1413</v>
+        <v>1410</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>567</v>
@@ -18596,7 +18596,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>1414</v>
+        <v>1411</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>567</v>
@@ -18604,7 +18604,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>1415</v>
+        <v>1412</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>567</v>
@@ -18612,7 +18612,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>1416</v>
+        <v>1413</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>567</v>
@@ -18620,7 +18620,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>567</v>
@@ -18628,7 +18628,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>567</v>
@@ -18636,7 +18636,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>567</v>
@@ -18644,7 +18644,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>567</v>
@@ -18652,7 +18652,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>567</v>
@@ -18660,7 +18660,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>567</v>
@@ -18668,7 +18668,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>567</v>
@@ -18676,7 +18676,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>567</v>
@@ -18684,7 +18684,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>1425</v>
+        <v>1422</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>567</v>
@@ -18692,7 +18692,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1426</v>
+        <v>1423</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>567</v>
@@ -18700,7 +18700,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>567</v>
@@ -18708,7 +18708,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>567</v>
@@ -18716,7 +18716,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>567</v>
@@ -18724,7 +18724,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>567</v>
@@ -18732,7 +18732,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="B27" s="27" t="s">
         <v>567</v>
@@ -18740,7 +18740,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>1432</v>
+        <v>1429</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>567</v>
@@ -18748,7 +18748,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>1433</v>
+        <v>1430</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>567</v>
@@ -18756,7 +18756,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>1434</v>
+        <v>1431</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>567</v>
@@ -18764,7 +18764,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
-        <v>1435</v>
+        <v>1432</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -18772,7 +18772,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -18780,7 +18780,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>567</v>
@@ -18799,7 +18799,7 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
@@ -18815,7 +18815,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
       <c r="B2" t="s">
         <v>564</v>
@@ -18823,7 +18823,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="B3" s="27" t="s">
         <v>564</v>
@@ -18831,7 +18831,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>564</v>
@@ -18839,7 +18839,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>564</v>
@@ -18847,7 +18847,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>564</v>
@@ -18855,7 +18855,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>564</v>
@@ -18863,7 +18863,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1448</v>
+        <v>1445</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -18871,7 +18871,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1449</v>
+        <v>1446</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>9</v>
@@ -18879,7 +18879,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1450</v>
+        <v>1447</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>9</v>
@@ -18887,7 +18887,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1451</v>
+        <v>1448</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>9</v>
@@ -18895,7 +18895,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1452</v>
+        <v>1449</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>9</v>
@@ -18903,7 +18903,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1453</v>
+        <v>1450</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>9</v>
@@ -18911,7 +18911,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1454</v>
+        <v>1451</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>564</v>
@@ -18919,7 +18919,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1455</v>
+        <v>1452</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>9</v>
@@ -18927,7 +18927,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1456</v>
+        <v>1453</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>564</v>
@@ -18935,7 +18935,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>9</v>
@@ -18943,7 +18943,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1458</v>
+        <v>1455</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>9</v>
@@ -18951,7 +18951,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1459</v>
+        <v>1456</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>9</v>
@@ -18959,7 +18959,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1460</v>
+        <v>1457</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>9</v>
@@ -18967,7 +18967,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1461</v>
+        <v>1458</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>9</v>
@@ -18975,7 +18975,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1462</v>
+        <v>1459</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>9</v>
@@ -18983,7 +18983,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1463</v>
+        <v>1460</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>564</v>
@@ -18991,7 +18991,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>564</v>
@@ -18999,7 +18999,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
       <c r="B25" s="27" t="s">
         <v>9</v>
@@ -19007,7 +19007,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1466</v>
+        <v>1463</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>9</v>
@@ -19015,7 +19015,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1467</v>
+        <v>1464</v>
       </c>
       <c r="B27" t="s">
         <v>567</v>
@@ -19023,7 +19023,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>564</v>
@@ -19031,7 +19031,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>564</v>
@@ -19039,7 +19039,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>9</v>
@@ -19047,7 +19047,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1471</v>
+        <v>1468</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>567</v>
@@ -19055,7 +19055,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
       <c r="B32" s="27" t="s">
         <v>567</v>
@@ -19063,7 +19063,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>9</v>
@@ -19071,7 +19071,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>9</v>
@@ -19079,7 +19079,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>9</v>
@@ -19087,7 +19087,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1476</v>
+        <v>1473</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>9</v>
@@ -19095,7 +19095,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1477</v>
+        <v>1474</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>9</v>
@@ -19103,7 +19103,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1478</v>
+        <v>1475</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>9</v>
@@ -19111,7 +19111,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1479</v>
+        <v>1476</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>9</v>
@@ -19119,7 +19119,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1480</v>
+        <v>1477</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>9</v>
@@ -19127,7 +19127,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1481</v>
+        <v>1478</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>564</v>
@@ -19146,7 +19146,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -19311,7 +19311,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -19430,7 +19430,7 @@
       <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -20329,7 +20329,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
@@ -20337,13 +20337,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B1" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="C1" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -20354,139 +20354,139 @@
         <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="B3" t="s">
         <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="B4" t="s">
         <v>213</v>
       </c>
       <c r="C4" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B5" t="s">
         <v>213</v>
       </c>
       <c r="C5" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="B6" t="s">
         <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B7" t="s">
         <v>199</v>
       </c>
       <c r="C7" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="B8" t="s">
         <v>213</v>
       </c>
       <c r="C8" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="B9" t="s">
         <v>213</v>
       </c>
       <c r="C9" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="B10" t="s">
         <v>203</v>
       </c>
       <c r="C10" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="B11" t="s">
         <v>214</v>
       </c>
       <c r="C11" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="B12" t="s">
         <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="B13" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="C13" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B14" t="s">
         <v>205</v>
       </c>
       <c r="C14" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
     </row>
   </sheetData>
@@ -20502,7 +20502,7 @@
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -20904,7 +20904,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
       <c r="B29" s="28" t="s">
         <v>226</v>
@@ -20932,7 +20932,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>1439</v>
+        <v>1436</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>221</v>
@@ -20946,7 +20946,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1440</v>
+        <v>1437</v>
       </c>
       <c r="B32" s="28" t="s">
         <v>226</v>
@@ -20960,7 +20960,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1441</v>
+        <v>1438</v>
       </c>
       <c r="B33" s="27" t="s">
         <v>25</v>
@@ -20974,7 +20974,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1483</v>
+        <v>1480</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>232</v>
@@ -21000,14 +21000,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B1" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -21023,7 +21023,7 @@
         <v>860</v>
       </c>
       <c r="B3" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -21031,7 +21031,7 @@
         <v>245</v>
       </c>
       <c r="B4" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -21039,7 +21039,7 @@
         <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -21055,7 +21055,7 @@
         <v>861</v>
       </c>
       <c r="B7" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -21063,7 +21063,7 @@
         <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -21079,7 +21079,7 @@
         <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -21087,7 +21087,7 @@
         <v>863</v>
       </c>
       <c r="B11" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -21095,7 +21095,7 @@
         <v>864</v>
       </c>
       <c r="B12" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -21103,7 +21103,7 @@
         <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -21111,7 +21111,7 @@
         <v>262</v>
       </c>
       <c r="B14" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -21119,7 +21119,7 @@
         <v>865</v>
       </c>
       <c r="B15" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -21143,7 +21143,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -22274,7 +22274,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -22450,7 +22450,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -22472,7 +22472,7 @@
       <selection activeCell="B50" sqref="B2:B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="54.140625" style="27" customWidth="1"/>
     <col min="3" max="3" width="180.5703125" style="31" customWidth="1"/>
@@ -22484,10 +22484,10 @@
         <v>37</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -22495,7 +22495,7 @@
         <v>986</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>1525</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -22503,23 +22503,23 @@
         <v>985</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1485</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
-        <v>1486</v>
+        <v>1483</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>1487</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>1488</v>
+        <v>1485</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>1489</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -22527,199 +22527,199 @@
         <v>988</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>1490</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>1491</v>
+        <v>1488</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>1492</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="27" t="s">
-        <v>1503</v>
+        <v>1500</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>1504</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>1509</v>
+        <v>1506</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>1510</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>1495</v>
+        <v>1492</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>1496</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>1501</v>
+        <v>1498</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>1502</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
-        <v>1493</v>
+        <v>1490</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>1494</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>1511</v>
+        <v>1508</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>1512</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>1505</v>
+        <v>1502</v>
       </c>
       <c r="C14" s="27" t="s">
-        <v>1506</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
-        <v>1523</v>
+        <v>1520</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>1524</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>1499</v>
+        <v>1496</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>1500</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>1521</v>
+        <v>1518</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>1522</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>1519</v>
+        <v>1516</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>1520</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>1513</v>
+        <v>1510</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>1514</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>1517</v>
+        <v>1514</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>1518</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="27" t="s">
-        <v>1515</v>
+        <v>1512</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>1516</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="27" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>1507</v>
+        <v>1504</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>1508</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>1526</v>
+        <v>1523</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>1527</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>1536</v>
+        <v>1533</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>1537</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>1534</v>
+        <v>1531</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>1535</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -22727,95 +22727,95 @@
         <v>1011</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>1532</v>
+        <v>1529</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>1533</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="27" t="s">
-        <v>1530</v>
+        <v>1527</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>1531</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>1538</v>
+        <v>1535</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>1539</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>1540</v>
+        <v>1537</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -22823,335 +22823,335 @@
         <v>987</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="27" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="27" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="27" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="27" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="27" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="C51" s="27" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="27" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="27" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="27" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>1607</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="27" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="27" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>1609</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="27" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="27" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="27" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
-        <v>1649</v>
+        <v>1646</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
-        <v>1645</v>
+        <v>1642</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
-        <v>1637</v>
+        <v>1634</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>1638</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
-        <v>1659</v>
+        <v>1656</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
-        <v>1629</v>
+        <v>1626</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>1630</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>1639</v>
+        <v>1636</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -23159,127 +23159,127 @@
         <v>984</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="C88" s="31" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="27" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="27" t="s">
-        <v>1647</v>
+        <v>1644</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>1648</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
-        <v>1641</v>
+        <v>1638</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="27" t="s">
-        <v>1635</v>
+        <v>1632</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="27" t="s">
-        <v>1665</v>
+        <v>1662</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="27" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="C98" s="31" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="27" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="27" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
     </row>
   </sheetData>
@@ -23301,7 +23301,7 @@
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -24200,7 +24200,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -25100,7 +25100,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -25363,7 +25363,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -25394,13 +25394,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="80.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -25547,12 +25548,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>1223</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -25728,13 +25729,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -25873,12 +25875,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>1223</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changing email default values attribute setter
Updating CT, default value for all dataset when it's not set. Don't have to check org name.+ Default value comes from Look-up table.
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngariepy\Documents\GitHub\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="868" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="PyCSW_config" sheetId="40" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5375" uniqueCount="1696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5377" uniqueCount="1698">
   <si>
     <t>default_key</t>
   </si>
@@ -5153,6 +5153,12 @@
   </si>
   <si>
     <t>ON</t>
+  </si>
+  <si>
+    <t>_default_email</t>
+  </si>
+  <si>
+    <t>pilote@donneesquebec.ca</t>
   </si>
 </sst>
 </file>
@@ -5294,8 +5300,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -5313,7 +5319,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5577,11 +5583,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.28515625" bestFit="1" customWidth="1"/>
@@ -5655,7 +5661,7 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.5703125" customWidth="1"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
@@ -5898,7 +5904,7 @@
       <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -6176,13 +6182,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
@@ -6506,6 +6512,14 @@
       </c>
       <c r="B40" t="s">
         <v>1248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1697</v>
       </c>
     </row>
   </sheetData>
@@ -6525,7 +6539,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
@@ -6880,7 +6894,7 @@
       <selection activeCell="B471" sqref="B471:D471"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="168.42578125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
@@ -13594,7 +13608,7 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -13970,7 +13984,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
@@ -14014,7 +14028,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
@@ -14189,7 +14203,7 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -14901,7 +14915,7 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
   </cols>
@@ -15119,7 +15133,7 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
@@ -15187,7 +15201,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" customWidth="1"/>
@@ -15278,7 +15292,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
@@ -15453,7 +15467,7 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="43.28515625" customWidth="1"/>
@@ -15957,7 +15971,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -16020,7 +16034,7 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="2" width="38.85546875" customWidth="1"/>
@@ -16279,7 +16293,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
@@ -16591,7 +16605,7 @@
       <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82" customWidth="1"/>
     <col min="2" max="2" width="95" customWidth="1"/>
@@ -17912,7 +17926,7 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="60.42578125" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" customWidth="1"/>
@@ -18195,7 +18209,7 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="53.5703125" customWidth="1"/>
@@ -18542,7 +18556,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -18707,7 +18721,7 @@
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="1"/>
     <col min="2" max="2" width="45.140625" customWidth="1"/>
@@ -19684,7 +19698,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
@@ -19803,7 +19817,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
@@ -19976,7 +19990,7 @@
       <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -20474,7 +20488,7 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -20617,7 +20631,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
@@ -21748,7 +21762,7 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" customWidth="1"/>
@@ -21946,7 +21960,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="54.140625" style="27" customWidth="1"/>
     <col min="3" max="3" width="180.5703125" style="31" customWidth="1"/>
@@ -22777,7 +22791,7 @@
       <selection activeCell="A2" sqref="A2:A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="207.5703125" customWidth="1"/>
   </cols>
@@ -23310,7 +23324,7 @@
       <selection activeCell="C80" sqref="C1:C80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -24209,7 +24223,7 @@
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
@@ -25108,7 +25122,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.85546875" customWidth="1"/>
     <col min="2" max="2" width="74.85546875" customWidth="1"/>
@@ -26008,7 +26022,7 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
@@ -26271,7 +26285,7 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -26306,7 +26320,7 @@
       <selection activeCell="B12" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="80.42578125" customWidth="1"/>

</xml_diff>

<commit_message>
Fixing bug for longueil logo
Fixing bug for longueil logo
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5077,9 +5077,6 @@
     <t>https://raw.githubusercontent.com/federal-geospatial-platform/fgp-metadata-proxy/master/images/resampled/laval.png</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/federal-geospatial-platform/fgp-metadata-proxy/master/images/resampled/llongueuil.gif</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/federal-geospatial-platform/fgp-metadata-proxy/master/images/resampled/montreal.png</t>
   </si>
   <si>
@@ -5165,6 +5162,9 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/federal-geospatial-platform/fgp-metadata-proxy/master/images/resampled/stationnement_mtl.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/federal-geospatial-platform/fgp-metadata-proxy/master/images/resampled/longueuil.png</t>
   </si>
 </sst>
 </file>
@@ -16087,7 +16087,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16515,7 +16515,7 @@
         <v>954</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>1670</v>
+        <v>1699</v>
       </c>
       <c r="D25" t="s">
         <v>888</v>
@@ -16532,7 +16532,7 @@
         <v>955</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="D26" t="s">
         <v>888</v>
@@ -16549,7 +16549,7 @@
         <v>956</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="D27" t="s">
         <v>888</v>
@@ -16566,7 +16566,7 @@
         <v>957</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="D28" t="s">
         <v>888</v>
@@ -16583,7 +16583,7 @@
         <v>958</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D29" t="s">
         <v>888</v>
@@ -16600,7 +16600,7 @@
         <v>959</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D30" t="s">
         <v>888</v>
@@ -16617,7 +16617,7 @@
         <v>960</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D31" t="s">
         <v>888</v>
@@ -16634,7 +16634,7 @@
         <v>1241</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="D32" t="s">
         <v>888</v>
@@ -16651,7 +16651,7 @@
         <v>961</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D33" t="s">
         <v>888</v>
@@ -16668,7 +16668,7 @@
         <v>1242</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D34" t="s">
         <v>888</v>
@@ -16787,7 +16787,7 @@
         <v>886</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="D41" t="s">
         <v>888</v>
@@ -16804,7 +16804,7 @@
         <v>1237</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="D42" t="s">
         <v>888</v>
@@ -16821,7 +16821,7 @@
         <v>1238</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="D43" t="s">
         <v>888</v>
@@ -16872,7 +16872,7 @@
         <v>1239</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="D46" t="s">
         <v>888</v>
@@ -16889,7 +16889,7 @@
         <v>897</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="D47" t="s">
         <v>888</v>
@@ -16906,7 +16906,7 @@
         <v>1240</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="D48" t="s">
         <v>888</v>
@@ -16940,7 +16940,7 @@
         <v>901</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="D50" t="s">
         <v>888</v>
@@ -16974,7 +16974,7 @@
         <v>907</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D52" t="s">
         <v>888</v>
@@ -16991,7 +16991,7 @@
         <v>1249</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="D53" t="s">
         <v>888</v>
@@ -17008,7 +17008,7 @@
         <v>927</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D54" t="s">
         <v>888</v>
@@ -17042,7 +17042,7 @@
         <v>929</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="D56" t="s">
         <v>888</v>
@@ -17059,7 +17059,7 @@
         <v>930</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="D57" t="s">
         <v>888</v>
@@ -17076,7 +17076,7 @@
         <v>1243</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="D58" t="s">
         <v>888</v>
@@ -17093,7 +17093,7 @@
         <v>1244</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D59" t="s">
         <v>888</v>
@@ -17110,7 +17110,7 @@
         <v>1245</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D60" t="s">
         <v>888</v>
@@ -17127,7 +17127,7 @@
         <v>1246</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D61" t="s">
         <v>888</v>
@@ -17144,7 +17144,7 @@
         <v>943</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D62" t="s">
         <v>888</v>
@@ -17178,7 +17178,7 @@
         <v>945</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="D64" t="s">
         <v>888</v>
@@ -17195,7 +17195,7 @@
         <v>1250</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D65" t="s">
         <v>888</v>
@@ -17212,7 +17212,7 @@
         <v>1247</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D66" t="s">
         <v>888</v>
@@ -17229,7 +17229,7 @@
         <v>1248</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D67" t="s">
         <v>888</v>

</xml_diff>

<commit_message>
made most of nic's changes
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/NRCAN/fgp-metadata-proxy/FME_files/LOOKUP_TABLES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556B3CEC-BBAD-BC4F-A65A-21646FE2E3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB7A67-F126-8C44-8A3C-FDAB1FEAA494}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-200" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="868" firstSheet="12" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PyCSW_config" sheetId="40" r:id="rId1"/>
@@ -37,28 +37,29 @@
     <sheet name="License_QC" sheetId="27" r:id="rId22"/>
     <sheet name="NB_ESRISERVICES" sheetId="51" r:id="rId23"/>
     <sheet name="NB_Remove" sheetId="46" r:id="rId24"/>
-    <sheet name="NB_KeywordRemove" sheetId="48" r:id="rId25"/>
-    <sheet name="NB_SlashCountSeparator" sheetId="42" r:id="rId26"/>
-    <sheet name="NB_TOPICS_DATASET" sheetId="50" r:id="rId27"/>
-    <sheet name="NB_TOPICS_GENERIC" sheetId="49" r:id="rId28"/>
-    <sheet name="Progress" sheetId="10" r:id="rId29"/>
-    <sheet name="QC_JSON_CONFIG" sheetId="31" r:id="rId30"/>
-    <sheet name="ResourceType_TBS_QC" sheetId="32" r:id="rId31"/>
-    <sheet name="Role" sheetId="11" r:id="rId32"/>
-    <sheet name="Sector_ON" sheetId="35" r:id="rId33"/>
-    <sheet name="Sector_NB" sheetId="43" r:id="rId34"/>
-    <sheet name="Sector_QC" sheetId="22" r:id="rId35"/>
-    <sheet name="Spatial_ON" sheetId="36" r:id="rId36"/>
-    <sheet name="SpatialRep_API_ON" sheetId="37" r:id="rId37"/>
-    <sheet name="SpatialRef" sheetId="13" r:id="rId38"/>
-    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId39"/>
-    <sheet name="SubjectNTopic_TBS_QC" sheetId="30" r:id="rId40"/>
-    <sheet name="Update" sheetId="6" r:id="rId41"/>
-    <sheet name="UpdateFrequency_TBS_QC" sheetId="29" r:id="rId42"/>
-    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId43"/>
-    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId44"/>
-    <sheet name="WMS_URL_QC" sheetId="38" r:id="rId45"/>
-    <sheet name="QC_MAP_RES_REMOVE" sheetId="39" r:id="rId46"/>
+    <sheet name="NB_GeoDataTypes" sheetId="52" r:id="rId25"/>
+    <sheet name="NB_Keywords" sheetId="48" r:id="rId26"/>
+    <sheet name="NB_SlashCountSeparator" sheetId="42" r:id="rId27"/>
+    <sheet name="NB_TOPICS_DATASET" sheetId="50" r:id="rId28"/>
+    <sheet name="NB_TOPICS_GENERIC" sheetId="49" r:id="rId29"/>
+    <sheet name="Progress" sheetId="10" r:id="rId30"/>
+    <sheet name="QC_JSON_CONFIG" sheetId="31" r:id="rId31"/>
+    <sheet name="ResourceType_TBS_QC" sheetId="32" r:id="rId32"/>
+    <sheet name="Role" sheetId="11" r:id="rId33"/>
+    <sheet name="Sector_ON" sheetId="35" r:id="rId34"/>
+    <sheet name="Sector_NB" sheetId="43" r:id="rId35"/>
+    <sheet name="Sector_QC" sheetId="22" r:id="rId36"/>
+    <sheet name="Spatial_ON" sheetId="36" r:id="rId37"/>
+    <sheet name="SpatialRep_API_ON" sheetId="37" r:id="rId38"/>
+    <sheet name="SpatialRef" sheetId="13" r:id="rId39"/>
+    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId40"/>
+    <sheet name="SubjectNTopic_TBS_QC" sheetId="30" r:id="rId41"/>
+    <sheet name="Update" sheetId="6" r:id="rId42"/>
+    <sheet name="UpdateFrequency_TBS_QC" sheetId="29" r:id="rId43"/>
+    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId44"/>
+    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId45"/>
+    <sheet name="WMS_URL_QC" sheetId="38" r:id="rId46"/>
+    <sheet name="QC_MAP_RES_REMOVE" sheetId="39" r:id="rId47"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5938" uniqueCount="1936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6235" uniqueCount="2042">
   <si>
     <t>default_key</t>
   </si>
@@ -5883,15 +5884,340 @@
   </si>
   <si>
     <t>NB</t>
+  </si>
+  <si>
+    <t>tag_validity</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>nursing</t>
+  </si>
+  <si>
+    <t>limits</t>
+  </si>
+  <si>
+    <t>local service districts</t>
+  </si>
+  <si>
+    <t>parcels</t>
+  </si>
+  <si>
+    <t>nbhc</t>
+  </si>
+  <si>
+    <t>french immersion</t>
+  </si>
+  <si>
+    <t>mineral</t>
+  </si>
+  <si>
+    <t>federal</t>
+  </si>
+  <si>
+    <t>point cloud</t>
+  </si>
+  <si>
+    <t>orignial</t>
+  </si>
+  <si>
+    <t>lyme disease</t>
+  </si>
+  <si>
+    <t>downtown</t>
+  </si>
+  <si>
+    <t>mineral deposits</t>
+  </si>
+  <si>
+    <t>ecodistrict</t>
+  </si>
+  <si>
+    <t>parish</t>
+  </si>
+  <si>
+    <t>district scolaire</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>ecosection</t>
+  </si>
+  <si>
+    <t>watershed</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>nuisance</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>roadkill</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>natural</t>
+  </si>
+  <si>
+    <t>senior</t>
+  </si>
+  <si>
+    <t>accident</t>
+  </si>
+  <si>
+    <t>bear</t>
+  </si>
+  <si>
+    <t>fundy</t>
+  </si>
+  <si>
+    <t>central business district</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>commercial truck</t>
+  </si>
+  <si>
+    <t>tick</t>
+  </si>
+  <si>
+    <t>forest</t>
+  </si>
+  <si>
+    <t>bedrock</t>
+  </si>
+  <si>
+    <t>offshore</t>
+  </si>
+  <si>
+    <t>ecoregion</t>
+  </si>
+  <si>
+    <t>wellfield</t>
+  </si>
+  <si>
+    <t>local government</t>
+  </si>
+  <si>
+    <t>drivers exam</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>wetland</t>
+  </si>
+  <si>
+    <t>conservation</t>
+  </si>
+  <si>
+    <t>hospitals</t>
+  </si>
+  <si>
+    <t>well</t>
+  </si>
+  <si>
+    <t>peat</t>
+  </si>
+  <si>
+    <t>fishing</t>
+  </si>
+  <si>
+    <t>crown land</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>public school</t>
+  </si>
+  <si>
+    <t>northumberland</t>
+  </si>
+  <si>
+    <t>ours</t>
+  </si>
+  <si>
+    <t>lake</t>
+  </si>
+  <si>
+    <t>ecole</t>
+  </si>
+  <si>
+    <t>drillhole</t>
+  </si>
+  <si>
+    <t>minerals</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>deer</t>
+  </si>
+  <si>
+    <t>csnb</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>protected</t>
+  </si>
+  <si>
+    <t>moose</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>corporate registry</t>
+  </si>
+  <si>
+    <t>mining</t>
+  </si>
+  <si>
+    <t>military</t>
+  </si>
+  <si>
+    <t>geology</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>licensed</t>
+  </si>
+  <si>
+    <t>mineral exploration</t>
+  </si>
+  <si>
+    <t>municipality</t>
+  </si>
+  <si>
+    <t>new brunswick</t>
+  </si>
+  <si>
+    <t>petroleum</t>
+  </si>
+  <si>
+    <t>school year</t>
+  </si>
+  <si>
+    <t>rail</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>school district</t>
+  </si>
+  <si>
+    <t>wildlife</t>
+  </si>
+  <si>
+    <t>sections</t>
+  </si>
+  <si>
+    <t>community boundaries</t>
+  </si>
+  <si>
+    <t>service centre</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>national</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>railway</t>
+  </si>
+  <si>
+    <t>inland</t>
+  </si>
+  <si>
+    <t>pipeline</t>
+  </si>
+  <si>
+    <t>assessment</t>
+  </si>
+  <si>
+    <t>seafloor</t>
+  </si>
+  <si>
+    <t>land use</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>New Brunswick data</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>polygon</t>
+  </si>
+  <si>
+    <t>multipoint</t>
+  </si>
+  <si>
+    <t>multiline</t>
+  </si>
+  <si>
+    <t>multipolygon</t>
+  </si>
+  <si>
+    <t>datatype</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5982,6 +6308,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -6027,27 +6359,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -6055,7 +6388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -6065,30 +6398,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Hyperlink 3" xfId="5" xr:uid="{936E26A9-6C8B-6842-A1AF-9FBF27EF1270}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{2CEFD527-886F-834C-9CCC-35544F7406DC}"/>
+    <cellStyle name="Normal 4" xfId="6" xr:uid="{E04371D7-9CD3-8E47-923E-BEA66BF5575D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6368,7 +6705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -16524,418 +16861,56 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D4E8AF-B2CC-A841-BA4B-ADF3FBC1AAF2}">
-  <dimension ref="D1:D81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353E734B-FA88-F240-81B5-0B79D6736D9B}">
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="41"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D1" t="s">
-        <v>1829</v>
-      </c>
-    </row>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D2" t="s">
-        <v>1828</v>
-      </c>
-    </row>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="5" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="6" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="7" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D7" t="s">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="8" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="9" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
-        <v>1821</v>
-      </c>
-    </row>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
-        <v>1820</v>
-      </c>
-    </row>
-    <row r="11" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
-        <v>1819</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D12" t="s">
-        <v>1818</v>
-      </c>
-    </row>
-    <row r="13" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D13" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="14" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
-        <v>1816</v>
-      </c>
-    </row>
-    <row r="15" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D15" t="s">
-        <v>1815</v>
-      </c>
-    </row>
-    <row r="16" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>1813</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
-        <v>1812</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
-        <v>1811</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" t="s">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" t="s">
-        <v>1809</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
-        <v>1808</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" t="s">
-        <v>1807</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
-        <v>1806</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D25" t="s">
-        <v>1805</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
-        <v>1804</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
-        <v>1802</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
-        <v>1799</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D32" t="s">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
-        <v>1797</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
-        <v>1795</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
-        <v>1791</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
-        <v>1786</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D47" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
-        <v>1780</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
-        <v>1776</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
-        <v>1773</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D62" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D63" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
-        <v>1768</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D65" t="s">
-        <v>1767</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
-        <v>1766</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D67" t="s">
-        <v>1765</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D68" t="s">
-        <v>1764</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D69" t="s">
-        <v>1763</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
-        <v>1762</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D74" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D75" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
-        <v>1756</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D77" t="s">
-        <v>1755</v>
-      </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D79" t="s">
-        <v>1753</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D80" t="s">
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D81" t="s">
-        <v>1751</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="41" t="s">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -16944,6 +16919,1506 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D4E8AF-B2CC-A841-BA4B-ADF3FBC1AAF2}">
+  <dimension ref="A1:B185"/>
+  <sheetViews>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>1964</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
+        <v>2029</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="39" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
+        <v>1965</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="39" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="40" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>2023</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="40" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="40" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="40" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="40" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="40" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="40" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="39" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="40" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="39" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="39" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="39" t="s">
+        <v>1980</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="39" t="s">
+        <v>1987</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="39" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="39" t="s">
+        <v>1998</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="39" t="s">
+        <v>2001</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="39" t="s">
+        <v>1953</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="40" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="39" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="39" t="s">
+        <v>1995</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="39" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="40" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="39" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="39" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="40" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="40" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="39" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="39" t="s">
+        <v>1955</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="39" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="40" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B47" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="40" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B48" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="40" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="40" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B50" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="39" t="s">
+        <v>1945</v>
+      </c>
+      <c r="B51" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="40" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B52" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="40" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B53" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="39" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="40" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="40" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="39" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="40" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="40" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="39" t="s">
+        <v>1943</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="39" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="39" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="40" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B63" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="39" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B64" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="40" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B65" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="40" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B66" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="40" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B67" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="39" t="s">
+        <v>2025</v>
+      </c>
+      <c r="B68" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="39" t="s">
+        <v>565</v>
+      </c>
+      <c r="B69" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="40" t="s">
+        <v>564</v>
+      </c>
+      <c r="B70" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="39" t="s">
+        <v>1989</v>
+      </c>
+      <c r="B72" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="40" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B73" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="39" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B74" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="40" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B75" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76" s="39" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B76" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77" s="39" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B77" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="40" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B78" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="40" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B79" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="40" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B80" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A81" s="39" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B81" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="39" t="s">
+        <v>2031</v>
+      </c>
+      <c r="B82" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A83" s="39" t="s">
+        <v>2010</v>
+      </c>
+      <c r="B83" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="40" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B84" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="40" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B85" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="40" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B86" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A87" s="39" t="s">
+        <v>1939</v>
+      </c>
+      <c r="B87" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A88" s="39" t="s">
+        <v>1977</v>
+      </c>
+      <c r="B88" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A89" s="39" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B89" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A90" s="39" t="s">
+        <v>1948</v>
+      </c>
+      <c r="B90" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="40" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B91" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A92" s="39" t="s">
+        <v>1997</v>
+      </c>
+      <c r="B92" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="40" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B93" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="39" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B94" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A95" s="39" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B95" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A96" s="39" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B96" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A97" s="39" t="s">
+        <v>2011</v>
+      </c>
+      <c r="B97" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="40" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B98" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A99" s="39" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B99" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A100" s="39" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B100" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="39" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B101" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="40" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B102" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A103" s="39" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B103" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="40" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B104" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A105" s="39" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B105" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="39" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B106" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A107" s="39" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B107" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="40" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B108" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="40" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B109" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A110" s="39" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B110" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="40" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B111" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="40" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B112" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="39" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B113" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A114" s="39" t="s">
+        <v>2013</v>
+      </c>
+      <c r="B114" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A115" s="39" t="s">
+        <v>2034</v>
+      </c>
+      <c r="B115" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="40" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B116" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A117" s="39" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B117" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="40" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B118" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="40" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B119" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="40" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B120" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="39" t="s">
+        <v>1958</v>
+      </c>
+      <c r="B121" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="39" t="s">
+        <v>1938</v>
+      </c>
+      <c r="B122" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="39" t="s">
+        <v>1974</v>
+      </c>
+      <c r="B123" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="39" t="s">
+        <v>2017</v>
+      </c>
+      <c r="B124" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="39" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B125" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="39" t="s">
+        <v>1992</v>
+      </c>
+      <c r="B126" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="39" t="s">
+        <v>2009</v>
+      </c>
+      <c r="B127" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="40" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B128" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="40" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B129" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A130" s="39" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B130" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A131" s="39" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B131" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A132" s="39" t="s">
+        <v>1954</v>
+      </c>
+      <c r="B132" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="40" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B133" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A134" s="39" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B134" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="40" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B135" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="40" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B136" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A137" s="39" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B137" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="40" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B138" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A139" s="39" t="s">
+        <v>2028</v>
+      </c>
+      <c r="B139" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="40" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B140" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="39" t="s">
+        <v>1946</v>
+      </c>
+      <c r="B141" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A142" s="39" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B142" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="40" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B143" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="39" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B144" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="40" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B145" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A146" s="39" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B146" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A147" s="39" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B147" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A148" s="39" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B148" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A149" s="39" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B149" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A150" s="39" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B150" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="40" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B151" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="40" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B152" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="40" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B153" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="40" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B154" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A155" s="39" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B155" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="40" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B156" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A157" s="39" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B157" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="40" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B158" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A159" s="39" t="s">
+        <v>1957</v>
+      </c>
+      <c r="B159" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A160" s="39" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B160" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A161" s="39" t="s">
+        <v>2015</v>
+      </c>
+      <c r="B161" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A162" s="39" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B162" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A163" s="39" t="s">
+        <v>2020</v>
+      </c>
+      <c r="B163" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A164" s="39" t="s">
+        <v>1963</v>
+      </c>
+      <c r="B164" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A165" s="39" t="s">
+        <v>2022</v>
+      </c>
+      <c r="B165" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="40" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B166" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="40" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B167" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="40" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B168" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="40" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B169" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A170" s="39" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B170" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="40" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B171" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="40" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B172" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="40" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B173" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A174" s="39" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B174" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A175" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="B175" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="40" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B176" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A177" s="39" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B177" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A178" s="39" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B178" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A179" s="39" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B179" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A180" s="39" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B180" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A181" s="39" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B181" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A182" s="39" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B182" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A183" s="39" t="s">
+        <v>2019</v>
+      </c>
+      <c r="B183" s="40" t="s">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="40" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B184" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="40" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B185" s="40" t="s">
+        <v>1937</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5224612A-E8BC-3B4B-868A-2E969A670E59}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -16987,11 +18462,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E172906-5832-BA43-9640-F9D97BB32E78}">
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C35" workbookViewId="0">
       <selection activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
@@ -17616,7 +19091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A505167C-0F6B-3F4A-80B6-E3860631B820}">
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -17901,181 +19376,6 @@
       </c>
       <c r="B34" s="33" t="s">
         <v>166</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1"/>
-    <col min="2" max="2" width="39.6640625" customWidth="1"/>
-    <col min="3" max="3" width="35.5" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>472</v>
-      </c>
-      <c r="B2" t="s">
-        <v>472</v>
-      </c>
-      <c r="C2" t="s">
-        <v>473</v>
-      </c>
-      <c r="D2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>475</v>
-      </c>
-      <c r="B3" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" t="s">
-        <v>476</v>
-      </c>
-      <c r="D3" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>478</v>
-      </c>
-      <c r="B4" t="s">
-        <v>478</v>
-      </c>
-      <c r="C4" t="s">
-        <v>479</v>
-      </c>
-      <c r="D4" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>481</v>
-      </c>
-      <c r="D5" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B6" t="s">
-        <v>483</v>
-      </c>
-      <c r="C6" t="s">
-        <v>484</v>
-      </c>
-      <c r="D6" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>486</v>
-      </c>
-      <c r="B7" t="s">
-        <v>486</v>
-      </c>
-      <c r="C7" t="s">
-        <v>487</v>
-      </c>
-      <c r="D7" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>489</v>
-      </c>
-      <c r="B8" t="s">
-        <v>489</v>
-      </c>
-      <c r="C8" t="s">
-        <v>490</v>
-      </c>
-      <c r="D8" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>492</v>
-      </c>
-      <c r="B9" t="s">
-        <v>492</v>
-      </c>
-      <c r="C9" t="s">
-        <v>493</v>
-      </c>
-      <c r="D9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>495</v>
-      </c>
-      <c r="B10" t="s">
-        <v>472</v>
-      </c>
-      <c r="C10" t="s">
-        <v>473</v>
-      </c>
-      <c r="D10" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>496</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>481</v>
-      </c>
-      <c r="D11" t="s">
-        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -19061,6 +20361,181 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B4" t="s">
+        <v>478</v>
+      </c>
+      <c r="C4" t="s">
+        <v>479</v>
+      </c>
+      <c r="D4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>483</v>
+      </c>
+      <c r="B6" t="s">
+        <v>483</v>
+      </c>
+      <c r="C6" t="s">
+        <v>484</v>
+      </c>
+      <c r="D6" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>486</v>
+      </c>
+      <c r="B7" t="s">
+        <v>486</v>
+      </c>
+      <c r="C7" t="s">
+        <v>487</v>
+      </c>
+      <c r="D7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>489</v>
+      </c>
+      <c r="B8" t="s">
+        <v>489</v>
+      </c>
+      <c r="C8" t="s">
+        <v>490</v>
+      </c>
+      <c r="D8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>492</v>
+      </c>
+      <c r="B9" t="s">
+        <v>492</v>
+      </c>
+      <c r="C9" t="s">
+        <v>493</v>
+      </c>
+      <c r="D9" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>495</v>
+      </c>
+      <c r="B10" t="s">
+        <v>472</v>
+      </c>
+      <c r="C10" t="s">
+        <v>473</v>
+      </c>
+      <c r="D10" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>496</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>481</v>
+      </c>
+      <c r="D11" t="s">
+        <v>482</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -19564,7 +21039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -19627,7 +21102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -19886,7 +21361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -20198,7 +21673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C13296E-A4B4-7548-B29A-EA44B283FB12}">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -20354,7 +21829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:E77"/>
   <sheetViews>
@@ -21730,7 +23205,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -22013,7 +23488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -22360,7 +23835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -22522,125 +23997,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>567</v>
-      </c>
-      <c r="D2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>565</v>
-      </c>
-      <c r="B3" t="s">
-        <v>565</v>
-      </c>
-      <c r="C3" t="s">
-        <v>564</v>
-      </c>
-      <c r="D3" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>562</v>
-      </c>
-      <c r="B4" t="s">
-        <v>562</v>
-      </c>
-      <c r="C4" t="s">
-        <v>561</v>
-      </c>
-      <c r="D4" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>560</v>
-      </c>
-      <c r="B5" t="s">
-        <v>560</v>
-      </c>
-      <c r="C5" t="s">
-        <v>560</v>
-      </c>
-      <c r="D5" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>558</v>
-      </c>
-      <c r="B6" t="s">
-        <v>558</v>
-      </c>
-      <c r="C6" t="s">
-        <v>557</v>
-      </c>
-      <c r="D6" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>555</v>
-      </c>
-      <c r="B7" t="s">
-        <v>555</v>
-      </c>
-      <c r="C7" t="s">
-        <v>554</v>
-      </c>
-      <c r="D7" t="s">
-        <v>553</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -23544,6 +24900,125 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C3" t="s">
+        <v>564</v>
+      </c>
+      <c r="D3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B4" t="s">
+        <v>562</v>
+      </c>
+      <c r="C4" t="s">
+        <v>561</v>
+      </c>
+      <c r="D4" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B5" t="s">
+        <v>560</v>
+      </c>
+      <c r="C5" t="s">
+        <v>560</v>
+      </c>
+      <c r="D5" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>558</v>
+      </c>
+      <c r="B6" t="s">
+        <v>558</v>
+      </c>
+      <c r="C6" t="s">
+        <v>557</v>
+      </c>
+      <c r="D6" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B7" t="s">
+        <v>555</v>
+      </c>
+      <c r="C7" t="s">
+        <v>554</v>
+      </c>
+      <c r="D7" t="s">
+        <v>553</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -23716,7 +25191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:D34"/>
   <sheetViews>
@@ -24214,7 +25689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -24357,7 +25832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:B140"/>
   <sheetViews>
@@ -25496,7 +26971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -25694,7 +27169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:C100"/>
   <sheetViews>
@@ -26525,7 +28000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:A107"/>
   <sheetViews>

</xml_diff>

<commit_message>
Corrected ISO abbreviation from YK to YT
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="4680" windowWidth="31440" windowHeight="21000" tabRatio="868" firstSheet="44" activeTab="53"/>
+    <workbookView xWindow="2505" yWindow="4680" windowWidth="31440" windowHeight="21000" tabRatio="868" firstSheet="16" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="Format" sheetId="7" r:id="rId15"/>
     <sheet name="Format_TBS_QC" sheetId="28" r:id="rId16"/>
     <sheet name="FrenchTranslation" sheetId="8" r:id="rId17"/>
-    <sheet name="Geodata_YK" sheetId="67" r:id="rId18"/>
+    <sheet name="Geodata_YT" sheetId="67" r:id="rId18"/>
     <sheet name="Geohub_ON_URL" sheetId="52" r:id="rId19"/>
     <sheet name="Geospatial_BC" sheetId="25" r:id="rId20"/>
     <sheet name="Geospatial_QC" sheetId="20" r:id="rId21"/>
@@ -65,7 +65,7 @@
     <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId51"/>
     <sheet name="UUID_Spatial_ON" sheetId="62" r:id="rId52"/>
     <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId53"/>
-    <sheet name="UUID_YK" sheetId="68" r:id="rId54"/>
+    <sheet name="UUID_YT" sheetId="68" r:id="rId54"/>
     <sheet name="ValidFormatList" sheetId="65" r:id="rId55"/>
     <sheet name="WMS_URL_QC" sheetId="38" r:id="rId56"/>
   </sheets>
@@ -27064,8 +27064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B307"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41593,7 +41593,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48578,7 +48578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1420"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new tags for ontario isotopics
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2510" yWindow="4680" windowWidth="11810" windowHeight="3020" tabRatio="883" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="2510" yWindow="4680" windowWidth="11810" windowHeight="3020" tabRatio="883" firstSheet="26" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12435" uniqueCount="5859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12651" uniqueCount="5919">
   <si>
     <t>default_key</t>
   </si>
@@ -17678,6 +17678,186 @@
   </si>
   <si>
     <t>liscense_id</t>
+  </si>
+  <si>
+    <t>agri-food trade</t>
+  </si>
+  <si>
+    <t>apple production</t>
+  </si>
+  <si>
+    <t>asparagus production</t>
+  </si>
+  <si>
+    <t>bean production</t>
+  </si>
+  <si>
+    <t>beet production</t>
+  </si>
+  <si>
+    <t>broccoli production</t>
+  </si>
+  <si>
+    <t>cabbage production</t>
+  </si>
+  <si>
+    <t>carrot production</t>
+  </si>
+  <si>
+    <t>cattle exports</t>
+  </si>
+  <si>
+    <t>celery production</t>
+  </si>
+  <si>
+    <t>census of agriculture</t>
+  </si>
+  <si>
+    <t>commercial fruit crops production</t>
+  </si>
+  <si>
+    <t>commercial vegetable crops production</t>
+  </si>
+  <si>
+    <t>cucumber production</t>
+  </si>
+  <si>
+    <t>dairy production</t>
+  </si>
+  <si>
+    <t>egg production</t>
+  </si>
+  <si>
+    <t>exportations de bovins</t>
+  </si>
+  <si>
+    <t>farm data by county</t>
+  </si>
+  <si>
+    <t>farm expenses</t>
+  </si>
+  <si>
+    <t>farm income</t>
+  </si>
+  <si>
+    <t>field crop production</t>
+  </si>
+  <si>
+    <t>fruit and vegetable production</t>
+  </si>
+  <si>
+    <t>fruit production and yield</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>government payments to farmers</t>
+  </si>
+  <si>
+    <t>grain corn</t>
+  </si>
+  <si>
+    <t>green pea production</t>
+  </si>
+  <si>
+    <t>honey production</t>
+  </si>
+  <si>
+    <t>livestock numbers</t>
+  </si>
+  <si>
+    <t>local food</t>
+  </si>
+  <si>
+    <t>manufacturing industries</t>
+  </si>
+  <si>
+    <t>maple syrup production</t>
+  </si>
+  <si>
+    <t>mushroom production</t>
+  </si>
+  <si>
+    <t>nurseries</t>
+  </si>
+  <si>
+    <t>onion production</t>
+  </si>
+  <si>
+    <t>ontario fruit and vegetables</t>
+  </si>
+  <si>
+    <t>ontario greenhouse vegetable production</t>
+  </si>
+  <si>
+    <t>pepper production</t>
+  </si>
+  <si>
+    <t>personnes âgées</t>
+  </si>
+  <si>
+    <t>pig exports</t>
+  </si>
+  <si>
+    <t>potato production</t>
+  </si>
+  <si>
+    <t>poultry production</t>
+  </si>
+  <si>
+    <t>prestations</t>
+  </si>
+  <si>
+    <t>production des betteraves</t>
+  </si>
+  <si>
+    <t>production des citrouilles</t>
+  </si>
+  <si>
+    <t>production des épinards</t>
+  </si>
+  <si>
+    <t>production des légumes de serre en ontario</t>
+  </si>
+  <si>
+    <t>production des poivrons</t>
+  </si>
+  <si>
+    <t>production des radis</t>
+  </si>
+  <si>
+    <t>production des rutabagas</t>
+  </si>
+  <si>
+    <t>production des tomates</t>
+  </si>
+  <si>
+    <t>production du maïs sucré</t>
+  </si>
+  <si>
+    <t>pumpkin production</t>
+  </si>
+  <si>
+    <t>radish production</t>
+  </si>
+  <si>
+    <t>recensement de l'agriculture</t>
+  </si>
+  <si>
+    <t>rutabaga production</t>
+  </si>
+  <si>
+    <t>sécurité de la vieillesse</t>
+  </si>
+  <si>
+    <t>spinach production</t>
+  </si>
+  <si>
+    <t>sweetcorn production</t>
+  </si>
+  <si>
+    <t>tomato production</t>
   </si>
 </sst>
 </file>
@@ -17858,7 +18038,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -17921,6 +18101,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -19595,7 +19778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -34562,10 +34745,10 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C263"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -34589,18 +34772,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
-        <v>5687</v>
+        <v>5847</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
-        <v>5688</v>
+        <v>5687</v>
       </c>
       <c r="B3" s="38" t="s">
         <v>172</v>
@@ -34611,7 +34794,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
-        <v>5689</v>
+        <v>5688</v>
       </c>
       <c r="B4" s="38" t="s">
         <v>172</v>
@@ -34622,7 +34805,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
-        <v>5690</v>
+        <v>5689</v>
       </c>
       <c r="B5" s="38" t="s">
         <v>172</v>
@@ -34633,7 +34816,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
-        <v>5691</v>
+        <v>5690</v>
       </c>
       <c r="B6" s="38" t="s">
         <v>172</v>
@@ -34644,7 +34827,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="s">
-        <v>5692</v>
+        <v>5691</v>
       </c>
       <c r="B7" s="38" t="s">
         <v>172</v>
@@ -34655,7 +34838,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
-        <v>5693</v>
+        <v>5692</v>
       </c>
       <c r="B8" s="38" t="s">
         <v>172</v>
@@ -34666,7 +34849,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
-        <v>5694</v>
+        <v>5693</v>
       </c>
       <c r="B9" s="38" t="s">
         <v>172</v>
@@ -34677,7 +34860,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="38" t="s">
-        <v>5695</v>
+        <v>5694</v>
       </c>
       <c r="B10" s="38" t="s">
         <v>172</v>
@@ -34688,7 +34871,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="38" t="s">
-        <v>5696</v>
+        <v>5695</v>
       </c>
       <c r="B11" s="38" t="s">
         <v>172</v>
@@ -34699,7 +34882,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="38" t="s">
-        <v>5697</v>
+        <v>5696</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>172</v>
@@ -34710,7 +34893,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
-        <v>5698</v>
+        <v>5697</v>
       </c>
       <c r="B13" s="38" t="s">
         <v>172</v>
@@ -34721,7 +34904,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="s">
-        <v>5699</v>
+        <v>5698</v>
       </c>
       <c r="B14" s="38" t="s">
         <v>172</v>
@@ -34732,7 +34915,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
-        <v>1827</v>
+        <v>5699</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>172</v>
@@ -34743,7 +34926,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
-        <v>5700</v>
+        <v>1827</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>172</v>
@@ -34754,18 +34937,18 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="38" t="s">
-        <v>5701</v>
+        <v>5700</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="38" t="s">
-        <v>5702</v>
+        <v>5701</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>175</v>
@@ -34776,7 +34959,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="38" t="s">
-        <v>5703</v>
+        <v>5702</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>175</v>
@@ -34787,7 +34970,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="38" t="s">
-        <v>5687</v>
+        <v>5703</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>175</v>
@@ -34798,7 +34981,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="38" t="s">
-        <v>5704</v>
+        <v>5687</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>175</v>
@@ -34809,7 +34992,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="38" t="s">
-        <v>5705</v>
+        <v>5704</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>175</v>
@@ -34820,7 +35003,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="38" t="s">
-        <v>5706</v>
+        <v>5705</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>175</v>
@@ -34831,7 +35014,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="38" t="s">
-        <v>5707</v>
+        <v>5706</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>175</v>
@@ -34842,7 +35025,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
-        <v>5708</v>
+        <v>5707</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>175</v>
@@ -34853,7 +35036,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="38" t="s">
-        <v>5709</v>
+        <v>5708</v>
       </c>
       <c r="B26" s="38" t="s">
         <v>175</v>
@@ -34864,7 +35047,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="38" t="s">
-        <v>5710</v>
+        <v>5709</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>175</v>
@@ -34875,7 +35058,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="38" t="s">
-        <v>5711</v>
+        <v>5710</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>175</v>
@@ -34886,7 +35069,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="38" t="s">
-        <v>5712</v>
+        <v>5711</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>175</v>
@@ -34897,7 +35080,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="38" t="s">
-        <v>5713</v>
+        <v>5712</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>175</v>
@@ -34908,7 +35091,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="38" t="s">
-        <v>5714</v>
+        <v>5713</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>175</v>
@@ -34919,7 +35102,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="38" t="s">
-        <v>5715</v>
+        <v>5714</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>175</v>
@@ -34930,7 +35113,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="38" t="s">
-        <v>5716</v>
+        <v>5715</v>
       </c>
       <c r="B33" s="38" t="s">
         <v>175</v>
@@ -34941,7 +35124,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="38" t="s">
-        <v>5717</v>
+        <v>5716</v>
       </c>
       <c r="B34" s="38" t="s">
         <v>175</v>
@@ -34952,7 +35135,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="38" t="s">
-        <v>5718</v>
+        <v>5717</v>
       </c>
       <c r="B35" s="38" t="s">
         <v>175</v>
@@ -34963,7 +35146,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="38" t="s">
-        <v>5719</v>
+        <v>5718</v>
       </c>
       <c r="B36" s="38" t="s">
         <v>175</v>
@@ -34974,7 +35157,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="38" t="s">
-        <v>5720</v>
+        <v>5719</v>
       </c>
       <c r="B37" s="38" t="s">
         <v>175</v>
@@ -34985,7 +35168,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="38" t="s">
-        <v>1897</v>
+        <v>5720</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>175</v>
@@ -34996,7 +35179,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="38" t="s">
-        <v>5721</v>
+        <v>1897</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>175</v>
@@ -35007,7 +35190,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="38" t="s">
-        <v>5722</v>
+        <v>5721</v>
       </c>
       <c r="B40" s="38" t="s">
         <v>175</v>
@@ -35018,7 +35201,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="38" t="s">
-        <v>5723</v>
+        <v>5722</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>175</v>
@@ -35029,7 +35212,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="38" t="s">
-        <v>5724</v>
+        <v>5723</v>
       </c>
       <c r="B42" s="38" t="s">
         <v>175</v>
@@ -35040,7 +35223,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="38" t="s">
-        <v>5725</v>
+        <v>5724</v>
       </c>
       <c r="B43" s="38" t="s">
         <v>175</v>
@@ -35051,7 +35234,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="38" t="s">
-        <v>5726</v>
+        <v>5725</v>
       </c>
       <c r="B44" s="38" t="s">
         <v>175</v>
@@ -35062,7 +35245,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="38" t="s">
-        <v>5727</v>
+        <v>5726</v>
       </c>
       <c r="B45" s="38" t="s">
         <v>175</v>
@@ -35073,7 +35256,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="38" t="s">
-        <v>5728</v>
+        <v>5727</v>
       </c>
       <c r="B46" s="38" t="s">
         <v>175</v>
@@ -35084,7 +35267,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="38" t="s">
-        <v>5729</v>
+        <v>5728</v>
       </c>
       <c r="B47" s="38" t="s">
         <v>175</v>
@@ -35095,7 +35278,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="38" t="s">
-        <v>5730</v>
+        <v>5729</v>
       </c>
       <c r="B48" s="38" t="s">
         <v>175</v>
@@ -35106,18 +35289,18 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="38" t="s">
-        <v>5702</v>
+        <v>5730</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C49" s="38" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="38" t="s">
-        <v>5703</v>
+        <v>5702</v>
       </c>
       <c r="B50" s="38" t="s">
         <v>171</v>
@@ -35128,7 +35311,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="38" t="s">
-        <v>5687</v>
+        <v>5703</v>
       </c>
       <c r="B51" s="38" t="s">
         <v>171</v>
@@ -35139,7 +35322,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="38" t="s">
-        <v>5704</v>
+        <v>5687</v>
       </c>
       <c r="B52" s="38" t="s">
         <v>171</v>
@@ -35150,7 +35333,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="38" t="s">
-        <v>171</v>
+        <v>5704</v>
       </c>
       <c r="B53" s="38" t="s">
         <v>171</v>
@@ -35161,7 +35344,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="38" t="s">
-        <v>5731</v>
+        <v>171</v>
       </c>
       <c r="B54" s="38" t="s">
         <v>171</v>
@@ -35172,7 +35355,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="38" t="s">
-        <v>5732</v>
+        <v>5731</v>
       </c>
       <c r="B55" s="38" t="s">
         <v>171</v>
@@ -35183,7 +35366,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="38" t="s">
-        <v>1832</v>
+        <v>5732</v>
       </c>
       <c r="B56" s="38" t="s">
         <v>171</v>
@@ -35194,7 +35377,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="38" t="s">
-        <v>5733</v>
+        <v>1832</v>
       </c>
       <c r="B57" s="38" t="s">
         <v>171</v>
@@ -35205,18 +35388,18 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="38" t="s">
-        <v>5734</v>
+        <v>5733</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="38" t="s">
-        <v>5735</v>
+        <v>5734</v>
       </c>
       <c r="B59" s="38" t="s">
         <v>177</v>
@@ -35227,7 +35410,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="38" t="s">
-        <v>5736</v>
+        <v>5735</v>
       </c>
       <c r="B60" s="38" t="s">
         <v>177</v>
@@ -35238,7 +35421,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="38" t="s">
-        <v>5737</v>
+        <v>5736</v>
       </c>
       <c r="B61" s="38" t="s">
         <v>177</v>
@@ -35249,7 +35432,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="38" t="s">
-        <v>5738</v>
+        <v>5737</v>
       </c>
       <c r="B62" s="38" t="s">
         <v>177</v>
@@ -35260,7 +35443,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="38" t="s">
-        <v>5739</v>
+        <v>5738</v>
       </c>
       <c r="B63" s="38" t="s">
         <v>177</v>
@@ -35271,7 +35454,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="38" t="s">
-        <v>5740</v>
+        <v>5739</v>
       </c>
       <c r="B64" s="38" t="s">
         <v>177</v>
@@ -35282,7 +35465,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="38" t="s">
-        <v>5741</v>
+        <v>5740</v>
       </c>
       <c r="B65" s="38" t="s">
         <v>177</v>
@@ -35293,7 +35476,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="38" t="s">
-        <v>5742</v>
+        <v>5741</v>
       </c>
       <c r="B66" s="38" t="s">
         <v>177</v>
@@ -35304,7 +35487,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="38" t="s">
-        <v>5743</v>
+        <v>5742</v>
       </c>
       <c r="B67" s="38" t="s">
         <v>177</v>
@@ -35315,7 +35498,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="38" t="s">
-        <v>5744</v>
+        <v>5743</v>
       </c>
       <c r="B68" s="38" t="s">
         <v>177</v>
@@ -35326,18 +35509,18 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="38" t="s">
-        <v>5745</v>
+        <v>5744</v>
       </c>
       <c r="B69" s="38" t="s">
-        <v>5746</v>
+        <v>177</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="38" t="s">
-        <v>5709</v>
+        <v>5745</v>
       </c>
       <c r="B70" s="38" t="s">
         <v>5746</v>
@@ -35348,7 +35531,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="38" t="s">
-        <v>5710</v>
+        <v>5709</v>
       </c>
       <c r="B71" s="38" t="s">
         <v>5746</v>
@@ -35359,18 +35542,18 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="38" t="s">
-        <v>5747</v>
+        <v>5710</v>
       </c>
       <c r="B72" s="38" t="s">
-        <v>178</v>
+        <v>5746</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="38" t="s">
-        <v>5748</v>
+        <v>5747</v>
       </c>
       <c r="B73" s="38" t="s">
         <v>178</v>
@@ -35381,7 +35564,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="38" t="s">
-        <v>5749</v>
+        <v>5748</v>
       </c>
       <c r="B74" s="38" t="s">
         <v>178</v>
@@ -35392,7 +35575,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="38" t="s">
-        <v>5750</v>
+        <v>5749</v>
       </c>
       <c r="B75" s="38" t="s">
         <v>178</v>
@@ -35403,7 +35586,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="38" t="s">
-        <v>5751</v>
+        <v>5750</v>
       </c>
       <c r="B76" s="38" t="s">
         <v>178</v>
@@ -35414,7 +35597,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="38" t="s">
-        <v>5752</v>
+        <v>5751</v>
       </c>
       <c r="B77" s="38" t="s">
         <v>178</v>
@@ -35425,7 +35608,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="38" t="s">
-        <v>178</v>
+        <v>5752</v>
       </c>
       <c r="B78" s="38" t="s">
         <v>178</v>
@@ -35436,7 +35619,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="38" t="s">
-        <v>5753</v>
+        <v>178</v>
       </c>
       <c r="B79" s="38" t="s">
         <v>178</v>
@@ -35447,7 +35630,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="38" t="s">
-        <v>1673</v>
+        <v>5753</v>
       </c>
       <c r="B80" s="38" t="s">
         <v>178</v>
@@ -35458,7 +35641,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="38" t="s">
-        <v>5754</v>
+        <v>1673</v>
       </c>
       <c r="B81" s="38" t="s">
         <v>178</v>
@@ -35469,7 +35652,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="38" t="s">
-        <v>5755</v>
+        <v>5754</v>
       </c>
       <c r="B82" s="38" t="s">
         <v>178</v>
@@ -35480,7 +35663,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="38" t="s">
-        <v>5756</v>
+        <v>5755</v>
       </c>
       <c r="B83" s="38" t="s">
         <v>178</v>
@@ -35491,7 +35674,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="38" t="s">
-        <v>1677</v>
+        <v>5756</v>
       </c>
       <c r="B84" s="38" t="s">
         <v>178</v>
@@ -35502,7 +35685,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="38" t="s">
-        <v>5757</v>
+        <v>1677</v>
       </c>
       <c r="B85" s="38" t="s">
         <v>178</v>
@@ -35513,18 +35696,18 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="38" t="s">
-        <v>5758</v>
+        <v>5757</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>5759</v>
+        <v>178</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>5759</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="38" t="s">
-        <v>5760</v>
+        <v>5758</v>
       </c>
       <c r="B87" s="38" t="s">
         <v>5759</v>
@@ -35535,7 +35718,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="38" t="s">
-        <v>5761</v>
+        <v>5760</v>
       </c>
       <c r="B88" s="38" t="s">
         <v>5759</v>
@@ -35546,7 +35729,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="38" t="s">
-        <v>5762</v>
+        <v>5761</v>
       </c>
       <c r="B89" s="38" t="s">
         <v>5759</v>
@@ -35557,7 +35740,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="38" t="s">
-        <v>5763</v>
+        <v>5762</v>
       </c>
       <c r="B90" s="38" t="s">
         <v>5759</v>
@@ -35568,7 +35751,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="38" t="s">
-        <v>5764</v>
+        <v>5763</v>
       </c>
       <c r="B91" s="38" t="s">
         <v>5759</v>
@@ -35579,7 +35762,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="38" t="s">
-        <v>5765</v>
+        <v>5764</v>
       </c>
       <c r="B92" s="38" t="s">
         <v>5759</v>
@@ -35590,7 +35773,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="38" t="s">
-        <v>5766</v>
+        <v>5765</v>
       </c>
       <c r="B93" s="38" t="s">
         <v>5759</v>
@@ -35601,7 +35784,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="38" t="s">
-        <v>5767</v>
+        <v>5766</v>
       </c>
       <c r="B94" s="38" t="s">
         <v>5759</v>
@@ -35612,7 +35795,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="38" t="s">
-        <v>5768</v>
+        <v>5767</v>
       </c>
       <c r="B95" s="38" t="s">
         <v>5759</v>
@@ -35623,7 +35806,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="38" t="s">
-        <v>5769</v>
+        <v>5768</v>
       </c>
       <c r="B96" s="38" t="s">
         <v>5759</v>
@@ -35634,7 +35817,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="38" t="s">
-        <v>5770</v>
+        <v>5769</v>
       </c>
       <c r="B97" s="38" t="s">
         <v>5759</v>
@@ -35645,7 +35828,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="38" t="s">
-        <v>5771</v>
+        <v>5770</v>
       </c>
       <c r="B98" s="38" t="s">
         <v>5759</v>
@@ -35656,7 +35839,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="38" t="s">
-        <v>5772</v>
+        <v>5771</v>
       </c>
       <c r="B99" s="38" t="s">
         <v>5759</v>
@@ -35667,7 +35850,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="38" t="s">
-        <v>5773</v>
+        <v>5772</v>
       </c>
       <c r="B100" s="38" t="s">
         <v>5759</v>
@@ -35678,7 +35861,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="38" t="s">
-        <v>5774</v>
+        <v>5773</v>
       </c>
       <c r="B101" s="38" t="s">
         <v>5759</v>
@@ -35689,7 +35872,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="38" t="s">
-        <v>5775</v>
+        <v>5774</v>
       </c>
       <c r="B102" s="38" t="s">
         <v>5759</v>
@@ -35700,7 +35883,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="38" t="s">
-        <v>5776</v>
+        <v>5775</v>
       </c>
       <c r="B103" s="38" t="s">
         <v>5759</v>
@@ -35711,7 +35894,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="38" t="s">
-        <v>5777</v>
+        <v>5776</v>
       </c>
       <c r="B104" s="38" t="s">
         <v>5759</v>
@@ -35722,7 +35905,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="38" t="s">
-        <v>5778</v>
+        <v>5777</v>
       </c>
       <c r="B105" s="38" t="s">
         <v>5759</v>
@@ -35733,18 +35916,18 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="38" t="s">
-        <v>5779</v>
+        <v>5778</v>
       </c>
       <c r="B106" s="38" t="s">
-        <v>5780</v>
+        <v>5759</v>
       </c>
       <c r="C106" s="38" t="s">
-        <v>181</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="38" t="s">
-        <v>5781</v>
+        <v>5779</v>
       </c>
       <c r="B107" s="38" t="s">
         <v>5780</v>
@@ -35755,7 +35938,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="38" t="s">
-        <v>5782</v>
+        <v>5781</v>
       </c>
       <c r="B108" s="38" t="s">
         <v>5780</v>
@@ -35766,7 +35949,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="38" t="s">
-        <v>1831</v>
+        <v>5782</v>
       </c>
       <c r="B109" s="38" t="s">
         <v>5780</v>
@@ -35777,29 +35960,29 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="38" t="s">
-        <v>5783</v>
+        <v>1831</v>
       </c>
       <c r="B110" s="38" t="s">
-        <v>182</v>
+        <v>5780</v>
       </c>
       <c r="C110" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="38" t="s">
-        <v>5687</v>
+        <v>5783</v>
       </c>
       <c r="B111" s="38" t="s">
-        <v>5784</v>
+        <v>182</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="38" t="s">
-        <v>5704</v>
+        <v>5687</v>
       </c>
       <c r="B112" s="38" t="s">
         <v>5784</v>
@@ -35810,7 +35993,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="38" t="s">
-        <v>5785</v>
+        <v>5704</v>
       </c>
       <c r="B113" s="38" t="s">
         <v>5784</v>
@@ -35821,18 +36004,18 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="38" t="s">
-        <v>5786</v>
+        <v>5785</v>
       </c>
       <c r="B114" s="38" t="s">
-        <v>185</v>
+        <v>5784</v>
       </c>
       <c r="C114" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="38" t="s">
-        <v>5707</v>
+        <v>5786</v>
       </c>
       <c r="B115" s="38" t="s">
         <v>185</v>
@@ -35843,7 +36026,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="38" t="s">
-        <v>5711</v>
+        <v>5707</v>
       </c>
       <c r="B116" s="38" t="s">
         <v>185</v>
@@ -35854,7 +36037,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="38" t="s">
-        <v>5712</v>
+        <v>5711</v>
       </c>
       <c r="B117" s="38" t="s">
         <v>185</v>
@@ -35865,7 +36048,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="38" t="s">
-        <v>5713</v>
+        <v>5712</v>
       </c>
       <c r="B118" s="38" t="s">
         <v>185</v>
@@ -35876,7 +36059,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="38" t="s">
-        <v>5787</v>
+        <v>5713</v>
       </c>
       <c r="B119" s="38" t="s">
         <v>185</v>
@@ -35887,7 +36070,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="38" t="s">
-        <v>5788</v>
+        <v>5787</v>
       </c>
       <c r="B120" s="38" t="s">
         <v>185</v>
@@ -35898,7 +36081,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="38" t="s">
-        <v>5789</v>
+        <v>5788</v>
       </c>
       <c r="B121" s="38" t="s">
         <v>185</v>
@@ -35909,7 +36092,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="38" t="s">
-        <v>5790</v>
+        <v>5789</v>
       </c>
       <c r="B122" s="38" t="s">
         <v>185</v>
@@ -35920,7 +36103,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="38" t="s">
-        <v>5791</v>
+        <v>5790</v>
       </c>
       <c r="B123" s="38" t="s">
         <v>185</v>
@@ -35931,7 +36114,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="38" t="s">
-        <v>5792</v>
+        <v>5791</v>
       </c>
       <c r="B124" s="38" t="s">
         <v>185</v>
@@ -35942,7 +36125,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="38" t="s">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="B125" s="38" t="s">
         <v>185</v>
@@ -35953,7 +36136,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="38" t="s">
-        <v>5794</v>
+        <v>5793</v>
       </c>
       <c r="B126" s="38" t="s">
         <v>185</v>
@@ -35964,7 +36147,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="38" t="s">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="B127" s="38" t="s">
         <v>185</v>
@@ -35975,7 +36158,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="38" t="s">
-        <v>5796</v>
+        <v>5795</v>
       </c>
       <c r="B128" s="38" t="s">
         <v>185</v>
@@ -35986,7 +36169,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="38" t="s">
-        <v>5797</v>
+        <v>5796</v>
       </c>
       <c r="B129" s="38" t="s">
         <v>185</v>
@@ -35997,7 +36180,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="38" t="s">
-        <v>5798</v>
+        <v>5797</v>
       </c>
       <c r="B130" s="38" t="s">
         <v>185</v>
@@ -36008,7 +36191,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="38" t="s">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="B131" s="38" t="s">
         <v>185</v>
@@ -36019,7 +36202,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="38" t="s">
-        <v>5800</v>
+        <v>5799</v>
       </c>
       <c r="B132" s="38" t="s">
         <v>185</v>
@@ -36030,7 +36213,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="38" t="s">
-        <v>5801</v>
+        <v>5800</v>
       </c>
       <c r="B133" s="38" t="s">
         <v>185</v>
@@ -36041,7 +36224,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="38" t="s">
-        <v>5802</v>
+        <v>5801</v>
       </c>
       <c r="B134" s="38" t="s">
         <v>185</v>
@@ -36052,7 +36235,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="38" t="s">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="B135" s="38" t="s">
         <v>185</v>
@@ -36063,7 +36246,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="38" t="s">
-        <v>5804</v>
+        <v>5803</v>
       </c>
       <c r="B136" s="38" t="s">
         <v>185</v>
@@ -36074,7 +36257,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="38" t="s">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="B137" s="38" t="s">
         <v>185</v>
@@ -36085,7 +36268,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="38" t="s">
-        <v>5806</v>
+        <v>5805</v>
       </c>
       <c r="B138" s="38" t="s">
         <v>185</v>
@@ -36096,7 +36279,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="38" t="s">
-        <v>5721</v>
+        <v>5806</v>
       </c>
       <c r="B139" s="38" t="s">
         <v>185</v>
@@ -36107,7 +36290,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="38" t="s">
-        <v>5807</v>
+        <v>5721</v>
       </c>
       <c r="B140" s="38" t="s">
         <v>185</v>
@@ -36118,7 +36301,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="38" t="s">
-        <v>5722</v>
+        <v>5807</v>
       </c>
       <c r="B141" s="38" t="s">
         <v>185</v>
@@ -36129,7 +36312,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="38" t="s">
-        <v>5808</v>
+        <v>5722</v>
       </c>
       <c r="B142" s="38" t="s">
         <v>185</v>
@@ -36140,7 +36323,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="38" t="s">
-        <v>5809</v>
+        <v>5808</v>
       </c>
       <c r="B143" s="38" t="s">
         <v>185</v>
@@ -36151,7 +36334,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="38" t="s">
-        <v>5810</v>
+        <v>5809</v>
       </c>
       <c r="B144" s="38" t="s">
         <v>185</v>
@@ -36162,7 +36345,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="38" t="s">
-        <v>5811</v>
+        <v>5810</v>
       </c>
       <c r="B145" s="38" t="s">
         <v>185</v>
@@ -36173,7 +36356,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="38" t="s">
-        <v>5812</v>
+        <v>5811</v>
       </c>
       <c r="B146" s="38" t="s">
         <v>185</v>
@@ -36184,7 +36367,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="38" t="s">
-        <v>5813</v>
+        <v>5812</v>
       </c>
       <c r="B147" s="38" t="s">
         <v>185</v>
@@ -36195,7 +36378,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="38" t="s">
-        <v>5814</v>
+        <v>5813</v>
       </c>
       <c r="B148" s="38" t="s">
         <v>185</v>
@@ -36206,7 +36389,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="38" t="s">
-        <v>5815</v>
+        <v>5814</v>
       </c>
       <c r="B149" s="38" t="s">
         <v>185</v>
@@ -36217,7 +36400,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="38" t="s">
-        <v>5816</v>
+        <v>5815</v>
       </c>
       <c r="B150" s="38" t="s">
         <v>185</v>
@@ -36228,7 +36411,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="38" t="s">
-        <v>5817</v>
+        <v>5816</v>
       </c>
       <c r="B151" s="38" t="s">
         <v>185</v>
@@ -36239,7 +36422,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="38" t="s">
-        <v>5818</v>
+        <v>5817</v>
       </c>
       <c r="B152" s="38" t="s">
         <v>185</v>
@@ -36250,7 +36433,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="38" t="s">
-        <v>5819</v>
+        <v>5818</v>
       </c>
       <c r="B153" s="38" t="s">
         <v>185</v>
@@ -36261,7 +36444,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="38" t="s">
-        <v>5820</v>
+        <v>5819</v>
       </c>
       <c r="B154" s="38" t="s">
         <v>185</v>
@@ -36272,7 +36455,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="38" t="s">
-        <v>5821</v>
+        <v>5820</v>
       </c>
       <c r="B155" s="38" t="s">
         <v>185</v>
@@ -36283,7 +36466,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="38" t="s">
-        <v>5822</v>
+        <v>5821</v>
       </c>
       <c r="B156" s="38" t="s">
         <v>185</v>
@@ -36294,7 +36477,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="38" t="s">
-        <v>5823</v>
+        <v>5822</v>
       </c>
       <c r="B157" s="38" t="s">
         <v>185</v>
@@ -36305,7 +36488,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="38" t="s">
-        <v>5824</v>
+        <v>5823</v>
       </c>
       <c r="B158" s="38" t="s">
         <v>185</v>
@@ -36316,7 +36499,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="38" t="s">
-        <v>5825</v>
+        <v>5824</v>
       </c>
       <c r="B159" s="38" t="s">
         <v>185</v>
@@ -36327,7 +36510,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="38" t="s">
-        <v>5826</v>
+        <v>5825</v>
       </c>
       <c r="B160" s="38" t="s">
         <v>185</v>
@@ -36338,7 +36521,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="38" t="s">
-        <v>5827</v>
+        <v>5826</v>
       </c>
       <c r="B161" s="38" t="s">
         <v>185</v>
@@ -36349,7 +36532,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="38" t="s">
-        <v>5828</v>
+        <v>5827</v>
       </c>
       <c r="B162" s="38" t="s">
         <v>185</v>
@@ -36360,7 +36543,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="38" t="s">
-        <v>5829</v>
+        <v>5828</v>
       </c>
       <c r="B163" s="38" t="s">
         <v>185</v>
@@ -36371,7 +36554,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="38" t="s">
-        <v>5830</v>
+        <v>5829</v>
       </c>
       <c r="B164" s="38" t="s">
         <v>185</v>
@@ -36382,7 +36565,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="38" t="s">
-        <v>5831</v>
+        <v>5830</v>
       </c>
       <c r="B165" s="38" t="s">
         <v>185</v>
@@ -36393,7 +36576,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="38" t="s">
-        <v>5832</v>
+        <v>5831</v>
       </c>
       <c r="B166" s="38" t="s">
         <v>185</v>
@@ -36404,7 +36587,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="38" t="s">
-        <v>5833</v>
+        <v>5832</v>
       </c>
       <c r="B167" s="38" t="s">
         <v>185</v>
@@ -36415,7 +36598,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="38" t="s">
-        <v>5834</v>
+        <v>5833</v>
       </c>
       <c r="B168" s="38" t="s">
         <v>185</v>
@@ -36426,7 +36609,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="38" t="s">
-        <v>5835</v>
+        <v>5834</v>
       </c>
       <c r="B169" s="38" t="s">
         <v>185</v>
@@ -36437,7 +36620,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="38" t="s">
-        <v>5836</v>
+        <v>5835</v>
       </c>
       <c r="B170" s="38" t="s">
         <v>185</v>
@@ -36448,7 +36631,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="38" t="s">
-        <v>5837</v>
+        <v>5836</v>
       </c>
       <c r="B171" s="38" t="s">
         <v>185</v>
@@ -36459,7 +36642,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="38" t="s">
-        <v>5838</v>
+        <v>5837</v>
       </c>
       <c r="B172" s="38" t="s">
         <v>185</v>
@@ -36470,18 +36653,18 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="38" t="s">
-        <v>5839</v>
+        <v>5838</v>
       </c>
       <c r="B173" s="38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C173" s="38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="38" t="s">
-        <v>5709</v>
+        <v>5839</v>
       </c>
       <c r="B174" s="38" t="s">
         <v>186</v>
@@ -36492,7 +36675,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" s="38" t="s">
-        <v>5710</v>
+        <v>5709</v>
       </c>
       <c r="B175" s="38" t="s">
         <v>186</v>
@@ -36503,18 +36686,18 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" s="38" t="s">
-        <v>5705</v>
+        <v>5710</v>
       </c>
       <c r="B176" s="38" t="s">
-        <v>1238</v>
+        <v>186</v>
       </c>
       <c r="C176" s="38" t="s">
-        <v>1238</v>
+        <v>186</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" s="38" t="s">
-        <v>5706</v>
+        <v>5705</v>
       </c>
       <c r="B177" s="38" t="s">
         <v>1238</v>
@@ -36525,7 +36708,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" s="38" t="s">
-        <v>5840</v>
+        <v>5706</v>
       </c>
       <c r="B178" s="38" t="s">
         <v>1238</v>
@@ -36536,7 +36719,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="38" t="s">
-        <v>5841</v>
+        <v>5840</v>
       </c>
       <c r="B179" s="38" t="s">
         <v>1238</v>
@@ -36547,7 +36730,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" s="38" t="s">
-        <v>5839</v>
+        <v>5841</v>
       </c>
       <c r="B180" s="38" t="s">
         <v>1238</v>
@@ -36558,7 +36741,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" s="38" t="s">
-        <v>5842</v>
+        <v>5839</v>
       </c>
       <c r="B181" s="38" t="s">
         <v>1238</v>
@@ -36569,7 +36752,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="38" t="s">
-        <v>5843</v>
+        <v>5842</v>
       </c>
       <c r="B182" s="38" t="s">
         <v>1238</v>
@@ -36580,7 +36763,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" s="38" t="s">
-        <v>5717</v>
+        <v>5843</v>
       </c>
       <c r="B183" s="38" t="s">
         <v>1238</v>
@@ -36591,7 +36774,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" s="38" t="s">
-        <v>5844</v>
+        <v>5717</v>
       </c>
       <c r="B184" s="38" t="s">
         <v>1238</v>
@@ -36602,18 +36785,18 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" s="38" t="s">
-        <v>5745</v>
+        <v>5844</v>
       </c>
       <c r="B185" s="38" t="s">
-        <v>5845</v>
+        <v>1238</v>
       </c>
       <c r="C185" s="38" t="s">
-        <v>169</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" s="38" t="s">
-        <v>5708</v>
+        <v>5745</v>
       </c>
       <c r="B186" s="38" t="s">
         <v>5845</v>
@@ -36624,7 +36807,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" s="38" t="s">
-        <v>5717</v>
+        <v>5708</v>
       </c>
       <c r="B187" s="38" t="s">
         <v>5845</v>
@@ -36635,7 +36818,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" s="38" t="s">
-        <v>5846</v>
+        <v>5717</v>
       </c>
       <c r="B188" s="38" t="s">
         <v>5845</v>
@@ -36646,7 +36829,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" s="38" t="s">
-        <v>5731</v>
+        <v>5846</v>
       </c>
       <c r="B189" s="38" t="s">
         <v>5845</v>
@@ -36657,7 +36840,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" s="38" t="s">
-        <v>5732</v>
+        <v>5731</v>
       </c>
       <c r="B190" s="38" t="s">
         <v>5845</v>
@@ -36668,13 +36851,805 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" s="38" t="s">
-        <v>5847</v>
+        <v>5732</v>
       </c>
       <c r="B191" s="38" t="s">
+        <v>5845</v>
+      </c>
+      <c r="C191" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" s="51" t="s">
+        <v>5859</v>
+      </c>
+      <c r="B192" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C192" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" s="51" t="s">
+        <v>5859</v>
+      </c>
+      <c r="B193" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C193" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" s="51" t="s">
+        <v>5860</v>
+      </c>
+      <c r="B194" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C194" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" s="51" t="s">
+        <v>5861</v>
+      </c>
+      <c r="B195" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C195" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A196" s="51" t="s">
+        <v>5862</v>
+      </c>
+      <c r="B196" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C196" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A197" s="51" t="s">
+        <v>5863</v>
+      </c>
+      <c r="B197" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C197" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A198" s="51" t="s">
+        <v>5864</v>
+      </c>
+      <c r="B198" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C198" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A199" s="51" t="s">
+        <v>5865</v>
+      </c>
+      <c r="B199" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C199" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A200" s="51" t="s">
+        <v>5866</v>
+      </c>
+      <c r="B200" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C200" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A201" s="51" t="s">
+        <v>5867</v>
+      </c>
+      <c r="B201" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C201" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A202" s="51" t="s">
+        <v>5867</v>
+      </c>
+      <c r="B202" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C202" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A203" s="51" t="s">
+        <v>5868</v>
+      </c>
+      <c r="B203" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C203" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A204" s="51" t="s">
+        <v>5869</v>
+      </c>
+      <c r="B204" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C204" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A205" s="51" t="s">
+        <v>5869</v>
+      </c>
+      <c r="B205" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C205" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A206" s="51" t="s">
+        <v>5870</v>
+      </c>
+      <c r="B206" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C206" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A207" s="51" t="s">
+        <v>5871</v>
+      </c>
+      <c r="B207" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C207" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A208" s="51" t="s">
+        <v>5872</v>
+      </c>
+      <c r="B208" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C208" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A209" s="51" t="s">
+        <v>5873</v>
+      </c>
+      <c r="B209" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C209" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A210" s="51" t="s">
+        <v>5874</v>
+      </c>
+      <c r="B210" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C210" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A211" s="51" t="s">
+        <v>5875</v>
+      </c>
+      <c r="B211" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C211" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A212" s="51" t="s">
+        <v>5875</v>
+      </c>
+      <c r="B212" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C212" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A213" s="51" t="s">
+        <v>5876</v>
+      </c>
+      <c r="B213" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C213" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A214" s="51" t="s">
+        <v>5876</v>
+      </c>
+      <c r="B214" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C214" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A215" s="51" t="s">
+        <v>5877</v>
+      </c>
+      <c r="B215" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C215" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A216" s="51" t="s">
+        <v>5877</v>
+      </c>
+      <c r="B216" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C216" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A217" s="51" t="s">
+        <v>5878</v>
+      </c>
+      <c r="B217" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C217" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A218" s="51" t="s">
+        <v>5878</v>
+      </c>
+      <c r="B218" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C218" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A219" s="51" t="s">
+        <v>5879</v>
+      </c>
+      <c r="B219" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C219" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A220" s="51" t="s">
+        <v>5880</v>
+      </c>
+      <c r="B220" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C220" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" s="51" t="s">
+        <v>5881</v>
+      </c>
+      <c r="B221" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C221" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" s="51" t="s">
+        <v>5882</v>
+      </c>
+      <c r="B222" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C222" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" s="51" t="s">
+        <v>5883</v>
+      </c>
+      <c r="B223" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C223" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" s="51" t="s">
+        <v>5883</v>
+      </c>
+      <c r="B224" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C224" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" s="51" t="s">
+        <v>5884</v>
+      </c>
+      <c r="B225" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C225" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" s="51" t="s">
+        <v>5885</v>
+      </c>
+      <c r="B226" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C226" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A227" s="51" t="s">
+        <v>5886</v>
+      </c>
+      <c r="B227" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C227" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" s="51" t="s">
+        <v>5887</v>
+      </c>
+      <c r="B228" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C228" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" s="51" t="s">
+        <v>5888</v>
+      </c>
+      <c r="B229" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C229" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A230" s="51" t="s">
+        <v>5888</v>
+      </c>
+      <c r="B230" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="C191" s="38" t="s">
+      <c r="C230" s="38" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A231" s="51" t="s">
+        <v>5889</v>
+      </c>
+      <c r="B231" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C231" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A232" s="51" t="s">
+        <v>5890</v>
+      </c>
+      <c r="B232" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C232" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A233" s="51" t="s">
+        <v>5891</v>
+      </c>
+      <c r="B233" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C233" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A234" s="51" t="s">
+        <v>5892</v>
+      </c>
+      <c r="B234" s="38" t="s">
+        <v>5759</v>
+      </c>
+      <c r="C234" s="38" t="s">
+        <v>5759</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A235" s="51" t="s">
+        <v>5893</v>
+      </c>
+      <c r="B235" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C235" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A236" s="51" t="s">
+        <v>5894</v>
+      </c>
+      <c r="B236" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C236" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A237" s="51" t="s">
+        <v>5895</v>
+      </c>
+      <c r="B237" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C237" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A238" s="51" t="s">
+        <v>5896</v>
+      </c>
+      <c r="B238" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C238" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A239" s="51" t="s">
+        <v>5897</v>
+      </c>
+      <c r="B239" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="C239" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A240" s="51" t="s">
+        <v>5898</v>
+      </c>
+      <c r="B240" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C240" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A241" s="51" t="s">
+        <v>5898</v>
+      </c>
+      <c r="B241" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C241" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A242" s="51" t="s">
+        <v>5899</v>
+      </c>
+      <c r="B242" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C242" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A243" s="51" t="s">
+        <v>5900</v>
+      </c>
+      <c r="B243" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C243" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A244" s="51" t="s">
+        <v>5901</v>
+      </c>
+      <c r="B244" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C244" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A245" s="51" t="s">
+        <v>5902</v>
+      </c>
+      <c r="B245" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C245" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A246" s="51" t="s">
+        <v>5903</v>
+      </c>
+      <c r="B246" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C246" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A247" s="51" t="s">
+        <v>5904</v>
+      </c>
+      <c r="B247" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C247" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A248" s="51" t="s">
+        <v>5905</v>
+      </c>
+      <c r="B248" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C248" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A249" s="51" t="s">
+        <v>5906</v>
+      </c>
+      <c r="B249" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C249" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A250" s="51" t="s">
+        <v>5907</v>
+      </c>
+      <c r="B250" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C250" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A251" s="51" t="s">
+        <v>5908</v>
+      </c>
+      <c r="B251" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C251" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A252" s="51" t="s">
+        <v>5909</v>
+      </c>
+      <c r="B252" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C252" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A253" s="51" t="s">
+        <v>5910</v>
+      </c>
+      <c r="B253" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C253" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A254" s="51" t="s">
+        <v>5911</v>
+      </c>
+      <c r="B254" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C254" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A255" s="51" t="s">
+        <v>5912</v>
+      </c>
+      <c r="B255" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C255" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A256" s="51" t="s">
+        <v>5913</v>
+      </c>
+      <c r="B256" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C256" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A257" s="51" t="s">
+        <v>5913</v>
+      </c>
+      <c r="B257" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C257" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A258" s="51" t="s">
+        <v>5914</v>
+      </c>
+      <c r="B258" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C258" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A259" s="51" t="s">
+        <v>5915</v>
+      </c>
+      <c r="B259" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="C259" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A260" s="51" t="s">
+        <v>5915</v>
+      </c>
+      <c r="B260" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C260" s="38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A261" s="51" t="s">
+        <v>5916</v>
+      </c>
+      <c r="B261" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C261" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A262" s="51" t="s">
+        <v>5917</v>
+      </c>
+      <c r="B262" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C262" s="38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A263" s="51" t="s">
+        <v>5918</v>
+      </c>
+      <c r="B263" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="C263" s="38" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subjects for ontario tbs data update
added new tags to ontario subject table for tbs
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2510" yWindow="4680" windowWidth="11810" windowHeight="3020" tabRatio="883" firstSheet="26" activeTab="28"/>
+    <workbookView xWindow="2510" yWindow="4680" windowWidth="11810" windowHeight="3020" tabRatio="883" firstSheet="47" activeTab="52"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12651" uniqueCount="5919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12797" uniqueCount="5919">
   <si>
     <t>default_key</t>
   </si>
@@ -34747,8 +34747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C263"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C187" sqref="C187"/>
+    <sheetView topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="A192" sqref="A192:C263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47388,15 +47388,15 @@
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B274"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" style="38" customWidth="1"/>
+    <col min="1" max="1" width="39.7265625" style="38" customWidth="1"/>
     <col min="2" max="2" width="22.54296875" style="38" customWidth="1"/>
     <col min="3" max="16384" width="8.7265625" style="38"/>
   </cols>
@@ -47411,7 +47411,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
-        <v>5783</v>
+        <v>5847</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>1241</v>
@@ -47419,34 +47419,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
-        <v>5734</v>
+        <v>5783</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>1236</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
-        <v>5688</v>
+        <v>5734</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>1248</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
-        <v>5760</v>
+        <v>5688</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>5759</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="s">
-        <v>5787</v>
+        <v>5760</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>5854</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -47454,55 +47454,55 @@
         <v>5787</v>
       </c>
       <c r="B7" s="38" t="s">
-        <v>1241</v>
+        <v>5854</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="38" t="s">
-        <v>5735</v>
+        <v>5787</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>1236</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
-        <v>5714</v>
+        <v>5735</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>1250</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="38" t="s">
-        <v>5689</v>
+        <v>5714</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="38" t="s">
-        <v>5715</v>
+        <v>5689</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="38" t="s">
-        <v>5690</v>
+        <v>5715</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
-        <v>5788</v>
+        <v>5690</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>1241</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -47510,47 +47510,47 @@
         <v>5788</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
-        <v>5842</v>
+        <v>5788</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>1238</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
-        <v>5747</v>
+        <v>5842</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>1254</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="38" t="s">
-        <v>5789</v>
+        <v>5747</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>1241</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="38" t="s">
-        <v>5790</v>
+        <v>5789</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>1248</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="38" t="s">
-        <v>5791</v>
+        <v>5790</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>1241</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -47558,36 +47558,36 @@
         <v>5791</v>
       </c>
       <c r="B20" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="38" t="s">
-        <v>5843</v>
+        <v>5791</v>
       </c>
       <c r="B21" s="38" t="s">
-        <v>1238</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="38" t="s">
-        <v>5748</v>
+        <v>5843</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>1254</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="38" t="s">
-        <v>5792</v>
+        <v>5748</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>1239</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="38" t="s">
-        <v>5793</v>
+        <v>5792</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>1239</v>
@@ -47595,23 +47595,23 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="38" t="s">
-        <v>5701</v>
+        <v>5793</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>1250</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="38" t="s">
-        <v>5749</v>
+        <v>5701</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="38" t="s">
-        <v>5750</v>
+        <v>5749</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>1254</v>
@@ -47619,7 +47619,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="38" t="s">
-        <v>5751</v>
+        <v>5750</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>1254</v>
@@ -47627,10 +47627,10 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="38" t="s">
-        <v>5716</v>
+        <v>5751</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>1250</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -47638,15 +47638,15 @@
         <v>5716</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="38" t="s">
-        <v>5794</v>
+        <v>5716</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>5854</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -47654,15 +47654,15 @@
         <v>5794</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>1241</v>
+        <v>5854</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="38" t="s">
-        <v>5795</v>
+        <v>5794</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>5854</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -47670,84 +47670,84 @@
         <v>5795</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>1241</v>
+        <v>5854</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="38" t="s">
-        <v>5736</v>
+        <v>5795</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>1236</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="38" t="s">
-        <v>5691</v>
+        <v>5736</v>
       </c>
       <c r="B36" s="38" t="s">
-        <v>1248</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="38" t="s">
-        <v>5752</v>
+        <v>5691</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="38" t="s">
-        <v>5796</v>
+        <v>5752</v>
       </c>
       <c r="B38" s="38" t="s">
-        <v>1239</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="38" t="s">
-        <v>5717</v>
+        <v>5796</v>
       </c>
       <c r="B39" s="38" t="s">
-        <v>1250</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="38" t="s">
-        <v>5761</v>
+        <v>5717</v>
       </c>
       <c r="B40" s="38" t="s">
-        <v>5759</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="38" t="s">
-        <v>5844</v>
+        <v>5761</v>
       </c>
       <c r="B41" s="38" t="s">
-        <v>1238</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="38" t="s">
-        <v>5797</v>
+        <v>5844</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>1245</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="38" t="s">
-        <v>5718</v>
+        <v>5797</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>1250</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="38" t="s">
-        <v>5719</v>
+        <v>5718</v>
       </c>
       <c r="B44" s="38" t="s">
         <v>1250</v>
@@ -47755,15 +47755,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="38" t="s">
-        <v>5798</v>
+        <v>5719</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>1245</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="38" t="s">
-        <v>5799</v>
+        <v>5798</v>
       </c>
       <c r="B46" s="38" t="s">
         <v>1245</v>
@@ -47771,31 +47771,31 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="38" t="s">
-        <v>5800</v>
+        <v>5799</v>
       </c>
       <c r="B47" s="38" t="s">
-        <v>5759</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="38" t="s">
-        <v>5801</v>
+        <v>5800</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>1241</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="38" t="s">
-        <v>5802</v>
+        <v>5801</v>
       </c>
       <c r="B49" s="38" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="38" t="s">
-        <v>5803</v>
+        <v>5802</v>
       </c>
       <c r="B50" s="38" t="s">
         <v>1245</v>
@@ -47803,31 +47803,31 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="38" t="s">
-        <v>5762</v>
+        <v>5803</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>5759</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="38" t="s">
-        <v>5846</v>
+        <v>5762</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>1250</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="38" t="s">
-        <v>171</v>
+        <v>5846</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="38" t="s">
-        <v>5731</v>
+        <v>171</v>
       </c>
       <c r="B54" s="38" t="s">
         <v>1248</v>
@@ -47838,7 +47838,7 @@
         <v>5731</v>
       </c>
       <c r="B55" s="38" t="s">
-        <v>5856</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -47846,15 +47846,15 @@
         <v>5731</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>1250</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="38" t="s">
-        <v>5702</v>
+        <v>5731</v>
       </c>
       <c r="B57" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -47862,7 +47862,7 @@
         <v>5702</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>5856</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -47870,15 +47870,15 @@
         <v>5702</v>
       </c>
       <c r="B59" s="38" t="s">
-        <v>1250</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="38" t="s">
-        <v>5732</v>
+        <v>5702</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -47886,7 +47886,7 @@
         <v>5732</v>
       </c>
       <c r="B61" s="38" t="s">
-        <v>5856</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -47894,15 +47894,15 @@
         <v>5732</v>
       </c>
       <c r="B62" s="38" t="s">
-        <v>1250</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="38" t="s">
-        <v>5703</v>
+        <v>5732</v>
       </c>
       <c r="B63" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -47910,7 +47910,7 @@
         <v>5703</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>5856</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -47918,44 +47918,44 @@
         <v>5703</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>1250</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="38" t="s">
-        <v>5804</v>
+        <v>5703</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>1239</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="38" t="s">
-        <v>5805</v>
+        <v>5804</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="38" t="s">
-        <v>5720</v>
+        <v>5805</v>
       </c>
       <c r="B68" s="38" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="38" t="s">
-        <v>5692</v>
+        <v>5720</v>
       </c>
       <c r="B69" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="38" t="s">
-        <v>5693</v>
+        <v>5692</v>
       </c>
       <c r="B70" s="38" t="s">
         <v>1248</v>
@@ -47963,23 +47963,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="38" t="s">
-        <v>5687</v>
+        <v>5693</v>
       </c>
       <c r="B71" s="38" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="38" t="s">
-        <v>1897</v>
+        <v>5687</v>
       </c>
       <c r="B72" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="38" t="s">
-        <v>5704</v>
+        <v>1897</v>
       </c>
       <c r="B73" s="38" t="s">
         <v>1248</v>
@@ -47987,15 +47987,15 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="38" t="s">
-        <v>5705</v>
+        <v>5704</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="38" t="s">
-        <v>5706</v>
+        <v>5705</v>
       </c>
       <c r="B75" s="38" t="s">
         <v>1250</v>
@@ -48003,23 +48003,23 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="38" t="s">
-        <v>5694</v>
+        <v>5706</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="38" t="s">
-        <v>5806</v>
+        <v>5694</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>1243</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="38" t="s">
-        <v>5721</v>
+        <v>5806</v>
       </c>
       <c r="B78" s="38" t="s">
         <v>1243</v>
@@ -48030,20 +48030,20 @@
         <v>5721</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="38" t="s">
-        <v>5807</v>
+        <v>5721</v>
       </c>
       <c r="B80" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="38" t="s">
-        <v>5722</v>
+        <v>5807</v>
       </c>
       <c r="B81" s="38" t="s">
         <v>1243</v>
@@ -48054,12 +48054,12 @@
         <v>5722</v>
       </c>
       <c r="B82" s="38" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="38" t="s">
-        <v>5723</v>
+        <v>5722</v>
       </c>
       <c r="B83" s="38" t="s">
         <v>1250</v>
@@ -48067,15 +48067,15 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="38" t="s">
-        <v>178</v>
+        <v>5723</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="38" t="s">
-        <v>5753</v>
+        <v>178</v>
       </c>
       <c r="B85" s="38" t="s">
         <v>1254</v>
@@ -48083,23 +48083,23 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="38" t="s">
-        <v>5808</v>
+        <v>5753</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>1241</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="38" t="s">
-        <v>1673</v>
+        <v>5808</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>1254</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="38" t="s">
-        <v>5754</v>
+        <v>1673</v>
       </c>
       <c r="B88" s="38" t="s">
         <v>1254</v>
@@ -48107,15 +48107,15 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="38" t="s">
-        <v>5809</v>
+        <v>5754</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>1241</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="38" t="s">
-        <v>5810</v>
+        <v>5809</v>
       </c>
       <c r="B90" s="38" t="s">
         <v>1241</v>
@@ -48126,15 +48126,15 @@
         <v>5810</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="38" t="s">
-        <v>5724</v>
+        <v>5810</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -48142,20 +48142,20 @@
         <v>5724</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="38" t="s">
-        <v>5712</v>
+        <v>5724</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="38" t="s">
-        <v>5725</v>
+        <v>5712</v>
       </c>
       <c r="B95" s="38" t="s">
         <v>1250</v>
@@ -48166,20 +48166,20 @@
         <v>5725</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="38" t="s">
-        <v>5840</v>
+        <v>5725</v>
       </c>
       <c r="B97" s="38" t="s">
-        <v>1238</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="38" t="s">
-        <v>5841</v>
+        <v>5840</v>
       </c>
       <c r="B98" s="38" t="s">
         <v>1238</v>
@@ -48187,55 +48187,55 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="38" t="s">
-        <v>5779</v>
+        <v>5841</v>
       </c>
       <c r="B99" s="38" t="s">
-        <v>1248</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="38" t="s">
-        <v>5811</v>
+        <v>5779</v>
       </c>
       <c r="B100" s="38" t="s">
-        <v>1239</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="38" t="s">
-        <v>5726</v>
+        <v>5811</v>
       </c>
       <c r="B101" s="38" t="s">
-        <v>5857</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="38" t="s">
-        <v>5763</v>
+        <v>5726</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>5759</v>
+        <v>5857</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="38" t="s">
-        <v>5812</v>
+        <v>5763</v>
       </c>
       <c r="B103" s="38" t="s">
-        <v>1239</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="38" t="s">
-        <v>5781</v>
+        <v>5812</v>
       </c>
       <c r="B104" s="38" t="s">
-        <v>1248</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="38" t="s">
-        <v>5782</v>
+        <v>5781</v>
       </c>
       <c r="B105" s="38" t="s">
         <v>1248</v>
@@ -48243,50 +48243,50 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="38" t="s">
-        <v>5737</v>
+        <v>5782</v>
       </c>
       <c r="B106" s="38" t="s">
-        <v>1236</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="38" t="s">
-        <v>5813</v>
+        <v>5737</v>
       </c>
       <c r="B107" s="38" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="38" t="s">
-        <v>5738</v>
+        <v>5813</v>
       </c>
       <c r="B108" s="38" t="s">
-        <v>1236</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="38" t="s">
-        <v>5814</v>
+        <v>5738</v>
       </c>
       <c r="B109" s="38" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="38" t="s">
-        <v>5815</v>
+        <v>5814</v>
       </c>
       <c r="B110" s="38" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="38" t="s">
-        <v>5816</v>
+        <v>5815</v>
       </c>
       <c r="B111" s="38" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -48294,23 +48294,23 @@
         <v>5816</v>
       </c>
       <c r="B112" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="38" t="s">
-        <v>5727</v>
+        <v>5816</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="38" t="s">
-        <v>5817</v>
+        <v>5727</v>
       </c>
       <c r="B114" s="38" t="s">
-        <v>1241</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -48318,15 +48318,15 @@
         <v>5817</v>
       </c>
       <c r="B115" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="38" t="s">
-        <v>5818</v>
+        <v>5817</v>
       </c>
       <c r="B116" s="38" t="s">
-        <v>1241</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -48334,23 +48334,23 @@
         <v>5818</v>
       </c>
       <c r="B117" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="38" t="s">
-        <v>5764</v>
+        <v>5818</v>
       </c>
       <c r="B118" s="38" t="s">
-        <v>5759</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="38" t="s">
-        <v>5819</v>
+        <v>5764</v>
       </c>
       <c r="B119" s="38" t="s">
-        <v>1241</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -48358,12 +48358,12 @@
         <v>5819</v>
       </c>
       <c r="B120" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="38" t="s">
-        <v>5820</v>
+        <v>5819</v>
       </c>
       <c r="B121" s="38" t="s">
         <v>5855</v>
@@ -48371,23 +48371,23 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="38" t="s">
-        <v>5745</v>
+        <v>5820</v>
       </c>
       <c r="B122" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="38" t="s">
-        <v>5695</v>
+        <v>5745</v>
       </c>
       <c r="B123" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="38" t="s">
-        <v>5696</v>
+        <v>5695</v>
       </c>
       <c r="B124" s="38" t="s">
         <v>1248</v>
@@ -48395,7 +48395,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="38" t="s">
-        <v>5697</v>
+        <v>5696</v>
       </c>
       <c r="B125" s="38" t="s">
         <v>1248</v>
@@ -48403,15 +48403,15 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="38" t="s">
-        <v>5755</v>
+        <v>5697</v>
       </c>
       <c r="B126" s="38" t="s">
-        <v>1254</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="38" t="s">
-        <v>5756</v>
+        <v>5755</v>
       </c>
       <c r="B127" s="38" t="s">
         <v>1254</v>
@@ -48419,58 +48419,58 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="38" t="s">
-        <v>5765</v>
+        <v>5756</v>
       </c>
       <c r="B128" s="38" t="s">
-        <v>5759</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="38" t="s">
-        <v>5821</v>
+        <v>5765</v>
       </c>
       <c r="B129" s="38" t="s">
-        <v>5855</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="38" t="s">
-        <v>5786</v>
+        <v>5821</v>
       </c>
       <c r="B130" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="38" t="s">
-        <v>5766</v>
+        <v>5786</v>
       </c>
       <c r="B131" s="38" t="s">
-        <v>1239</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="38" t="s">
-        <v>5767</v>
+        <v>5766</v>
       </c>
       <c r="B132" s="38" t="s">
-        <v>5759</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="38" t="s">
-        <v>5839</v>
+        <v>5767</v>
       </c>
       <c r="B133" s="38" t="s">
-        <v>1238</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="38" t="s">
-        <v>5822</v>
+        <v>5839</v>
       </c>
       <c r="B134" s="38" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -48478,39 +48478,39 @@
         <v>5822</v>
       </c>
       <c r="B135" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="38" t="s">
-        <v>5707</v>
+        <v>5822</v>
       </c>
       <c r="B136" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="38" t="s">
-        <v>5823</v>
+        <v>5707</v>
       </c>
       <c r="B137" s="38" t="s">
-        <v>5759</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="38" t="s">
-        <v>5739</v>
+        <v>5823</v>
       </c>
       <c r="B138" s="38" t="s">
-        <v>1236</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="38" t="s">
-        <v>5824</v>
+        <v>5739</v>
       </c>
       <c r="B139" s="38" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -48518,23 +48518,23 @@
         <v>5824</v>
       </c>
       <c r="B140" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="38" t="s">
-        <v>5728</v>
+        <v>5824</v>
       </c>
       <c r="B141" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="38" t="s">
-        <v>5825</v>
+        <v>5728</v>
       </c>
       <c r="B142" s="38" t="s">
-        <v>1241</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -48542,20 +48542,20 @@
         <v>5825</v>
       </c>
       <c r="B143" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="38" t="s">
-        <v>5729</v>
+        <v>5825</v>
       </c>
       <c r="B144" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="38" t="s">
-        <v>5708</v>
+        <v>5729</v>
       </c>
       <c r="B145" s="38" t="s">
         <v>1250</v>
@@ -48563,7 +48563,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="38" t="s">
-        <v>5709</v>
+        <v>5708</v>
       </c>
       <c r="B146" s="38" t="s">
         <v>1250</v>
@@ -48571,10 +48571,10 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="38" t="s">
-        <v>5826</v>
+        <v>5709</v>
       </c>
       <c r="B147" s="38" t="s">
-        <v>1241</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -48582,15 +48582,15 @@
         <v>5826</v>
       </c>
       <c r="B148" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="38" t="s">
-        <v>5768</v>
+        <v>5826</v>
       </c>
       <c r="B149" s="38" t="s">
-        <v>1250</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -48598,39 +48598,39 @@
         <v>5768</v>
       </c>
       <c r="B150" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="38" t="s">
-        <v>5827</v>
+        <v>5768</v>
       </c>
       <c r="B151" s="38" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="38" t="s">
-        <v>5828</v>
+        <v>5827</v>
       </c>
       <c r="B152" s="38" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="38" t="s">
-        <v>5769</v>
+        <v>5828</v>
       </c>
       <c r="B153" s="38" t="s">
-        <v>5759</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="38" t="s">
-        <v>5829</v>
+        <v>5769</v>
       </c>
       <c r="B154" s="38" t="s">
-        <v>1241</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -48638,36 +48638,36 @@
         <v>5829</v>
       </c>
       <c r="B155" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" s="38" t="s">
-        <v>5830</v>
+        <v>5829</v>
       </c>
       <c r="B156" s="38" t="s">
-        <v>1239</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="38" t="s">
-        <v>5831</v>
+        <v>5830</v>
       </c>
       <c r="B157" s="38" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="38" t="s">
-        <v>1677</v>
+        <v>5831</v>
       </c>
       <c r="B158" s="38" t="s">
-        <v>1254</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="38" t="s">
-        <v>5757</v>
+        <v>1677</v>
       </c>
       <c r="B159" s="38" t="s">
         <v>1254</v>
@@ -48675,23 +48675,23 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="38" t="s">
-        <v>5832</v>
+        <v>5757</v>
       </c>
       <c r="B160" s="38" t="s">
-        <v>1245</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="38" t="s">
-        <v>5770</v>
+        <v>5832</v>
       </c>
       <c r="B161" s="38" t="s">
-        <v>5759</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" s="38" t="s">
-        <v>5771</v>
+        <v>5770</v>
       </c>
       <c r="B162" s="38" t="s">
         <v>5759</v>
@@ -48699,15 +48699,15 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="38" t="s">
-        <v>5740</v>
+        <v>5771</v>
       </c>
       <c r="B163" s="38" t="s">
-        <v>1236</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="38" t="s">
-        <v>5741</v>
+        <v>5740</v>
       </c>
       <c r="B164" s="38" t="s">
         <v>1236</v>
@@ -48715,7 +48715,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="38" t="s">
-        <v>5785</v>
+        <v>5741</v>
       </c>
       <c r="B165" s="38" t="s">
         <v>1236</v>
@@ -48723,34 +48723,34 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="38" t="s">
-        <v>5833</v>
+        <v>5785</v>
       </c>
       <c r="B166" s="38" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="38" t="s">
-        <v>5834</v>
+        <v>5833</v>
       </c>
       <c r="B167" s="38" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="38" t="s">
-        <v>5742</v>
+        <v>5834</v>
       </c>
       <c r="B168" s="38" t="s">
-        <v>1236</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" s="38" t="s">
-        <v>5835</v>
+        <v>5742</v>
       </c>
       <c r="B169" s="38" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
@@ -48758,20 +48758,20 @@
         <v>5835</v>
       </c>
       <c r="B170" s="38" t="s">
-        <v>5855</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" s="38" t="s">
-        <v>5772</v>
+        <v>5835</v>
       </c>
       <c r="B171" s="38" t="s">
-        <v>5759</v>
+        <v>5855</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" s="38" t="s">
-        <v>5773</v>
+        <v>5772</v>
       </c>
       <c r="B172" s="38" t="s">
         <v>5759</v>
@@ -48779,18 +48779,18 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" s="38" t="s">
-        <v>5743</v>
+        <v>5773</v>
       </c>
       <c r="B173" s="38" t="s">
-        <v>1236</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" s="38" t="s">
-        <v>5758</v>
+        <v>5743</v>
       </c>
       <c r="B174" s="38" t="s">
-        <v>1250</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
@@ -48798,15 +48798,15 @@
         <v>5758</v>
       </c>
       <c r="B175" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" s="38" t="s">
-        <v>5711</v>
+        <v>5758</v>
       </c>
       <c r="B176" s="38" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
@@ -48814,28 +48814,28 @@
         <v>5711</v>
       </c>
       <c r="B177" s="38" t="s">
-        <v>1243</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="38" t="s">
-        <v>5713</v>
+        <v>5711</v>
       </c>
       <c r="B178" s="38" t="s">
-        <v>1250</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="38" t="s">
-        <v>5774</v>
+        <v>5713</v>
       </c>
       <c r="B179" s="38" t="s">
-        <v>5759</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="38" t="s">
-        <v>5775</v>
+        <v>5774</v>
       </c>
       <c r="B180" s="38" t="s">
         <v>5759</v>
@@ -48843,26 +48843,26 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="38" t="s">
-        <v>5730</v>
+        <v>5775</v>
       </c>
       <c r="B181" s="38" t="s">
-        <v>5857</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="38" t="s">
-        <v>5776</v>
+        <v>5730</v>
       </c>
       <c r="B182" s="38" t="s">
-        <v>5759</v>
+        <v>5857</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="38" t="s">
-        <v>5836</v>
+        <v>5776</v>
       </c>
       <c r="B183" s="38" t="s">
-        <v>1241</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
@@ -48870,7 +48870,7 @@
         <v>5836</v>
       </c>
       <c r="B184" s="38" t="s">
-        <v>1238</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
@@ -48878,20 +48878,20 @@
         <v>5836</v>
       </c>
       <c r="B185" s="38" t="s">
-        <v>5854</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="38" t="s">
-        <v>5698</v>
+        <v>5836</v>
       </c>
       <c r="B186" s="38" t="s">
-        <v>1248</v>
+        <v>5854</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="38" t="s">
-        <v>5699</v>
+        <v>5698</v>
       </c>
       <c r="B187" s="38" t="s">
         <v>1248</v>
@@ -48899,23 +48899,23 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" s="38" t="s">
-        <v>5837</v>
+        <v>5699</v>
       </c>
       <c r="B188" s="38" t="s">
-        <v>1241</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" s="38" t="s">
-        <v>5777</v>
+        <v>5837</v>
       </c>
       <c r="B189" s="38" t="s">
-        <v>5759</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" s="38" t="s">
-        <v>5778</v>
+        <v>5777</v>
       </c>
       <c r="B190" s="38" t="s">
         <v>5759</v>
@@ -48923,18 +48923,18 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" s="38" t="s">
-        <v>5744</v>
+        <v>5778</v>
       </c>
       <c r="B191" s="38" t="s">
-        <v>1236</v>
+        <v>5759</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="38" t="s">
-        <v>1832</v>
+        <v>5744</v>
       </c>
       <c r="B192" s="38" t="s">
-        <v>1248</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
@@ -48942,15 +48942,15 @@
         <v>1832</v>
       </c>
       <c r="B193" s="38" t="s">
-        <v>5856</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="38" t="s">
-        <v>5733</v>
+        <v>1832</v>
       </c>
       <c r="B194" s="38" t="s">
-        <v>1248</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
@@ -48958,44 +48958,44 @@
         <v>5733</v>
       </c>
       <c r="B195" s="38" t="s">
-        <v>5856</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="38" t="s">
-        <v>1831</v>
+        <v>5733</v>
       </c>
       <c r="B196" s="38" t="s">
-        <v>1248</v>
+        <v>5856</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="38" t="s">
-        <v>5838</v>
+        <v>1831</v>
       </c>
       <c r="B197" s="38" t="s">
-        <v>1241</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="38" t="s">
-        <v>5710</v>
+        <v>5838</v>
       </c>
       <c r="B198" s="38" t="s">
-        <v>1250</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="38" t="s">
-        <v>1827</v>
+        <v>5710</v>
       </c>
       <c r="B199" s="38" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="38" t="s">
-        <v>5700</v>
+        <v>1827</v>
       </c>
       <c r="B200" s="38" t="s">
         <v>1248</v>
@@ -49003,10 +49003,594 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" s="38" t="s">
+        <v>5700</v>
+      </c>
+      <c r="B201" s="38" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A202" s="38" t="s">
         <v>5847</v>
       </c>
-      <c r="B201" s="38" t="s">
+      <c r="B202" s="38" t="s">
         <v>1241</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A203" s="51" t="s">
+        <v>5859</v>
+      </c>
+      <c r="B203" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A204" s="51" t="s">
+        <v>5859</v>
+      </c>
+      <c r="B204" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A205" s="51" t="s">
+        <v>5860</v>
+      </c>
+      <c r="B205" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A206" s="51" t="s">
+        <v>5861</v>
+      </c>
+      <c r="B206" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A207" s="51" t="s">
+        <v>5862</v>
+      </c>
+      <c r="B207" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A208" s="51" t="s">
+        <v>5863</v>
+      </c>
+      <c r="B208" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A209" s="51" t="s">
+        <v>5864</v>
+      </c>
+      <c r="B209" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A210" s="51" t="s">
+        <v>5865</v>
+      </c>
+      <c r="B210" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A211" s="51" t="s">
+        <v>5866</v>
+      </c>
+      <c r="B211" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A212" s="51" t="s">
+        <v>5867</v>
+      </c>
+      <c r="B212" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A213" s="51" t="s">
+        <v>5867</v>
+      </c>
+      <c r="B213" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A214" s="51" t="s">
+        <v>5868</v>
+      </c>
+      <c r="B214" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A215" s="51" t="s">
+        <v>5869</v>
+      </c>
+      <c r="B215" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A216" s="51" t="s">
+        <v>5869</v>
+      </c>
+      <c r="B216" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A217" s="51" t="s">
+        <v>5870</v>
+      </c>
+      <c r="B217" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A218" s="51" t="s">
+        <v>5871</v>
+      </c>
+      <c r="B218" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A219" s="51" t="s">
+        <v>5872</v>
+      </c>
+      <c r="B219" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A220" s="51" t="s">
+        <v>5873</v>
+      </c>
+      <c r="B220" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A221" s="51" t="s">
+        <v>5874</v>
+      </c>
+      <c r="B221" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A222" s="51" t="s">
+        <v>5875</v>
+      </c>
+      <c r="B222" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A223" s="51" t="s">
+        <v>5875</v>
+      </c>
+      <c r="B223" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A224" s="51" t="s">
+        <v>5876</v>
+      </c>
+      <c r="B224" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A225" s="51" t="s">
+        <v>5876</v>
+      </c>
+      <c r="B225" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A226" s="51" t="s">
+        <v>5877</v>
+      </c>
+      <c r="B226" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A227" s="51" t="s">
+        <v>5877</v>
+      </c>
+      <c r="B227" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A228" s="51" t="s">
+        <v>5878</v>
+      </c>
+      <c r="B228" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A229" s="51" t="s">
+        <v>5878</v>
+      </c>
+      <c r="B229" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A230" s="51" t="s">
+        <v>5879</v>
+      </c>
+      <c r="B230" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A231" s="51" t="s">
+        <v>5880</v>
+      </c>
+      <c r="B231" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A232" s="51" t="s">
+        <v>5881</v>
+      </c>
+      <c r="B232" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A233" s="51" t="s">
+        <v>5882</v>
+      </c>
+      <c r="B233" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A234" s="51" t="s">
+        <v>5883</v>
+      </c>
+      <c r="B234" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A235" s="51" t="s">
+        <v>5883</v>
+      </c>
+      <c r="B235" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A236" s="51" t="s">
+        <v>5884</v>
+      </c>
+      <c r="B236" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A237" s="51" t="s">
+        <v>5885</v>
+      </c>
+      <c r="B237" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A238" s="51" t="s">
+        <v>5886</v>
+      </c>
+      <c r="B238" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A239" s="51" t="s">
+        <v>5887</v>
+      </c>
+      <c r="B239" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A240" s="51" t="s">
+        <v>5888</v>
+      </c>
+      <c r="B240" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A241" s="51" t="s">
+        <v>5888</v>
+      </c>
+      <c r="B241" s="38" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A242" s="51" t="s">
+        <v>5889</v>
+      </c>
+      <c r="B242" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A243" s="51" t="s">
+        <v>5890</v>
+      </c>
+      <c r="B243" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A244" s="51" t="s">
+        <v>5891</v>
+      </c>
+      <c r="B244" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A245" s="51" t="s">
+        <v>5892</v>
+      </c>
+      <c r="B245" s="38" t="s">
+        <v>5759</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A246" s="51" t="s">
+        <v>5893</v>
+      </c>
+      <c r="B246" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A247" s="51" t="s">
+        <v>5894</v>
+      </c>
+      <c r="B247" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A248" s="51" t="s">
+        <v>5895</v>
+      </c>
+      <c r="B248" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A249" s="51" t="s">
+        <v>5896</v>
+      </c>
+      <c r="B249" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A250" s="51" t="s">
+        <v>5897</v>
+      </c>
+      <c r="B250" s="38" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A251" s="51" t="s">
+        <v>5898</v>
+      </c>
+      <c r="B251" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A252" s="51" t="s">
+        <v>5898</v>
+      </c>
+      <c r="B252" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A253" s="51" t="s">
+        <v>5899</v>
+      </c>
+      <c r="B253" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A254" s="51" t="s">
+        <v>5900</v>
+      </c>
+      <c r="B254" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A255" s="51" t="s">
+        <v>5901</v>
+      </c>
+      <c r="B255" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A256" s="51" t="s">
+        <v>5902</v>
+      </c>
+      <c r="B256" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A257" s="51" t="s">
+        <v>5903</v>
+      </c>
+      <c r="B257" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A258" s="51" t="s">
+        <v>5904</v>
+      </c>
+      <c r="B258" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A259" s="51" t="s">
+        <v>5905</v>
+      </c>
+      <c r="B259" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A260" s="51" t="s">
+        <v>5906</v>
+      </c>
+      <c r="B260" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A261" s="51" t="s">
+        <v>5907</v>
+      </c>
+      <c r="B261" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A262" s="51" t="s">
+        <v>5908</v>
+      </c>
+      <c r="B262" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A263" s="51" t="s">
+        <v>5909</v>
+      </c>
+      <c r="B263" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A264" s="51" t="s">
+        <v>5910</v>
+      </c>
+      <c r="B264" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A265" s="51" t="s">
+        <v>5911</v>
+      </c>
+      <c r="B265" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A266" s="51" t="s">
+        <v>5912</v>
+      </c>
+      <c r="B266" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A267" s="51" t="s">
+        <v>5913</v>
+      </c>
+      <c r="B267" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A268" s="51" t="s">
+        <v>5913</v>
+      </c>
+      <c r="B268" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A269" s="51" t="s">
+        <v>5914</v>
+      </c>
+      <c r="B269" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A270" s="51" t="s">
+        <v>5915</v>
+      </c>
+      <c r="B270" s="38" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A271" s="51" t="s">
+        <v>5915</v>
+      </c>
+      <c r="B271" s="38" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A272" s="51" t="s">
+        <v>5916</v>
+      </c>
+      <c r="B272" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A273" s="51" t="s">
+        <v>5917</v>
+      </c>
+      <c r="B273" s="38" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A274" s="51" t="s">
+        <v>5918</v>
+      </c>
+      <c r="B274" s="38" t="s">
+        <v>1236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lookup table corrections in Ontario JSON Config
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/LOOKUP_TABLES/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\fgp-metadata-proxy\FME_files\LOOKUP_TABLES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PT_Harvester\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2510" yWindow="4680" windowWidth="11810" windowHeight="3020" tabRatio="883" firstSheet="47" activeTab="52"/>
+    <workbookView xWindow="2510" yWindow="4680" windowWidth="11810" windowHeight="3020" tabRatio="883" firstSheet="37" activeTab="40"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -25,34 +25,34 @@
     <sheet name="Default_NB" sheetId="44" r:id="rId11"/>
     <sheet name="Default_ON" sheetId="34" r:id="rId12"/>
     <sheet name="Default_QC" sheetId="16" r:id="rId13"/>
-    <sheet name="ON_JSON_CONFIG" sheetId="81" r:id="rId14"/>
-    <sheet name="ESRI_AB" sheetId="15" r:id="rId15"/>
-    <sheet name="Format" sheetId="7" r:id="rId16"/>
-    <sheet name="Geodata_YT" sheetId="72" r:id="rId17"/>
-    <sheet name="Format_TBS_ON" sheetId="74" r:id="rId18"/>
-    <sheet name="Format_TBS_QC" sheetId="28" r:id="rId19"/>
-    <sheet name="FrenchTranslation" sheetId="8" r:id="rId20"/>
-    <sheet name="Geohub_ON_URL" sheetId="52" r:id="rId21"/>
-    <sheet name="Geospatial_BC" sheetId="25" r:id="rId22"/>
-    <sheet name="GeoportalWeblink_BC" sheetId="67" r:id="rId23"/>
-    <sheet name="GeoportalWeblink_ON" sheetId="68" r:id="rId24"/>
-    <sheet name="GeoportalWeblink_QC" sheetId="69" r:id="rId25"/>
-    <sheet name="Geospatial_QC_to_delete" sheetId="20" r:id="rId26"/>
-    <sheet name="Geospatial_ON_to_delete" sheetId="53" r:id="rId27"/>
-    <sheet name="GeospatialValidation" sheetId="63" r:id="rId28"/>
-    <sheet name="Isotopic_ON" sheetId="75" r:id="rId29"/>
-    <sheet name="Keyword" sheetId="5" r:id="rId30"/>
-    <sheet name="License_QC" sheetId="27" r:id="rId31"/>
-    <sheet name="License_ON" sheetId="64" r:id="rId32"/>
-    <sheet name="NB_ESRISERVICES" sheetId="51" r:id="rId33"/>
-    <sheet name="NB_Keywords" sheetId="60" r:id="rId34"/>
-    <sheet name="NB_Remove" sheetId="46" r:id="rId35"/>
-    <sheet name="NB_GeoDataTypes" sheetId="55" r:id="rId36"/>
-    <sheet name="NB_SlashCountSeparator" sheetId="42" r:id="rId37"/>
-    <sheet name="NB_TOPICS_DATASET" sheetId="56" r:id="rId38"/>
-    <sheet name="NB_TOPICS_GENERIC" sheetId="57" r:id="rId39"/>
-    <sheet name="NB_LINKBUILDER_GEO" sheetId="58" r:id="rId40"/>
-    <sheet name="NB_LINKBUILDER_NONGEO" sheetId="59" r:id="rId41"/>
+    <sheet name="ESRI_AB" sheetId="15" r:id="rId14"/>
+    <sheet name="Format" sheetId="7" r:id="rId15"/>
+    <sheet name="Geodata_YT" sheetId="72" r:id="rId16"/>
+    <sheet name="Format_TBS_ON" sheetId="74" r:id="rId17"/>
+    <sheet name="Format_TBS_QC" sheetId="28" r:id="rId18"/>
+    <sheet name="FrenchTranslation" sheetId="8" r:id="rId19"/>
+    <sheet name="Geohub_ON_URL" sheetId="52" r:id="rId20"/>
+    <sheet name="Geospatial_BC" sheetId="25" r:id="rId21"/>
+    <sheet name="GeoportalWeblink_BC" sheetId="67" r:id="rId22"/>
+    <sheet name="GeoportalWeblink_ON" sheetId="68" r:id="rId23"/>
+    <sheet name="GeoportalWeblink_QC" sheetId="69" r:id="rId24"/>
+    <sheet name="Geospatial_QC_to_delete" sheetId="20" r:id="rId25"/>
+    <sheet name="Geospatial_ON_to_delete" sheetId="53" r:id="rId26"/>
+    <sheet name="GeospatialValidation" sheetId="63" r:id="rId27"/>
+    <sheet name="Isotopic_ON" sheetId="75" r:id="rId28"/>
+    <sheet name="Keyword" sheetId="5" r:id="rId29"/>
+    <sheet name="License_QC" sheetId="27" r:id="rId30"/>
+    <sheet name="License_ON" sheetId="64" r:id="rId31"/>
+    <sheet name="NB_ESRISERVICES" sheetId="51" r:id="rId32"/>
+    <sheet name="NB_Keywords" sheetId="60" r:id="rId33"/>
+    <sheet name="NB_Remove" sheetId="46" r:id="rId34"/>
+    <sheet name="NB_GeoDataTypes" sheetId="55" r:id="rId35"/>
+    <sheet name="NB_SlashCountSeparator" sheetId="42" r:id="rId36"/>
+    <sheet name="NB_TOPICS_DATASET" sheetId="56" r:id="rId37"/>
+    <sheet name="NB_TOPICS_GENERIC" sheetId="57" r:id="rId38"/>
+    <sheet name="NB_LINKBUILDER_GEO" sheetId="58" r:id="rId39"/>
+    <sheet name="NB_LINKBUILDER_NONGEO" sheetId="59" r:id="rId40"/>
+    <sheet name="ON_JSON_CONFIG" sheetId="81" r:id="rId41"/>
     <sheet name="Progress" sheetId="10" r:id="rId42"/>
     <sheet name="PyCSW_config" sheetId="40" r:id="rId43"/>
     <sheet name="QC_JSON_CONFIG" sheetId="31" r:id="rId44"/>
@@ -81,10 +81,10 @@
     <sheet name="WMS_URL_QC" sheetId="38" r:id="rId67"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="22">GeoportalWeblink_BC!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="23">GeoportalWeblink_ON!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="24">GeoportalWeblink_QC!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="29">Keyword!$2:$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="21">GeoportalWeblink_BC!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="22">GeoportalWeblink_ON!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="23">GeoportalWeblink_QC!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="28">Keyword!$2:$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19776,509 +19776,6 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1284</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>1281</v>
-      </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1280</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>1182</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>1279</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>1278</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1277</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>764</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>1275</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>1274</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1273</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>1272</v>
-      </c>
-      <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>1185</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5858</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>1192</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>1194</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>760</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1269</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>1196</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>1198</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1198</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>1199</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1199</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>1204</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1204</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>1268</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1268</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B36" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>1257</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>1266</v>
-      </c>
-      <c r="B39" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>1265</v>
-      </c>
-      <c r="B40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B41" t="s">
-        <v>826</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>1263</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -20659,7 +20156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F491"/>
   <sheetViews>
@@ -28557,7 +28054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B307"/>
   <sheetViews>
@@ -31033,7 +30530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -31158,7 +30655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B48"/>
   <sheetViews>
@@ -31557,6 +31054,50 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -32430,50 +31971,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="49.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -32531,7 +32028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -32706,7 +32203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -32790,6 +32287,110 @@
       </c>
       <c r="B9" s="18" t="s">
         <v>2698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="38" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B10" s="38"/>
+    </row>
+  </sheetData>
+  <sortState ref="A3:B10">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="58.54296875" customWidth="1"/>
+    <col min="2" max="2" width="46.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="38" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
+        <v>2691</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
+        <v>2687</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>2696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>2693</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>2531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="38" t="s">
+        <v>2694</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="38" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>2699</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -32820,8 +32421,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.54296875" customWidth="1"/>
-    <col min="2" max="2" width="46.7265625" customWidth="1"/>
+    <col min="1" max="1" width="62.26953125" customWidth="1"/>
+    <col min="2" max="2" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -32861,7 +32462,7 @@
         <v>2687</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>2696</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -32893,7 +32494,7 @@
         <v>2690</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>2699</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -32915,110 +32516,6 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="62.26953125" customWidth="1"/>
-    <col min="2" max="2" width="65.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
-        <v>2686</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
-        <v>2691</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
-        <v>2692</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
-        <v>2687</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>2697</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
-        <v>2689</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
-        <v>2693</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>2531</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>2694</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>2533</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="38" t="s">
-        <v>2690</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
-        <v>2695</v>
-      </c>
-      <c r="B10" s="38"/>
-    </row>
-  </sheetData>
-  <sortState ref="A3:B10">
-    <sortCondition ref="A1"/>
-  </sortState>
-  <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
@@ -33738,7 +33235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -33989,7 +33486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
@@ -34743,7 +34240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C263"/>
   <sheetViews>
@@ -37654,6 +37151,292 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2712</v>
+      </c>
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2713</v>
+      </c>
+      <c r="B9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>2711</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>2709</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>186</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:B33">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -38558,292 +38341,6 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="36.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2712</v>
-      </c>
-      <c r="B4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>2713</v>
-      </c>
-      <c r="B9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>2711</v>
-      </c>
-      <c r="B11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>171</v>
-      </c>
-      <c r="B13" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>170</v>
-      </c>
-      <c r="B14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>160</v>
-      </c>
-      <c r="B16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B17" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B18" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B20" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>188</v>
-      </c>
-      <c r="B21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>180</v>
-      </c>
-      <c r="B22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>183</v>
-      </c>
-      <c r="B24" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>184</v>
-      </c>
-      <c r="B25" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1707</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>2710</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>185</v>
-      </c>
-      <c r="B28" s="38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>2709</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>186</v>
-      </c>
-      <c r="B30" s="38" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>187</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>168</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="A1:B33">
-    <sortCondition ref="A1"/>
-  </sortState>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38933,7 +38430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -39032,7 +38529,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -39248,7 +38745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B185"/>
   <sheetViews>
@@ -40750,7 +40247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -40800,7 +40297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -40858,7 +40355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -40902,7 +40399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B76"/>
   <sheetViews>
@@ -41531,7 +41028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -41808,6 +41305,97 @@
       </c>
       <c r="B33" s="32" t="s">
         <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9" style="20" customWidth="1"/>
+    <col min="2" max="2" width="67.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="31.81640625" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>836</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D2" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>1815</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>1813</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -42608,97 +42196,6 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9" style="20" customWidth="1"/>
-    <col min="2" max="2" width="67.453125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="31.81640625" style="20" customWidth="1"/>
-    <col min="4" max="16384" width="10.81640625" style="20"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>836</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1266</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>1818</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>1817</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>1816</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D2" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1815</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="D3" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>1814</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="D4" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>1813</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="20">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -42823,6 +42320,509 @@
       </c>
       <c r="D8" s="20">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="26.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>764</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5858</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>760</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B39" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B41" t="s">
+        <v>826</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1258</v>
       </c>
     </row>
   </sheetData>
@@ -47390,7 +47390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B274"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>

</xml_diff>